<commit_message>
Predisposto il tutto per il cambio allo swap
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -515,41 +515,41 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251547</v>
+        <v>251651</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D2" t="n">
-        <v>184.9154929577465</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>13129</v>
+        <v>46830</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -558,75 +558,73 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M2" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N2" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>0</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>250759</v>
+        <v>251742</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>30</v>
       </c>
       <c r="D3" t="n">
-        <v>118.2816901408451</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>8398</v>
+        <v>8226</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -635,17 +633,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L3" t="n">
         <v>4</v>
       </c>
       <c r="M3" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N3" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -653,57 +651,57 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-1.406147540983796</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>250894</v>
+        <v>251840</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>623.4084507042254</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-12 07:47:36</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>44262</v>
+        <v>5714</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -712,73 +710,75 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
         <v>5</v>
       </c>
       <c r="M4" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N4" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
+        <v>39758</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>39758</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>0</v>
+        <v>-0.4885587431712963</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251416</v>
+        <v>251229</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D5" t="n">
-        <v>158.056338028169</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-12 07:47:36</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-12 08:23:36</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-12 08:23:36</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-12 11:01:39</t>
+          <t>2025-05-09 09:15:43</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>11222</v>
+        <v>18739</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -787,27 +787,31 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
       </c>
-      <c r="N5" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>39723</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
@@ -819,41 +823,41 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251742</v>
+        <v>251225</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D6" t="n">
-        <v>134.8524590163935</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>8226</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -862,17 +866,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
         <v>4</v>
       </c>
       <c r="M6" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N6" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -880,57 +884,57 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-0.5131944444444444</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-0.5131944444444444</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251840</v>
+        <v>251227</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
-        <v>93.67213114754098</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>5714</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -939,17 +943,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N7" t="n">
-        <v>39758</v>
+        <v>39746</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -957,57 +961,57 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39758</v>
+        <v>39746</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-2.523611111111111</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-2.523611111111111</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251229</v>
+        <v>251782</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>307.1967213114754</v>
+        <v>170.0422535211268</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:08:31</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:08:31</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-09 09:15:43</t>
+          <t>2025-05-09 07:41:02</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>18739</v>
+        <v>12073</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1016,19 +1020,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
-        <v>70</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N8" t="n">
+        <v>39754</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1036,53 +1038,53 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39723</v>
+        <v>39754</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>0</v>
+        <v>-0.3201682316087963</v>
       </c>
       <c r="S8" s="1" t="n">
-        <v>0</v>
+        <v>-0.3201682316087963</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251225</v>
+        <v>251050</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>19</v>
+        <v>217</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1095,14 +1097,14 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="M9" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N9" t="n">
         <v>39747</v>
@@ -1117,49 +1119,49 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-0.5131944444444444</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S9" s="1" t="n">
-        <v>-0.5131944444444444</v>
+        <v>-1.442361111111111</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251227</v>
+        <v>251054</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1172,17 +1174,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="M10" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N10" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1190,57 +1192,57 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-2.523611111111111</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>-2.523611111111111</v>
+        <v>-1.466666666666667</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251782</v>
+        <v>251081</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="D11" t="n">
-        <v>170.0422535211268</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-09 07:41:02</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>12073</v>
+        <v>3012</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1249,17 +1251,19 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="M11" t="n">
-        <v>76</v>
-      </c>
-      <c r="N11" t="n">
-        <v>39754</v>
+        <v>70</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1267,57 +1271,57 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39754</v>
+        <v>39750</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-0.3201682316087963</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>-0.3201682316087963</v>
+        <v>-16.58293231612268</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251164</v>
+        <v>251284</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>55</v>
+        <v>40.5</v>
       </c>
       <c r="D12" t="n">
-        <v>204.0816326530612</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:55:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 07:55:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-08 11:19:04</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>10000</v>
+        <v>16340</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1326,17 +1330,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M12" t="n">
         <v>70</v>
       </c>
       <c r="N12" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1344,57 +1348,57 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-1.471584467118056</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>-1.471584467118056</v>
+        <v>-1.526104797974537</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251456</v>
+        <v>251547</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D13" t="n">
-        <v>183.6530612244898</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 11:19:04</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:09:04</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:09:04</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-09 07:12:44</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>8999</v>
+        <v>13129</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1407,13 +1411,13 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
       <c r="N13" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1421,57 +1425,57 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-3.300510204085648</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>-3.300510204085648</v>
+        <v>-1.443691314548611</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251651</v>
+        <v>250759</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" t="n">
-        <v>767.7049180327868</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>46830</v>
+        <v>8398</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1480,73 +1484,75 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M14" t="n">
         <v>76</v>
       </c>
       <c r="N14" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>0</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0</v>
+        <v>-0.5466647104861111</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251455</v>
+        <v>250894</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>82.765625</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 13:24:11</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 13:24:11</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-12 07:47:36</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>5297</v>
+        <v>44262</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1555,75 +1561,73 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M15" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N15" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>0</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251391</v>
+        <v>251416</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D16" t="n">
-        <v>91.640625</v>
+        <v>158.056338028169</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-12 07:47:36</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-12 08:23:36</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-12 08:23:36</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-12 11:01:39</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>5865</v>
+        <v>11222</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1636,21 +1640,19 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
       <c r="N16" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
@@ -1658,15 +1660,15 @@
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>0</v>
       </c>
       <c r="S16" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251395</v>
+        <v>251455</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1674,33 +1676,33 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D17" t="n">
-        <v>35.34375</v>
+        <v>82.765625</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>2262</v>
+        <v>5297</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1713,7 +1715,7 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M17" t="n">
         <v>70</v>
@@ -1731,19 +1733,19 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>-0.3623372395833334</v>
       </c>
       <c r="S17" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>-0.3623372395833334</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251371</v>
+        <v>251391</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1751,33 +1753,33 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>91.640625</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>5865</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1790,15 +1792,13 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
+      <c r="N18" t="n">
+        <v>39749</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1806,23 +1806,23 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-0.4377821180555556</v>
       </c>
       <c r="S18" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-0.4377821180555556</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251396</v>
+        <v>251395</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1830,29 +1830,29 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" t="n">
         <v>35.34375</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-07 12:00:45</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-07 12:00:45</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-07 12:36:05</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1887,19 +1887,19 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-0.5250651041666666</v>
+        <v>-0.4741319444444445</v>
       </c>
       <c r="S19" s="1" t="n">
-        <v>-0.5250651041666666</v>
+        <v>-0.4741319444444445</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251548</v>
+        <v>251371</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1910,30 +1910,30 @@
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>206.90625</v>
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-07 12:36:05</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-07 12:55:05</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-07 12:55:05</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-08 08:22:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>13242</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1951,8 +1951,10 @@
       <c r="M20" t="n">
         <v>70</v>
       </c>
-      <c r="N20" t="n">
-        <v>39749</v>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1960,23 +1962,23 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>39749</v>
+        <v>39666</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-1.348611111111111</v>
+        <v>-13.48732638888889</v>
       </c>
       <c r="S20" s="1" t="n">
-        <v>-1.348611111111111</v>
+        <v>-13.48732638888889</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>250923</v>
+        <v>251396</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1984,33 +1986,33 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D21" t="n">
-        <v>109.46875</v>
+        <v>35.34375</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-08 08:22:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-08 08:54:00</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-08 08:54:00</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:28</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>7006</v>
+        <v>2262</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2019,14 +2021,14 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M21" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N21" t="n">
         <v>39749</v>
@@ -2041,19 +2043,19 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-1.446853298611111</v>
+        <v>-0.5250651041666666</v>
       </c>
       <c r="S21" s="1" t="n">
-        <v>-1.446853298611111</v>
+        <v>-0.5250651041666666</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251477</v>
+        <v>251548</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2064,30 +2066,30 @@
         <v>19</v>
       </c>
       <c r="D22" t="n">
-        <v>468.734375</v>
+        <v>206.90625</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:28</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:28</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:28</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-09 10:51:12</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>29999</v>
+        <v>13242</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2096,17 +2098,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M22" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N22" t="n">
-        <v>39760</v>
+        <v>39749</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2114,78 +2116,76 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39760</v>
+        <v>39749</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-2.452224392361111</v>
+        <v>-1.348611111111111</v>
       </c>
       <c r="S22" s="1" t="n">
-        <v>-2.452224392361111</v>
+        <v>-1.348611111111111</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251706</v>
+        <v>250923</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D23" t="n">
-        <v>50.79365079365079</v>
+        <v>109.46875</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 08:54:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 08:54:00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-08 10:43:28</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>3200</v>
+        <v>7006</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N23" t="n">
+        <v>39749</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2193,57 +2193,57 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>39764</v>
+        <v>39749</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>0</v>
+        <v>-1.446853298611111</v>
       </c>
       <c r="S23" s="1" t="n">
-        <v>0</v>
+        <v>-1.446853298611111</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251050</v>
+        <v>251477</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>217</v>
+        <v>19</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>468.734375</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 10:43:28</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 11:02:28</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 11:02:28</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 10:51:12</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>29999</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2252,17 +2252,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="M24" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N24" t="n">
-        <v>39747</v>
+        <v>39760</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2270,76 +2270,78 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>39747</v>
+        <v>39760</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-2.452224392361111</v>
       </c>
       <c r="S24" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-2.452224392361111</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251054</v>
+        <v>251706</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>70</v>
-      </c>
-      <c r="N25" t="n">
-        <v>39747</v>
+        <v>0</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2347,57 +2349,57 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>39747</v>
+        <v>39764</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
       <c r="S25" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251081</v>
+        <v>251164</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>125</v>
+        <v>55</v>
       </c>
       <c r="D26" t="n">
-        <v>42.42253521126761</v>
+        <v>204.0816326530612</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>3012</v>
+        <v>10000</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2406,19 +2408,17 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="M26" t="n">
         <v>70</v>
       </c>
-      <c r="N26" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
+      <c r="N26" t="n">
+        <v>39749</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2426,57 +2426,57 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>39750</v>
+        <v>39749</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-1.471584467118056</v>
       </c>
       <c r="S26" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-1.471584467118056</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251284</v>
+        <v>251456</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>40.5</v>
+        <v>50</v>
       </c>
       <c r="D27" t="n">
-        <v>297.0909090909091</v>
+        <v>183.6530612244898</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-09 07:12:44</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>16340</v>
+        <v>8999</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2485,17 +2485,17 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M27" t="n">
         <v>70</v>
       </c>
       <c r="N27" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2503,18 +2503,18 @@
         </is>
       </c>
       <c r="P27" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-3.300510204085648</v>
       </c>
       <c r="S27" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-3.300510204085648</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
Prima ricerca locale con f.o. introdotta; al momento il trade-off con il parametro alfa sembra funzionare; cambiato il funzionamento della priorità (+1 per poterla utilizzare come divisore); cambiata l'assegnazione del ritardo alle commesse del terzo ciclo / euristico post-prime-ricerche-locali - posto pari a due_date - fine_lavorazione anziché zero
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -515,7 +515,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251840</v>
+        <v>251742</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>93.67213114754098</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -535,21 +535,21 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:35:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-08 09:08:40</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>5714</v>
+        <v>8226</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M2" t="n">
         <v>70</v>
       </c>
       <c r="N2" t="n">
-        <v>39758</v>
+        <v>39749</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -576,26 +576,26 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>39758</v>
+        <v>39749</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>-0.3810223132986111</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251229</v>
+        <v>251840</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -606,30 +606,30 @@
         <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>307.1967213114754</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-08 09:08:40</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-08 09:33:40</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-08 09:33:40</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-08 14:40:52</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>18739</v>
+        <v>5714</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -638,19 +638,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M3" t="n">
         <v>70</v>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+      <c r="N3" t="n">
+        <v>39758</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -658,18 +656,18 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39723</v>
+        <v>39758</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>0</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>0</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="T3" t="n">
         <v>1</v>
@@ -677,7 +675,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251742</v>
+        <v>251229</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -685,33 +683,33 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>134.8524590163935</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-08 14:40:52</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-09 07:10:52</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-09 07:10:52</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-09 09:25:43</t>
+          <t>2025-05-09 09:15:43</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>8226</v>
+        <v>18739</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -720,17 +718,19 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M4" t="n">
         <v>70</v>
       </c>
-      <c r="N4" t="n">
-        <v>39749</v>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39749</v>
+        <v>39723</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -746,52 +746,52 @@
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>-2.392862021863426</v>
+        <v>0</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>-2.392862021863426</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251455</v>
+        <v>251164</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D5" t="n">
-        <v>82.765625</v>
+        <v>204.0816326530612</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>5297</v>
+        <v>10000</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
@@ -822,56 +822,56 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>-1.471584467118056</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>-1.471584467118056</v>
       </c>
       <c r="T5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251391</v>
+        <v>251456</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="D6" t="n">
-        <v>91.640625</v>
+        <v>183.6530612244898</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-09 07:12:44</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>5865</v>
+        <v>8999</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -884,13 +884,13 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M6" t="n">
         <v>70</v>
       </c>
       <c r="N6" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -898,60 +898,60 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-3.300510204085648</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-3.300510204085648</v>
       </c>
       <c r="T6" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251395</v>
+        <v>251050</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>217</v>
       </c>
       <c r="D7" t="n">
-        <v>35.34375</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>2262</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -960,17 +960,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
       </c>
       <c r="N7" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -978,56 +978,56 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="T7" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251371</v>
+        <v>251054</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1040,19 +1040,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
+      <c r="N8" t="n">
+        <v>39747</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1060,60 +1058,60 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39666</v>
+        <v>39747</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S8" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="T8" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251396</v>
+        <v>251081</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="D9" t="n">
-        <v>35.34375</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-07 12:00:45</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-07 12:00:45</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-07 12:36:05</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>2262</v>
+        <v>3012</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1122,17 +1120,19 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
-      <c r="N9" t="n">
-        <v>39749</v>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1140,60 +1140,60 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39749</v>
+        <v>39750</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-0.5250651041666666</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S9" s="1" t="n">
-        <v>-0.5250651041666666</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="T9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251548</v>
+        <v>251225</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>19</v>
       </c>
       <c r="D10" t="n">
-        <v>206.90625</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-07 12:36:05</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-07 12:55:05</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-07 12:55:05</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 08:22:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>13242</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1202,17 +1202,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
         <v>4</v>
       </c>
       <c r="M10" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N10" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1220,60 +1220,60 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-1.348611111111111</v>
+        <v>-0.5131944444444444</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>-1.348611111111111</v>
+        <v>-0.5131944444444444</v>
       </c>
       <c r="T10" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>250923</v>
+        <v>251227</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>109.46875</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 08:22:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 08:54:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 08:54:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:28</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>7006</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1286,13 +1286,13 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M11" t="n">
         <v>76</v>
       </c>
       <c r="N11" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1300,60 +1300,60 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-1.446853298611111</v>
+        <v>-2.523611111111111</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>-1.446853298611111</v>
+        <v>-2.523611111111111</v>
       </c>
       <c r="T11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251477</v>
+        <v>251782</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" t="n">
-        <v>468.734375</v>
+        <v>170.0422535211268</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:28</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:28</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:28</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-09 10:51:12</t>
+          <t>2025-05-09 07:41:02</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>29999</v>
+        <v>12073</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         <v>76</v>
       </c>
       <c r="N12" t="n">
-        <v>39760</v>
+        <v>39754</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1380,18 +1380,18 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39760</v>
+        <v>39754</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-2.452224392361111</v>
+        <v>-0.3201682316087963</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>-2.452224392361111</v>
+        <v>-0.3201682316087963</v>
       </c>
       <c r="T12" t="n">
         <v>1</v>
@@ -1399,41 +1399,41 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251416</v>
+        <v>251284</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>32</v>
+        <v>40.5</v>
       </c>
       <c r="D13" t="n">
-        <v>175.34375</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-09 10:51:12</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-09 11:23:12</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-09 11:23:12</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-09 14:18:32</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>11222</v>
+        <v>16340</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1442,53 +1442,55 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
       <c r="N13" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>0</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>0</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="T13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251081</v>
+        <v>251651</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="D14" t="n">
-        <v>42.42253521126761</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1497,21 +1499,21 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-09 09:07:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-09 09:07:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-09 09:49:25</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>3012</v>
+        <v>46830</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1520,80 +1522,76 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="M14" t="n">
-        <v>70</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N14" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>39750</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>0</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>-16.40932120501157</v>
+        <v>0</v>
       </c>
       <c r="T14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251050</v>
+        <v>251547</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>125</v>
+        <v>34</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-09 09:49:25</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-09 11:54:25</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-09 11:54:25</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-09 11:54:25</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>13129</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1602,17 +1600,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
       </c>
       <c r="N15" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1620,60 +1618,60 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-1.49612676056713</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>-1.49612676056713</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="T15" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251054</v>
+        <v>250759</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-09 11:54:25</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-09 12:29:25</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-09 12:29:25</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-09 12:29:25</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>8398</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1682,14 +1680,14 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="M16" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N16" t="n">
         <v>39747</v>
@@ -1704,56 +1702,56 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-1.520432316122685</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="S16" s="1" t="n">
-        <v>-1.520432316122685</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="T16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251651</v>
+        <v>250894</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D17" t="n">
-        <v>767.7049180327868</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 13:24:11</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 13:24:11</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-12 07:47:36</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>46830</v>
+        <v>44262</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1782,7 +1780,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
@@ -1797,142 +1795,142 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251284</v>
+        <v>251706</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>40.5</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>297.0909090909091</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>16340</v>
+        <v>3200</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>39764</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>2025-05-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="R18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
         <v>7</v>
-      </c>
-      <c r="M18" t="n">
-        <v>70</v>
-      </c>
-      <c r="N18" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P18" t="n">
-        <v>39747</v>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>2025-05-12 00:00:00</t>
-        </is>
-      </c>
-      <c r="R18" s="1" t="n">
-        <v>-1.526104797974537</v>
-      </c>
-      <c r="S18" s="1" t="n">
-        <v>-1.526104797974537</v>
-      </c>
-      <c r="T18" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251706</v>
+        <v>251455</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D19" t="n">
-        <v>50.79365079365079</v>
+        <v>82.765625</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>3200</v>
+        <v>5297</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N19" t="n">
+        <v>39749</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1940,18 +1938,18 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>39764</v>
+        <v>39749</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>0</v>
+        <v>-0.3623372395833334</v>
       </c>
       <c r="S19" s="1" t="n">
-        <v>0</v>
+        <v>-0.3623372395833334</v>
       </c>
       <c r="T19" t="n">
         <v>7</v>
@@ -1959,41 +1957,41 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251547</v>
+        <v>251391</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D20" t="n">
-        <v>184.9154929577465</v>
+        <v>91.640625</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>13129</v>
+        <v>5865</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2006,7 +2004,7 @@
         </is>
       </c>
       <c r="L20" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M20" t="n">
         <v>70</v>
@@ -2024,14 +2022,14 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-0.4377821180555556</v>
       </c>
       <c r="S20" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-0.4377821180555556</v>
       </c>
       <c r="T20" t="n">
         <v>7</v>
@@ -2039,41 +2037,41 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>250759</v>
+        <v>251395</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D21" t="n">
-        <v>118.2816901408451</v>
+        <v>35.34375</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>8398</v>
+        <v>2262</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2082,17 +2080,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L21" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M21" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N21" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2100,60 +2098,60 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.4741319444444445</v>
       </c>
       <c r="S21" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.4741319444444445</v>
       </c>
       <c r="T21" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>250894</v>
+        <v>251371</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D22" t="n">
-        <v>623.4084507042254</v>
+        <v>0</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-12 07:47:36</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>44262</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2162,76 +2160,80 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M22" t="n">
-        <v>76</v>
-      </c>
-      <c r="N22" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P22" t="n">
-        <v>0</v>
+        <v>39666</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>0</v>
+        <v>-13.48732638888889</v>
       </c>
       <c r="S22" s="1" t="n">
-        <v>0</v>
+        <v>-13.48732638888889</v>
       </c>
       <c r="T22" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251456</v>
+        <v>251396</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D23" t="n">
-        <v>183.6530612244898</v>
+        <v>35.34375</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-08 07:40:00</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:39</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>8999</v>
+        <v>2262</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2244,13 +2246,13 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M23" t="n">
         <v>70</v>
       </c>
       <c r="N23" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2258,60 +2260,60 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-3.300510204085648</v>
+        <v>-0.5250651041666666</v>
       </c>
       <c r="S23" s="1" t="n">
-        <v>-2.446981292511574</v>
+        <v>-0.5250651041666666</v>
       </c>
       <c r="T23" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251164</v>
+        <v>251548</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D24" t="n">
-        <v>204.0816326530612</v>
+        <v>206.90625</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:39</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-08 11:33:39</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-08 11:33:39</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-08 14:57:44</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>10000</v>
+        <v>13242</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2324,7 +2326,7 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M24" t="n">
         <v>70</v>
@@ -2342,56 +2344,56 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-1.623426870752315</v>
+        <v>-1.348611111111111</v>
       </c>
       <c r="S24" s="1" t="n">
-        <v>-1.623426870752315</v>
+        <v>-1.348611111111111</v>
       </c>
       <c r="T24" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251227</v>
+        <v>250923</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>109.46875</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 08:54:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 08:54:00</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 10:43:28</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>7006</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2404,13 +2406,13 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M25" t="n">
         <v>76</v>
       </c>
       <c r="N25" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2418,60 +2420,60 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-2.523611111111111</v>
+        <v>-1.446853298611111</v>
       </c>
       <c r="S25" s="1" t="n">
-        <v>-2.513194444444444</v>
+        <v>-1.446853298611111</v>
       </c>
       <c r="T25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251782</v>
+        <v>251477</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D26" t="n">
-        <v>170.0422535211268</v>
+        <v>468.734375</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 10:43:28</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-08 12:36:00</t>
+          <t>2025-05-08 11:02:28</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-08 12:36:00</t>
+          <t>2025-05-08 11:02:28</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-09 07:26:02</t>
+          <t>2025-05-09 10:51:12</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>12073</v>
+        <v>29999</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2490,7 +2492,7 @@
         <v>76</v>
       </c>
       <c r="N26" t="n">
-        <v>39754</v>
+        <v>39760</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2498,18 +2500,18 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>39754</v>
+        <v>39760</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-0.3097515649421296</v>
+        <v>-2.452224392361111</v>
       </c>
       <c r="S26" s="1" t="n">
-        <v>-0.3097515649421296</v>
+        <v>-2.452224392361111</v>
       </c>
       <c r="T26" t="n">
         <v>1</v>
@@ -2517,41 +2519,41 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251225</v>
+        <v>251416</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>175.34375</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:26:02</t>
+          <t>2025-05-09 10:51:12</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:43:02</t>
+          <t>2025-05-09 11:23:12</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:43:02</t>
+          <t>2025-05-09 11:23:12</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:43:02</t>
+          <t>2025-05-09 14:18:32</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>11222</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2560,39 +2562,37 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M27" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N27" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>39747</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>-1.321557120497685</v>
+        <v>0</v>
       </c>
       <c r="S27" s="1" t="n">
-        <v>-1.321557120497685</v>
+        <v>0</v>
       </c>
       <c r="T27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -2661,7 +2661,7 @@
         </is>
       </c>
       <c r="R28" s="1" t="n">
-        <v>0</v>
+        <v>-14.31945422534722</v>
       </c>
       <c r="S28" t="n">
         <v>4</v>
@@ -2733,7 +2733,7 @@
         </is>
       </c>
       <c r="R29" s="1" t="n">
-        <v>0</v>
+        <v>-2.465152550092593</v>
       </c>
       <c r="S29" t="n">
         <v>8</v>
@@ -2805,7 +2805,7 @@
         </is>
       </c>
       <c r="R30" s="1" t="n">
-        <v>0</v>
+        <v>-2.5025390625</v>
       </c>
       <c r="S30" t="n">
         <v>8</v>
@@ -2877,7 +2877,7 @@
         </is>
       </c>
       <c r="R31" s="1" t="n">
-        <v>0</v>
+        <v>-2.560940346087963</v>
       </c>
       <c r="S31" t="n">
         <v>8</v>
@@ -2949,7 +2949,7 @@
         </is>
       </c>
       <c r="R32" s="1" t="n">
-        <v>0</v>
+        <v>-12.35892857142361</v>
       </c>
       <c r="S32" t="n">
         <v>7</v>
@@ -3021,7 +3021,7 @@
         </is>
       </c>
       <c r="R33" s="1" t="n">
-        <v>0</v>
+        <v>-9.585894097222223</v>
       </c>
       <c r="S33" t="n">
         <v>7</v>
@@ -3093,7 +3093,7 @@
         </is>
       </c>
       <c r="R34" s="1" t="n">
-        <v>0</v>
+        <v>-7.396717171712963</v>
       </c>
       <c r="S34" t="n">
         <v>7</v>
@@ -3453,7 +3453,7 @@
         </is>
       </c>
       <c r="R39" s="1" t="n">
-        <v>0</v>
+        <v>-238.3566999217477</v>
       </c>
       <c r="S39" t="n">
         <v>2</v>
@@ -3525,7 +3525,7 @@
         </is>
       </c>
       <c r="R40" s="1" t="n">
-        <v>0</v>
+        <v>-553.4429577464815</v>
       </c>
       <c r="S40" t="n">
         <v>4</v>
@@ -3597,7 +3597,7 @@
         </is>
       </c>
       <c r="R41" s="1" t="n">
-        <v>0</v>
+        <v>-108.3039906103241</v>
       </c>
       <c r="S41" t="n">
         <v>2</v>
@@ -3669,7 +3669,7 @@
         </is>
       </c>
       <c r="R42" s="1" t="n">
-        <v>0</v>
+        <v>-15.2991071428588</v>
       </c>
       <c r="S42" t="n">
         <v>4</v>
@@ -3741,7 +3741,7 @@
         </is>
       </c>
       <c r="R43" s="1" t="n">
-        <v>0</v>
+        <v>-14.50895947177083</v>
       </c>
       <c r="S43" t="n">
         <v>4</v>
@@ -3813,7 +3813,7 @@
         </is>
       </c>
       <c r="R44" s="1" t="n">
-        <v>0</v>
+        <v>-14.48929924241898</v>
       </c>
       <c r="S44" t="n">
         <v>4</v>
@@ -3885,7 +3885,7 @@
         </is>
       </c>
       <c r="R45" s="1" t="n">
-        <v>0</v>
+        <v>-12.53967136150463</v>
       </c>
       <c r="S45" t="n">
         <v>4</v>
@@ -3957,7 +3957,7 @@
         </is>
       </c>
       <c r="R46" s="1" t="n">
-        <v>0</v>
+        <v>-5.559761345856481</v>
       </c>
       <c r="S46" t="n">
         <v>4</v>
@@ -4029,7 +4029,7 @@
         </is>
       </c>
       <c r="R47" s="1" t="n">
-        <v>0</v>
+        <v>-4.566287878784722</v>
       </c>
       <c r="S47" t="n">
         <v>4</v>
@@ -4101,7 +4101,7 @@
         </is>
       </c>
       <c r="R48" s="1" t="n">
-        <v>0</v>
+        <v>-4.571914845173612</v>
       </c>
       <c r="S48" t="n">
         <v>4</v>
@@ -4173,7 +4173,7 @@
         </is>
       </c>
       <c r="R49" s="1" t="n">
-        <v>0</v>
+        <v>-4.580293715844907</v>
       </c>
       <c r="S49" t="n">
         <v>4</v>
@@ -4389,7 +4389,7 @@
         </is>
       </c>
       <c r="R52" s="1" t="n">
-        <v>0</v>
+        <v>-25.47753325508102</v>
       </c>
       <c r="S52" t="n">
         <v>2</v>
@@ -4461,7 +4461,7 @@
         </is>
       </c>
       <c r="R53" s="1" t="n">
-        <v>0</v>
+        <v>-25.36457702019676</v>
       </c>
       <c r="S53" t="n">
         <v>2</v>
@@ -4533,7 +4533,7 @@
         </is>
       </c>
       <c r="R54" s="1" t="n">
-        <v>0</v>
+        <v>-20.31067850637731</v>
       </c>
       <c r="S54" t="n">
         <v>2</v>
@@ -4605,7 +4605,7 @@
         </is>
       </c>
       <c r="R55" s="1" t="n">
-        <v>0</v>
+        <v>-15.31380919854167</v>
       </c>
       <c r="S55" t="n">
         <v>2</v>
@@ -4677,7 +4677,7 @@
         </is>
       </c>
       <c r="R56" s="1" t="n">
-        <v>0</v>
+        <v>-15.36771336554398</v>
       </c>
       <c r="S56" t="n">
         <v>2</v>
@@ -4749,7 +4749,7 @@
         </is>
       </c>
       <c r="R57" s="1" t="n">
-        <v>0</v>
+        <v>-8.350425170069444</v>
       </c>
       <c r="S57" t="n">
         <v>2</v>
@@ -4821,7 +4821,7 @@
         </is>
       </c>
       <c r="R58" s="1" t="n">
-        <v>0</v>
+        <v>-7.367928403761574</v>
       </c>
       <c r="S58" t="n">
         <v>2</v>
@@ -4893,7 +4893,7 @@
         </is>
       </c>
       <c r="R59" s="1" t="n">
-        <v>0</v>
+        <v>-285.306660798125</v>
       </c>
       <c r="S59" t="n">
         <v>1</v>
@@ -5037,7 +5037,7 @@
         </is>
       </c>
       <c r="R61" s="1" t="n">
-        <v>0</v>
+        <v>-225.3452982695833</v>
       </c>
       <c r="S61" t="n">
         <v>1</v>
@@ -5109,7 +5109,7 @@
         </is>
       </c>
       <c r="R62" s="1" t="n">
-        <v>0</v>
+        <v>-56.37124316939815</v>
       </c>
       <c r="S62" t="n">
         <v>1</v>
@@ -5181,7 +5181,7 @@
         </is>
       </c>
       <c r="R63" s="1" t="n">
-        <v>0</v>
+        <v>-46.368359375</v>
       </c>
       <c r="S63" t="n">
         <v>1</v>
@@ -5253,7 +5253,7 @@
         </is>
       </c>
       <c r="R64" s="1" t="n">
-        <v>0</v>
+        <v>-9.389824263043982</v>
       </c>
       <c r="S64" t="n">
         <v>1</v>
@@ -5325,7 +5325,7 @@
         </is>
       </c>
       <c r="R65" s="1" t="n">
-        <v>0</v>
+        <v>-5.3925</v>
       </c>
       <c r="S65" t="n">
         <v>1</v>
@@ -5397,7 +5397,7 @@
         </is>
       </c>
       <c r="R66" s="1" t="n">
-        <v>0</v>
+        <v>-4.505867552337963</v>
       </c>
       <c r="S66" t="n">
         <v>1</v>
@@ -5469,7 +5469,7 @@
         </is>
       </c>
       <c r="R67" s="1" t="n">
-        <v>0</v>
+        <v>-4.441128716747685</v>
       </c>
       <c r="S67" t="n">
         <v>1</v>
@@ -5541,7 +5541,7 @@
         </is>
       </c>
       <c r="R68" s="1" t="n">
-        <v>0</v>
+        <v>-4.457150607638889</v>
       </c>
       <c r="S68" t="n">
         <v>1</v>
@@ -5613,7 +5613,7 @@
         </is>
       </c>
       <c r="R69" s="1" t="n">
-        <v>0</v>
+        <v>-4.472814207650463</v>
       </c>
       <c r="S69" t="n">
         <v>1</v>
@@ -5685,7 +5685,7 @@
         </is>
       </c>
       <c r="R70" s="1" t="n">
-        <v>0</v>
+        <v>-4.513830203437499</v>
       </c>
       <c r="S70" t="n">
         <v>1</v>
@@ -5757,7 +5757,7 @@
         </is>
       </c>
       <c r="R71" s="1" t="n">
-        <v>0</v>
+        <v>-4.537901475694444</v>
       </c>
       <c r="S71" t="n">
         <v>1</v>
@@ -5829,7 +5829,7 @@
         </is>
       </c>
       <c r="R72" s="1" t="n">
-        <v>0</v>
+        <v>-4.563831967210648</v>
       </c>
       <c r="S72" t="n">
         <v>1</v>
@@ -5901,7 +5901,7 @@
         </is>
       </c>
       <c r="R73" s="1" t="n">
-        <v>0</v>
+        <v>-2.359575508611111</v>
       </c>
       <c r="S73" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Cambiata nomenclatura delle funzioni di ricerca locale (move -> insert)
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -515,18 +515,18 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251742</v>
+        <v>251547</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D2" t="n">
-        <v>134.8524590163935</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -535,21 +535,21 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>8226</v>
+        <v>13129</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -580,14 +580,14 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="T2" t="n">
         <v>7</v>
@@ -595,41 +595,41 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251840</v>
+        <v>250759</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D3" t="n">
-        <v>93.67213114754098</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>5714</v>
+        <v>8398</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -638,17 +638,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M3" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N3" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -656,18 +656,18 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39758</v>
+        <v>39747</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="T3" t="n">
         <v>1</v>
@@ -675,41 +675,41 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251229</v>
+        <v>250894</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>307.1967213114754</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-08 12:08:31</t>
+          <t>2025-05-08 13:24:11</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-08 12:08:31</t>
+          <t>2025-05-08 13:24:11</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-09 09:15:43</t>
+          <t>2025-05-12 07:47:36</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>18739</v>
+        <v>44262</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,31 +718,27 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M4" t="n">
-        <v>70</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N4" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>39723</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
@@ -752,46 +748,46 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251164</v>
+        <v>251416</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D5" t="n">
-        <v>204.0816326530612</v>
+        <v>158.056338028169</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-12 07:47:36</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-08 07:55:00</t>
+          <t>2025-05-12 08:23:36</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-08 07:55:00</t>
+          <t>2025-05-12 08:23:36</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-08 11:19:04</t>
+          <t>2025-05-12 11:01:39</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>10000</v>
+        <v>11222</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -804,74 +800,72 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
       </c>
       <c r="N5" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-1.471584467118056</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>-1.471584467118056</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251456</v>
+        <v>251742</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D6" t="n">
-        <v>183.6530612244898</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-08 11:19:04</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-08 12:09:04</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-08 12:09:04</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-09 07:12:44</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>8999</v>
+        <v>8226</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -884,13 +878,13 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M6" t="n">
         <v>70</v>
       </c>
       <c r="N6" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -898,60 +892,60 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-3.300510204085648</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>-3.300510204085648</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="T6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251050</v>
+        <v>251840</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>217</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>5714</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -960,17 +954,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
       </c>
       <c r="N7" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -978,60 +972,60 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="T7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251054</v>
+        <v>251229</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 09:15:43</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>18739</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1040,17 +1034,19 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
-      <c r="N8" t="n">
-        <v>39747</v>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1058,60 +1054,60 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39747</v>
+        <v>39723</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
       <c r="S8" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251081</v>
+        <v>251164</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>125</v>
+        <v>55</v>
       </c>
       <c r="D9" t="n">
-        <v>42.42253521126761</v>
+        <v>204.0816326530612</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>3012</v>
+        <v>10000</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1120,19 +1116,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
+      <c r="N9" t="n">
+        <v>39749</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1140,60 +1134,60 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39750</v>
+        <v>39749</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-1.471584467118056</v>
       </c>
       <c r="S9" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-1.471584467118056</v>
       </c>
       <c r="T9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251225</v>
+        <v>251456</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>183.6530612244898</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 07:12:44</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>8999</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1202,17 +1196,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M10" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N10" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1220,18 +1214,18 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-0.5131944444444444</v>
+        <v>-3.300510204085648</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>-0.5131944444444444</v>
+        <v>-3.300510204085648</v>
       </c>
       <c r="T10" t="n">
         <v>1</v>
@@ -1239,37 +1233,37 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251227</v>
+        <v>251050</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>15</v>
+        <v>217</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1282,17 +1276,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="M11" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N11" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1300,60 +1294,60 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-2.523611111111111</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>-2.523611111111111</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="T11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251782</v>
+        <v>251054</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D12" t="n">
-        <v>170.0422535211268</v>
+        <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-09 07:41:02</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>12073</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1362,17 +1356,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="M12" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N12" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1380,60 +1374,60 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-0.3201682316087963</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>-0.3201682316087963</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="T12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251284</v>
+        <v>251081</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>40.5</v>
+        <v>125</v>
       </c>
       <c r="D13" t="n">
-        <v>297.0909090909091</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>16340</v>
+        <v>3012</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1442,17 +1436,19 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
-      <c r="N13" t="n">
-        <v>39747</v>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1460,21 +1456,21 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39747</v>
+        <v>39750</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="T13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -1557,41 +1553,41 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251547</v>
+        <v>251225</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D15" t="n">
-        <v>184.9154929577465</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>13129</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1600,17 +1596,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
         <v>4</v>
       </c>
       <c r="M15" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N15" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1618,60 +1614,60 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-0.5131944444444444</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-0.5131944444444444</v>
       </c>
       <c r="T15" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>250759</v>
+        <v>251227</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>118.2816901408451</v>
+        <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>8398</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1680,7 +1676,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
@@ -1690,7 +1686,7 @@
         <v>76</v>
       </c>
       <c r="N16" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1698,18 +1694,18 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39747</v>
+        <v>39746</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-2.523611111111111</v>
       </c>
       <c r="S16" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-2.523611111111111</v>
       </c>
       <c r="T16" t="n">
         <v>1</v>
@@ -1717,41 +1713,41 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>250894</v>
+        <v>251782</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>17</v>
       </c>
       <c r="D17" t="n">
-        <v>623.4084507042254</v>
+        <v>170.0422535211268</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-12 07:47:36</t>
+          <t>2025-05-09 07:41:02</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>44262</v>
+        <v>12073</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1760,37 +1756,39 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M17" t="n">
         <v>76</v>
       </c>
       <c r="N17" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0</v>
+        <v>39754</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>39754</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>0</v>
+        <v>-0.3201682316087963</v>
       </c>
       <c r="S17" s="1" t="n">
-        <v>0</v>
+        <v>-0.3201682316087963</v>
       </c>
       <c r="T17" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -2519,41 +2517,41 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251416</v>
+        <v>251284</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>32</v>
+        <v>40.5</v>
       </c>
       <c r="D27" t="n">
-        <v>175.34375</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-09 10:51:12</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-09 11:23:12</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-09 11:23:12</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 14:18:32</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>11222</v>
+        <v>16340</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2562,37 +2560,39 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M27" t="n">
         <v>70</v>
       </c>
       <c r="N27" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>0</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S27" s="1" t="n">
-        <v>0</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="T27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
Implementata anche la terza ricerca locale (LS3)
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -515,18 +515,18 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251547</v>
+        <v>251742</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>184.9154929577465</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -535,21 +535,21 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>13129</v>
+        <v>8226</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -580,14 +580,14 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="T2" t="n">
         <v>7</v>
@@ -595,41 +595,41 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>250759</v>
+        <v>251840</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>118.2816901408451</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>8398</v>
+        <v>5714</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -638,17 +638,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M3" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N3" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -656,18 +656,18 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="T3" t="n">
         <v>1</v>
@@ -675,41 +675,41 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>250894</v>
+        <v>251229</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>623.4084507042254</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-08 12:08:31</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-12 07:47:36</t>
+          <t>2025-05-09 09:15:43</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>44262</v>
+        <v>18739</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,27 +718,31 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M4" t="n">
-        <v>76</v>
-      </c>
-      <c r="N4" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>39723</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
@@ -748,12 +752,12 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251416</v>
+        <v>251547</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -761,33 +765,33 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" t="n">
-        <v>158.056338028169</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-12 07:47:36</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-12 08:23:36</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-12 08:23:36</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-12 11:01:39</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>11222</v>
+        <v>13129</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -800,72 +804,74 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M5" t="n">
         <v>70</v>
       </c>
       <c r="N5" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
+        <v>39749</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>0</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>0</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="T5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251742</v>
+        <v>250759</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C6" t="n">
         <v>30</v>
       </c>
       <c r="D6" t="n">
-        <v>134.8524590163935</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>8226</v>
+        <v>8398</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -874,17 +880,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L6" t="n">
         <v>4</v>
       </c>
       <c r="M6" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N6" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -892,60 +898,60 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="T6" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251840</v>
+        <v>250894</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D7" t="n">
-        <v>93.67213114754098</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 13:24:11</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 13:24:11</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-12 07:47:36</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>5714</v>
+        <v>44262</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -954,78 +960,76 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
         <v>5</v>
       </c>
       <c r="M7" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N7" t="n">
-        <v>39758</v>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>39758</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>0</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251229</v>
+        <v>251416</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D8" t="n">
-        <v>307.1967213114754</v>
+        <v>158.056338028169</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-12 07:47:36</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:08:31</t>
+          <t>2025-05-12 08:23:36</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-08 12:08:31</t>
+          <t>2025-05-12 08:23:36</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-09 09:15:43</t>
+          <t>2025-05-12 11:01:39</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>18739</v>
+        <v>11222</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1034,31 +1038,27 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="N8" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>39723</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
@@ -1068,46 +1068,46 @@
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251164</v>
+        <v>251050</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="D9" t="n">
-        <v>204.0816326530612</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:55:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:55:00</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 11:19:04</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1116,17 +1116,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
       <c r="N9" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1134,60 +1134,60 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-1.471584467118056</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S9" s="1" t="n">
-        <v>-1.471584467118056</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="T9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251456</v>
+        <v>251054</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D10" t="n">
-        <v>183.6530612244898</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-08 11:19:04</t>
+          <t>2025-05-09 10:37:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:09:04</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 12:09:04</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-09 07:12:44</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>8999</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1196,17 +1196,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
       </c>
       <c r="N10" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1214,26 +1214,26 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39746</v>
+        <v>39747</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-3.300510204085648</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>-3.300510204085648</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="T10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251050</v>
+        <v>251081</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1241,33 +1241,33 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>217</v>
+        <v>125</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 13:17:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>3012</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1280,13 +1280,15 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M11" t="n">
         <v>70</v>
       </c>
-      <c r="N11" t="n">
-        <v>39747</v>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1294,18 +1296,18 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39747</v>
+        <v>39750</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="T11" t="n">
         <v>2</v>
@@ -1313,41 +1315,41 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251054</v>
+        <v>251651</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>767.7049180327868</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 07:29:00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>46830</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1356,78 +1358,76 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="M12" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N12" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>39747</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
       <c r="S12" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251081</v>
+        <v>251227</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="D13" t="n">
-        <v>42.42253521126761</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>3012</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1436,19 +1436,17 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
-        <v>70</v>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N13" t="n">
+        <v>39746</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1456,60 +1454,60 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39750</v>
+        <v>39746</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-2.523611111111111</v>
       </c>
       <c r="S13" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-2.513194444444444</v>
       </c>
       <c r="T13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251651</v>
+        <v>251225</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D14" t="n">
-        <v>767.7049180327868</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-08 12:19:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-09 07:29:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>46830</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1518,42 +1516,44 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M14" t="n">
         <v>76</v>
       </c>
       <c r="N14" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>0</v>
+        <v>-0.5236111111111111</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0</v>
+        <v>-0.5236111111111111</v>
       </c>
       <c r="T14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251225</v>
+        <v>251782</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1561,33 +1561,33 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>170.0422535211268</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 12:34:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 12:51:00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-09 07:41:02</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>12073</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1596,17 +1596,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M15" t="n">
         <v>76</v>
       </c>
       <c r="N15" t="n">
-        <v>39747</v>
+        <v>39754</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1614,18 +1614,18 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39747</v>
+        <v>39754</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.5131944444444444</v>
+        <v>-0.3201682316087963</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>-0.5131944444444444</v>
+        <v>-0.3201682316087963</v>
       </c>
       <c r="T15" t="n">
         <v>1</v>
@@ -1633,60 +1633,62 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251227</v>
+        <v>251706</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>76</v>
-      </c>
-      <c r="N16" t="n">
-        <v>39746</v>
+        <v>0</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1694,60 +1696,60 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39746</v>
+        <v>39764</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-2.523611111111111</v>
+        <v>0</v>
       </c>
       <c r="S16" s="1" t="n">
-        <v>-2.523611111111111</v>
+        <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251782</v>
+        <v>251164</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="D17" t="n">
-        <v>170.0422535211268</v>
+        <v>204.0816326530612</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-08 07:55:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-09 07:41:02</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>12073</v>
+        <v>10000</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1756,17 +1758,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M17" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N17" t="n">
-        <v>39754</v>
+        <v>39749</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1774,81 +1776,79 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39754</v>
+        <v>39749</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-04-22 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-0.3201682316087963</v>
+        <v>-1.471584467118056</v>
       </c>
       <c r="S17" s="1" t="n">
-        <v>-0.3201682316087963</v>
+        <v>-1.471584467118056</v>
       </c>
       <c r="T17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251706</v>
+        <v>251456</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D18" t="n">
-        <v>50.79365079365079</v>
+        <v>183.6530612244898</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 11:19:04</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:09:04</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-09 07:12:44</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>3200</v>
+        <v>8999</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="N18" t="n">
+        <v>39746</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1856,21 +1856,21 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39764</v>
+        <v>39746</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>0</v>
+        <v>-3.300510204085648</v>
       </c>
       <c r="S18" s="1" t="n">
-        <v>0</v>
+        <v>-3.300510204085648</v>
       </c>
       <c r="T18" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">

</xml_diff>

<commit_message>
Tentativo di cambiamento di LS1
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -515,7 +515,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>251742</v>
+        <v>251229</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D2" t="n">
-        <v>134.8524590163935</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -535,21 +535,21 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 07:40:00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-08 07:40:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 12:47:11</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>8226</v>
+        <v>18739</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -558,17 +558,19 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M2" t="n">
         <v>70</v>
       </c>
-      <c r="N2" t="n">
-        <v>39749</v>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -576,7 +578,7 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>39749</v>
+        <v>39723</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -584,13 +586,13 @@
         </is>
       </c>
       <c r="R2" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>0</v>
       </c>
       <c r="S2" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -610,22 +612,22 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-08 12:47:11</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 13:12:11</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-08 13:12:11</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 14:45:52</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -664,10 +666,10 @@
         </is>
       </c>
       <c r="R3" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-0.6151867031018519</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>-0.6151867031018519</v>
       </c>
       <c r="T3" t="n">
         <v>1</v>
@@ -675,7 +677,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251229</v>
+        <v>251455</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -686,30 +688,30 @@
         <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>307.1967213114754</v>
+        <v>86.8360655737705</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-08 14:45:52</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-08 12:08:31</t>
+          <t>2025-05-09 07:10:52</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-08 12:08:31</t>
+          <t>2025-05-09 07:10:52</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-05-09 09:15:43</t>
+          <t>2025-05-09 08:37:42</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>18739</v>
+        <v>5297</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -718,19 +720,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M4" t="n">
         <v>70</v>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
+      <c r="N4" t="n">
+        <v>39749</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -738,21 +738,21 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39723</v>
+        <v>39749</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0</v>
+        <v>-2.359517304189815</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>0</v>
+        <v>-2.359517304189815</v>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -761,33 +761,33 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>184.9154929577465</v>
+        <v>215.2295081967213</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 08:37:42</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-09 08:57:42</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-09 08:57:42</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-09 12:32:56</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -826,10 +826,10 @@
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-2.522871129328704</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-2.522871129328704</v>
       </c>
       <c r="T5" t="n">
         <v>7</v>
@@ -837,41 +837,41 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>250759</v>
+        <v>251371</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D6" t="n">
-        <v>118.2816901408451</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-09 07:47:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-09 07:47:00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-09 07:47:00</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>8398</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -880,17 +880,19 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
         <v>4</v>
       </c>
       <c r="M6" t="n">
-        <v>76</v>
-      </c>
-      <c r="N6" t="n">
-        <v>39747</v>
+        <v>70</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -898,60 +900,60 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39747</v>
+        <v>39666</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-13.48732638888889</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-15.32430555555556</v>
       </c>
       <c r="T6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>250894</v>
+        <v>251050</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>205</v>
       </c>
       <c r="D7" t="n">
-        <v>623.4084507042254</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-09 07:47:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-05-08 13:24:11</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-05-12 07:47:36</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>44262</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -960,76 +962,78 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="M7" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N7" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>0</v>
+        <v>-1.442361111111111</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>0</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="T7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251416</v>
+        <v>251054</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" t="n">
-        <v>158.056338028169</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-05-12 07:47:36</t>
+          <t>2025-05-09 11:12:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-12 08:23:36</t>
+          <t>2025-05-09 11:47:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-05-12 08:23:36</t>
+          <t>2025-05-09 11:47:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-05-12 11:01:39</t>
+          <t>2025-05-09 11:47:00</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>11222</v>
+        <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1038,34 +1042,36 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
       <c r="N8" t="n">
-        <v>39755</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0</v>
+        <v>39747</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-16 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>0</v>
+        <v>-1.466666666666667</v>
       </c>
       <c r="S8" s="1" t="n">
-        <v>0</v>
+        <v>-1.490972222222222</v>
       </c>
       <c r="T8" t="n">
         <v>2</v>
@@ -1073,7 +1079,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251050</v>
+        <v>251081</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1081,33 +1087,33 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>217</v>
+        <v>125</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>42.42253521126761</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-09 11:47:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 13:52:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 13:52:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-09 14:34:25</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>3012</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1120,13 +1126,15 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
-      <c r="N9" t="n">
-        <v>39747</v>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>39750 (esterno)</t>
+        </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1134,18 +1142,18 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39747</v>
+        <v>39750</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-16.58293231612268</v>
       </c>
       <c r="S9" s="1" t="n">
-        <v>-1.442361111111111</v>
+        <v>-16.60723787167824</v>
       </c>
       <c r="T9" t="n">
         <v>2</v>
@@ -1153,41 +1161,41 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251054</v>
+        <v>251782</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>170.0422535211268</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-09 10:37:00</t>
+          <t>2025-05-08 12:00:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-08 12:17:00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 07:07:02</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>12073</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1196,17 +1204,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="M10" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N10" t="n">
-        <v>39747</v>
+        <v>39754</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1214,60 +1222,60 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39747</v>
+        <v>39754</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-04-16 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>-0.3201682316087963</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>-1.466666666666667</v>
+        <v>-0.2965571204976852</v>
       </c>
       <c r="T10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251081</v>
+        <v>251284</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>125</v>
+        <v>40.5</v>
       </c>
       <c r="D11" t="n">
-        <v>42.42253521126761</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-09 11:12:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-09 13:17:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>3012</v>
+        <v>16340</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1276,19 +1284,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="M11" t="n">
         <v>70</v>
       </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>39750 (esterno)</t>
-        </is>
+      <c r="N11" t="n">
+        <v>39747</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1296,21 +1302,21 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39750</v>
+        <v>39747</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>-16.58293231612268</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="T11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -1393,41 +1399,41 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251227</v>
+        <v>251164</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>140.8450704225352</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:00:00</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 07:38:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 07:38:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 09:58:50</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1436,78 +1442,78 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L13" t="n">
+        <v>6</v>
+      </c>
+      <c r="M13" t="n">
+        <v>70</v>
+      </c>
+      <c r="N13" t="n">
+        <v>39749</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>39749</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2025-04-22 00:00:00</t>
+        </is>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>-1.471584467118056</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <v>-1.415864632233796</v>
+      </c>
+      <c r="T13" t="n">
         <v>4</v>
-      </c>
-      <c r="M13" t="n">
-        <v>76</v>
-      </c>
-      <c r="N13" t="n">
-        <v>39746</v>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P13" t="n">
-        <v>39746</v>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>2025-05-05 00:00:00</t>
-        </is>
-      </c>
-      <c r="R13" s="1" t="n">
-        <v>-2.523611111111111</v>
-      </c>
-      <c r="S13" s="1" t="n">
-        <v>-2.513194444444444</v>
-      </c>
-      <c r="T13" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251225</v>
+        <v>250759</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:19:00</t>
+          <t>2025-05-08 09:58:50</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-08 10:32:50</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-08 10:32:50</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-08 12:31:07</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>8398</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1516,7 +1522,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L14" t="n">
@@ -1538,14 +1544,14 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-0.5236111111111111</v>
+        <v>-0.5216158059490741</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>-0.5236111111111111</v>
+        <v>-0.5216158059490741</v>
       </c>
       <c r="T14" t="n">
         <v>1</v>
@@ -1553,41 +1559,41 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251782</v>
+        <v>251225</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" t="n">
-        <v>170.0422535211268</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:34:00</t>
+          <t>2025-05-08 12:31:07</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-08 12:46:07</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-08 12:51:00</t>
+          <t>2025-05-08 12:46:07</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-09 07:41:02</t>
+          <t>2025-05-08 12:46:07</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>12073</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1596,17 +1602,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M15" t="n">
         <v>76</v>
       </c>
       <c r="N15" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1614,18 +1620,18 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39754</v>
+        <v>39747</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.3201682316087963</v>
+        <v>-0.5320324726157407</v>
       </c>
       <c r="S15" s="1" t="n">
-        <v>-0.3201682316087963</v>
+        <v>-0.5320324726157407</v>
       </c>
       <c r="T15" t="n">
         <v>1</v>
@@ -1633,74 +1639,70 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251706</v>
+        <v>250894</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D16" t="n">
-        <v>50.79365079365079</v>
+        <v>623.4084507042254</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 12:46:07</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 13:03:07</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-08 13:03:07</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-12 07:26:32</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>3200</v>
+        <v>44262</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N16" t="n">
+        <v>39755</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>39764</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
@@ -1710,12 +1712,12 @@
         <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>251164</v>
+        <v>251456</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1723,10 +1725,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D17" t="n">
-        <v>204.0816326530612</v>
+        <v>183.6530612244898</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1735,21 +1737,21 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-08 07:55:00</t>
+          <t>2025-05-08 07:40:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-08 07:55:00</t>
+          <t>2025-05-08 07:40:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-08 11:19:04</t>
+          <t>2025-05-08 10:43:39</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>10000</v>
+        <v>8999</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1762,13 +1764,13 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M17" t="n">
         <v>70</v>
       </c>
       <c r="N17" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1776,60 +1778,60 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2025-04-22 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-1.471584467118056</v>
+        <v>-3.300510204085648</v>
       </c>
       <c r="S17" s="1" t="n">
-        <v>-1.471584467118056</v>
+        <v>-2.446981292511574</v>
       </c>
       <c r="T17" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251456</v>
+        <v>251742</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D18" t="n">
-        <v>183.6530612244898</v>
+        <v>128.53125</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-08 11:19:04</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:09:04</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-08 12:09:04</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-09 07:12:44</t>
+          <t>2025-05-07 09:27:31</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>8999</v>
+        <v>8226</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1842,13 +1844,13 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
       </c>
       <c r="N18" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1856,26 +1858,26 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-3.300510204085648</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S18" s="1" t="n">
-        <v>-3.300510204085648</v>
+        <v>-0.3941189236111111</v>
       </c>
       <c r="T18" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251455</v>
+        <v>251391</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1883,33 +1885,33 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" t="n">
-        <v>82.765625</v>
+        <v>91.640625</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-07 09:27:31</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-07 09:44:31</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-07 09:44:31</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-07 11:16:10</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>5297</v>
+        <v>5865</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1922,7 +1924,7 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M19" t="n">
         <v>70</v>
@@ -1940,14 +1942,14 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>-0.4695638020833333</v>
       </c>
       <c r="S19" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>-0.4695638020833333</v>
       </c>
       <c r="T19" t="n">
         <v>7</v>
@@ -1955,7 +1957,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251391</v>
+        <v>251227</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1963,33 +1965,33 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D20" t="n">
-        <v>91.640625</v>
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-07 11:16:10</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-07 11:48:10</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-07 11:48:10</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-07 11:48:10</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>5865</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1998,17 +2000,17 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N20" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -2016,21 +2018,21 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>39749</v>
+        <v>39746</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-1.491786024305556</v>
       </c>
       <c r="S20" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>-1.491786024305556</v>
       </c>
       <c r="T20" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -2043,29 +2045,29 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D21" t="n">
         <v>35.34375</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-07 11:48:10</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-07 12:22:10</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-07 12:22:10</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-07 12:57:30</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2104,10 +2106,10 @@
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>-0.53994140625</v>
       </c>
       <c r="S21" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>-0.53994140625</v>
       </c>
       <c r="T21" t="n">
         <v>7</v>
@@ -2115,7 +2117,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251371</v>
+        <v>251396</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2123,33 +2125,33 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>35.34375</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-07 12:57:30</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-07 13:12:30</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-07 13:12:30</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-07 13:47:51</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>2262</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2162,15 +2164,13 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M22" t="n">
         <v>70</v>
       </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
+      <c r="N22" t="n">
+        <v>39749</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2178,18 +2178,18 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39666</v>
+        <v>39749</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-0.57490234375</v>
       </c>
       <c r="S22" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>-0.57490234375</v>
       </c>
       <c r="T22" t="n">
         <v>7</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251396</v>
+        <v>251548</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2208,30 +2208,30 @@
         <v>19</v>
       </c>
       <c r="D23" t="n">
-        <v>35.34375</v>
+        <v>206.90625</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-07 13:47:51</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-07 12:00:45</t>
+          <t>2025-05-07 14:06:51</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-07 12:00:45</t>
+          <t>2025-05-07 14:06:51</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-07 12:36:05</t>
+          <t>2025-05-08 09:33:45</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>2262</v>
+        <v>13242</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M23" t="n">
         <v>70</v>
@@ -2262,14 +2262,14 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>-0.5250651041666666</v>
+        <v>-1.398448350694445</v>
       </c>
       <c r="S23" s="1" t="n">
-        <v>-0.5250651041666666</v>
+        <v>-1.398448350694445</v>
       </c>
       <c r="T23" t="n">
         <v>7</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251548</v>
+        <v>250923</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2285,33 +2285,33 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D24" t="n">
-        <v>206.90625</v>
+        <v>109.46875</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-07 12:36:05</t>
+          <t>2025-05-08 09:33:45</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-07 12:55:05</t>
+          <t>2025-05-08 10:05:45</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-07 12:55:05</t>
+          <t>2025-05-08 10:05:45</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-08 08:22:00</t>
+          <t>2025-05-08 11:55:14</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>13242</v>
+        <v>7006</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2320,14 +2320,14 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M24" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N24" t="n">
         <v>39749</v>
@@ -2342,22 +2342,22 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-1.348611111111111</v>
+        <v>-1.496690538194444</v>
       </c>
       <c r="S24" s="1" t="n">
-        <v>-1.348611111111111</v>
+        <v>-1.496690538194444</v>
       </c>
       <c r="T24" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>250923</v>
+        <v>251477</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2365,33 +2365,33 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D25" t="n">
-        <v>109.46875</v>
+        <v>468.734375</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-08 08:22:00</t>
+          <t>2025-05-08 11:55:14</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-08 08:54:00</t>
+          <t>2025-05-08 12:14:14</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-08 08:54:00</t>
+          <t>2025-05-08 12:14:14</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:28</t>
+          <t>2025-05-09 12:02:58</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>7006</v>
+        <v>29999</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2400,17 +2400,17 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M25" t="n">
         <v>76</v>
       </c>
       <c r="N25" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2418,26 +2418,26 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>39749</v>
+        <v>39760</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-1.446853298611111</v>
+        <v>-2.502061631944445</v>
       </c>
       <c r="S25" s="1" t="n">
-        <v>-1.446853298611111</v>
+        <v>-2.502061631944445</v>
       </c>
       <c r="T25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251477</v>
+        <v>251416</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2445,33 +2445,33 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D26" t="n">
-        <v>468.734375</v>
+        <v>175.34375</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:28</t>
+          <t>2025-05-09 12:02:58</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:28</t>
+          <t>2025-05-09 12:34:58</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-08 11:02:28</t>
+          <t>2025-05-09 12:34:58</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-09 10:51:12</t>
+          <t>2025-05-12 07:30:18</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>29999</v>
+        <v>11222</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2480,119 +2480,119 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M26" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N26" t="n">
-        <v>39760</v>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>39755</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>39760</v>
+        <v>0</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-2.452224392361111</v>
+        <v>0</v>
       </c>
       <c r="S26" s="1" t="n">
-        <v>-2.452224392361111</v>
+        <v>0</v>
       </c>
       <c r="T26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251284</v>
+        <v>251706</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>40.5</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>297.0909090909091</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>16340</v>
+        <v>3200</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P27" t="n">
+        <v>39764</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>2025-05-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="R27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
         <v>7</v>
-      </c>
-      <c r="M27" t="n">
-        <v>70</v>
-      </c>
-      <c r="N27" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="P27" t="n">
-        <v>39747</v>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>2025-05-12 00:00:00</t>
-        </is>
-      </c>
-      <c r="R27" s="1" t="n">
-        <v>-1.526104797974537</v>
-      </c>
-      <c r="S27" s="1" t="n">
-        <v>-1.526104797974537</v>
-      </c>
-      <c r="T27" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -2661,7 +2661,7 @@
         </is>
       </c>
       <c r="R28" s="1" t="n">
-        <v>-14.31945422534722</v>
+        <v>0</v>
       </c>
       <c r="S28" t="n">
         <v>4</v>
@@ -2733,7 +2733,7 @@
         </is>
       </c>
       <c r="R29" s="1" t="n">
-        <v>-2.465152550092593</v>
+        <v>0</v>
       </c>
       <c r="S29" t="n">
         <v>8</v>
@@ -2749,7 +2749,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D30" t="n">
         <v>42.453125</v>
@@ -2761,17 +2761,17 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-09 11:21:12</t>
+          <t>2025-05-09 11:10:12</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-09 11:21:12</t>
+          <t>2025-05-09 11:10:12</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-09 12:03:39</t>
+          <t>2025-05-09 11:52:39</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2805,7 +2805,7 @@
         </is>
       </c>
       <c r="R30" s="1" t="n">
-        <v>-2.5025390625</v>
+        <v>0</v>
       </c>
       <c r="S30" t="n">
         <v>8</v>
@@ -2877,7 +2877,7 @@
         </is>
       </c>
       <c r="R31" s="1" t="n">
-        <v>-2.560940346087963</v>
+        <v>0</v>
       </c>
       <c r="S31" t="n">
         <v>8</v>
@@ -2893,7 +2893,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D32" t="n">
         <v>255.1020408163265</v>
@@ -2905,17 +2905,17 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-05-09 12:21:45</t>
+          <t>2025-05-09 12:16:45</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-05-09 12:21:45</t>
+          <t>2025-05-09 12:16:45</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-05-12 08:36:51</t>
+          <t>2025-05-12 08:31:51</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2949,7 +2949,7 @@
         </is>
       </c>
       <c r="R32" s="1" t="n">
-        <v>-12.35892857142361</v>
+        <v>0</v>
       </c>
       <c r="S32" t="n">
         <v>7</v>
@@ -2972,22 +2972,22 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-05-09 12:03:39</t>
+          <t>2025-05-09 11:52:39</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-09 12:22:39</t>
+          <t>2025-05-09 12:11:39</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-05-09 12:22:39</t>
+          <t>2025-05-09 12:11:39</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-09 14:03:41</t>
+          <t>2025-05-09 13:52:41</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3021,7 +3021,7 @@
         </is>
       </c>
       <c r="R33" s="1" t="n">
-        <v>-9.585894097222223</v>
+        <v>0</v>
       </c>
       <c r="S33" t="n">
         <v>7</v>
@@ -3093,7 +3093,7 @@
         </is>
       </c>
       <c r="R34" s="1" t="n">
-        <v>-7.396717171712963</v>
+        <v>0</v>
       </c>
       <c r="S34" t="n">
         <v>7</v>
@@ -3177,33 +3177,33 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="D36" t="n">
-        <v>185.5633802816901</v>
+        <v>205.859375</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-09 13:52:41</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-12 08:04:25</t>
+          <t>2025-05-09 14:13:41</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-05-12 08:04:25</t>
+          <t>2025-05-09 14:13:41</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-12 11:09:59</t>
+          <t>2025-05-12 09:39:32</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3249,33 +3249,33 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D37" t="n">
-        <v>379.59375</v>
+        <v>342.1690140845071</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-05-09 14:03:41</t>
+          <t>2025-05-09 13:59:25</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-09 14:36:41</t>
+          <t>2025-05-12 07:04:25</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-05-09 14:36:41</t>
+          <t>2025-05-12 07:04:25</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-05-12 12:56:16</t>
+          <t>2025-05-12 12:46:35</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3453,7 +3453,7 @@
         </is>
       </c>
       <c r="R39" s="1" t="n">
-        <v>-238.3566999217477</v>
+        <v>0</v>
       </c>
       <c r="S39" t="n">
         <v>2</v>
@@ -3469,7 +3469,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D40" t="n">
         <v>140.2535211267606</v>
@@ -3481,17 +3481,17 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-05-12 08:17:36</t>
+          <t>2025-05-12 08:19:36</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-05-12 08:17:36</t>
+          <t>2025-05-12 08:19:36</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-05-12 10:37:51</t>
+          <t>2025-05-12 10:39:51</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3525,7 +3525,7 @@
         </is>
       </c>
       <c r="R40" s="1" t="n">
-        <v>-553.4429577464815</v>
+        <v>0</v>
       </c>
       <c r="S40" t="n">
         <v>4</v>
@@ -3533,41 +3533,41 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>245623</v>
+        <v>251373</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D41" t="n">
-        <v>372.0985915492957</v>
+        <v>348.8571428571428</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-05-12 08:33:38</t>
+          <t>2025-05-12 08:31:51</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-05-12 09:05:38</t>
+          <t>2025-05-12 09:16:51</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-05-12 09:05:38</t>
+          <t>2025-05-12 09:16:51</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-05-13 07:17:44</t>
+          <t>2025-05-13 07:05:42</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>26419</v>
+        <v>17094</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3576,14 +3576,14 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M41" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="O41" t="n">
         <v>0</v>
@@ -3593,53 +3593,53 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>2025-01-25 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R41" s="1" t="n">
-        <v>-108.3039906103241</v>
+        <v>0</v>
       </c>
       <c r="S41" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>251373</v>
+        <v>245623</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D42" t="n">
-        <v>348.8571428571428</v>
+        <v>372.0985915492957</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-05-12 08:36:51</t>
+          <t>2025-05-12 08:33:38</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-05-12 09:21:51</t>
+          <t>2025-05-12 09:05:38</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-05-12 09:21:51</t>
+          <t>2025-05-12 09:05:38</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-05-13 07:10:42</t>
+          <t>2025-05-13 07:17:44</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>17094</v>
+        <v>26419</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3648,14 +3648,14 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M42" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="O42" t="n">
         <v>0</v>
@@ -3665,14 +3665,14 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-01-25 00:00:00</t>
         </is>
       </c>
       <c r="R42" s="1" t="n">
-        <v>-15.2991071428588</v>
+        <v>0</v>
       </c>
       <c r="S42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -3741,7 +3741,7 @@
         </is>
       </c>
       <c r="R43" s="1" t="n">
-        <v>-14.50895947177083</v>
+        <v>0</v>
       </c>
       <c r="S43" t="n">
         <v>4</v>
@@ -3813,7 +3813,7 @@
         </is>
       </c>
       <c r="R44" s="1" t="n">
-        <v>-14.48929924241898</v>
+        <v>0</v>
       </c>
       <c r="S44" t="n">
         <v>4</v>
@@ -3825,33 +3825,33 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D45" t="n">
-        <v>122.2676056338028</v>
+        <v>135.640625</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-05-12 10:37:51</t>
+          <t>2025-05-12 09:39:32</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-05-12 10:54:51</t>
+          <t>2025-05-12 09:58:32</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-05-12 10:54:51</t>
+          <t>2025-05-12 09:58:32</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-05-12 12:57:07</t>
+          <t>2025-05-12 12:14:11</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3885,7 +3885,7 @@
         </is>
       </c>
       <c r="R45" s="1" t="n">
-        <v>-12.53967136150463</v>
+        <v>0</v>
       </c>
       <c r="S45" t="n">
         <v>4</v>
@@ -3897,33 +3897,33 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D46" t="n">
         <v>91.07042253521126</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-05-12 11:09:59</t>
+          <t>2025-05-12 10:39:51</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-05-12 11:54:59</t>
+          <t>2025-05-12 10:56:51</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-05-12 11:54:59</t>
+          <t>2025-05-12 10:56:51</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-05-12 13:26:03</t>
+          <t>2025-05-12 12:27:55</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3957,7 +3957,7 @@
         </is>
       </c>
       <c r="R46" s="1" t="n">
-        <v>-5.559761345856481</v>
+        <v>0</v>
       </c>
       <c r="S46" t="n">
         <v>4</v>
@@ -4029,7 +4029,7 @@
         </is>
       </c>
       <c r="R47" s="1" t="n">
-        <v>-4.566287878784722</v>
+        <v>0</v>
       </c>
       <c r="S47" t="n">
         <v>4</v>
@@ -4101,7 +4101,7 @@
         </is>
       </c>
       <c r="R48" s="1" t="n">
-        <v>-4.571914845173612</v>
+        <v>0</v>
       </c>
       <c r="S48" t="n">
         <v>4</v>
@@ -4113,33 +4113,33 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D49" t="n">
-        <v>56.91803278688525</v>
+        <v>54.25</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-05-12 12:16:42</t>
+          <t>2025-05-12 12:14:11</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-05-12 12:58:42</t>
+          <t>2025-05-12 12:29:11</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-05-12 12:58:42</t>
+          <t>2025-05-12 12:29:11</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-05-12 13:55:37</t>
+          <t>2025-05-12 13:23:26</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4173,7 +4173,7 @@
         </is>
       </c>
       <c r="R49" s="1" t="n">
-        <v>-4.580293715844907</v>
+        <v>0</v>
       </c>
       <c r="S49" t="n">
         <v>4</v>
@@ -4185,33 +4185,33 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D50" t="n">
-        <v>168.375</v>
+        <v>176.655737704918</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-05-12 12:56:16</t>
+          <t>2025-05-12 12:16:42</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-05-12 13:31:16</t>
+          <t>2025-05-12 12:58:42</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-05-12 13:31:16</t>
+          <t>2025-05-12 12:58:42</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-05-13 08:19:39</t>
+          <t>2025-05-13 07:55:21</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4268,22 +4268,22 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-05-12 12:57:07</t>
+          <t>2025-05-12 12:27:55</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-05-12 13:12:07</t>
+          <t>2025-05-12 12:42:55</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-05-12 13:12:07</t>
+          <t>2025-05-12 12:42:55</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-05-13 07:14:23</t>
+          <t>2025-05-12 14:45:11</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4333,29 +4333,29 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="D52" t="n">
         <v>266.5915492957747</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-05-12 13:26:03</t>
+          <t>2025-05-12 12:46:35</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-05-13 07:01:03</t>
+          <t>2025-05-12 13:31:35</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-05-13 07:01:03</t>
+          <t>2025-05-12 13:31:35</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:38</t>
+          <t>2025-05-13 09:58:10</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4389,7 +4389,7 @@
         </is>
       </c>
       <c r="R52" s="1" t="n">
-        <v>-25.47753325508102</v>
+        <v>0</v>
       </c>
       <c r="S52" t="n">
         <v>2</v>
@@ -4401,33 +4401,33 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>34.5</v>
+        <v>19</v>
       </c>
       <c r="D53" t="n">
-        <v>155.0363636363636</v>
+        <v>133.234375</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-05-12 13:35:27</t>
+          <t>2025-05-12 13:23:26</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-12 14:09:57</t>
+          <t>2025-05-12 13:42:26</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-12 14:09:57</t>
+          <t>2025-05-12 13:42:26</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-05-13 08:44:59</t>
+          <t>2025-05-13 07:55:40</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4461,7 +4461,7 @@
         </is>
       </c>
       <c r="R53" s="1" t="n">
-        <v>-25.36457702019676</v>
+        <v>0</v>
       </c>
       <c r="S53" t="n">
         <v>2</v>
@@ -4473,33 +4473,33 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>25</v>
+        <v>32.5</v>
       </c>
       <c r="D54" t="n">
-        <v>78.81967213114754</v>
+        <v>87.41818181818182</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-05-12 13:43:33</t>
+          <t>2025-05-12 13:35:27</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-12 14:08:33</t>
+          <t>2025-05-12 14:07:57</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-05-12 14:08:33</t>
+          <t>2025-05-12 14:07:57</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-05-13 07:27:22</t>
+          <t>2025-05-13 07:35:22</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4533,7 +4533,7 @@
         </is>
       </c>
       <c r="R54" s="1" t="n">
-        <v>-20.31067850637731</v>
+        <v>0</v>
       </c>
       <c r="S54" t="n">
         <v>2</v>
@@ -4545,33 +4545,33 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D55" t="n">
         <v>63.26229508196721</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-05-12 13:55:37</t>
+          <t>2025-05-12 13:43:33</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-12 14:28:37</t>
+          <t>2025-05-12 14:23:33</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-05-12 14:28:37</t>
+          <t>2025-05-12 14:23:33</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-05-13 07:31:53</t>
+          <t>2025-05-13 07:26:49</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4605,7 +4605,7 @@
         </is>
       </c>
       <c r="R55" s="1" t="n">
-        <v>-15.31380919854167</v>
+        <v>0</v>
       </c>
       <c r="S55" t="n">
         <v>2</v>
@@ -4617,33 +4617,33 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D56" t="n">
-        <v>74.14492753623189</v>
+        <v>72.05633802816901</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-05-12 14:50:21</t>
+          <t>2025-05-12 14:45:11</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-05-13 07:35:21</t>
+          <t>2025-05-13 07:04:11</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-05-13 07:35:21</t>
+          <t>2025-05-13 07:04:11</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-05-13 08:49:30</t>
+          <t>2025-05-13 08:16:15</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4677,7 +4677,7 @@
         </is>
       </c>
       <c r="R56" s="1" t="n">
-        <v>-15.36771336554398</v>
+        <v>0</v>
       </c>
       <c r="S56" t="n">
         <v>2</v>
@@ -4689,33 +4689,33 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D57" t="n">
-        <v>31.89795918367347</v>
+        <v>22.65217391304348</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-05-13 07:10:42</t>
+          <t>2025-05-12 14:50:21</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-13 07:52:42</t>
+          <t>2025-05-13 07:50:21</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-05-13 07:52:42</t>
+          <t>2025-05-13 07:50:21</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-05-13 08:24:36</t>
+          <t>2025-05-13 08:13:00</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4749,7 +4749,7 @@
         </is>
       </c>
       <c r="R57" s="1" t="n">
-        <v>-8.350425170069444</v>
+        <v>0</v>
       </c>
       <c r="S57" t="n">
         <v>2</v>
@@ -4761,33 +4761,33 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D58" t="n">
-        <v>70.4225352112676</v>
+        <v>102.0408163265306</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-05-13 07:14:23</t>
+          <t>2025-05-13 07:05:42</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-05-13 07:39:23</t>
+          <t>2025-05-13 08:00:42</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-05-13 07:39:23</t>
+          <t>2025-05-13 08:00:42</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2025-05-13 08:49:49</t>
+          <t>2025-05-13 09:42:45</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4821,7 +4821,7 @@
         </is>
       </c>
       <c r="R58" s="1" t="n">
-        <v>-7.367928403761574</v>
+        <v>0</v>
       </c>
       <c r="S58" t="n">
         <v>2</v>
@@ -4893,7 +4893,7 @@
         </is>
       </c>
       <c r="R59" s="1" t="n">
-        <v>-285.306660798125</v>
+        <v>0</v>
       </c>
       <c r="S59" t="n">
         <v>1</v>
@@ -4909,29 +4909,29 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D60" t="n">
         <v>217.6885245901639</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-05-13 07:27:22</t>
+          <t>2025-05-13 07:26:49</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-13 07:52:22</t>
+          <t>2025-05-13 08:06:49</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-05-13 07:52:22</t>
+          <t>2025-05-13 08:06:49</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-05-13 11:30:03</t>
+          <t>2025-05-13 11:44:30</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4977,33 +4977,33 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>29</v>
+        <v>32.5</v>
       </c>
       <c r="D61" t="n">
-        <v>16.34426229508197</v>
+        <v>18.12727272727273</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-05-13 07:31:53</t>
+          <t>2025-05-13 07:35:22</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-13 08:00:53</t>
+          <t>2025-05-13 08:07:52</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-05-13 08:00:53</t>
+          <t>2025-05-13 08:07:52</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-05-13 08:17:13</t>
+          <t>2025-05-13 08:26:00</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5037,7 +5037,7 @@
         </is>
       </c>
       <c r="R61" s="1" t="n">
-        <v>-225.3452982695833</v>
+        <v>0</v>
       </c>
       <c r="S61" t="n">
         <v>1</v>
@@ -5053,29 +5053,29 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D62" t="n">
         <v>12.36065573770492</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:17:13</t>
+          <t>2025-05-13 07:55:21</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:42:13</t>
+          <t>2025-05-13 08:24:21</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:42:13</t>
+          <t>2025-05-13 08:24:21</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:54:35</t>
+          <t>2025-05-13 08:36:43</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5109,7 +5109,7 @@
         </is>
       </c>
       <c r="R62" s="1" t="n">
-        <v>-56.37124316939815</v>
+        <v>0</v>
       </c>
       <c r="S62" t="n">
         <v>1</v>
@@ -5125,29 +5125,29 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D63" t="n">
         <v>11.78125</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-05-13 08:19:39</t>
+          <t>2025-05-13 07:55:40</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-13 08:38:39</t>
+          <t>2025-05-13 08:10:40</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-05-13 08:38:39</t>
+          <t>2025-05-13 08:10:40</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-05-13 08:50:26</t>
+          <t>2025-05-13 08:22:27</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5181,7 +5181,7 @@
         </is>
       </c>
       <c r="R63" s="1" t="n">
-        <v>-46.368359375</v>
+        <v>0</v>
       </c>
       <c r="S63" t="n">
         <v>1</v>
@@ -5193,33 +5193,33 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D64" t="n">
-        <v>489.734693877551</v>
+        <v>347.7826086956522</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-05-13 08:24:36</t>
+          <t>2025-05-13 08:13:00</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-05-13 09:11:36</t>
+          <t>2025-05-13 08:53:00</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-05-13 09:11:36</t>
+          <t>2025-05-13 08:53:00</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>2025-05-14 09:21:20</t>
+          <t>2025-05-13 14:40:47</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5253,7 +5253,7 @@
         </is>
       </c>
       <c r="R64" s="1" t="n">
-        <v>-9.389824263043982</v>
+        <v>0</v>
       </c>
       <c r="S64" t="n">
         <v>1</v>
@@ -5265,33 +5265,33 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>30.5</v>
+        <v>15</v>
       </c>
       <c r="D65" t="n">
-        <v>489.7090909090909</v>
+        <v>379.3521126760563</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-05-13 08:44:59</t>
+          <t>2025-05-13 08:16:15</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-05-13 09:15:29</t>
+          <t>2025-05-13 08:31:15</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-05-13 09:15:29</t>
+          <t>2025-05-13 08:31:15</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>2025-05-14 09:25:12</t>
+          <t>2025-05-13 14:50:36</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5325,7 +5325,7 @@
         </is>
       </c>
       <c r="R65" s="1" t="n">
-        <v>-5.3925</v>
+        <v>0</v>
       </c>
       <c r="S65" t="n">
         <v>1</v>
@@ -5337,33 +5337,33 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D66" t="n">
-        <v>173.9420289855072</v>
+        <v>187.53125</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-05-13 08:49:30</t>
+          <t>2025-05-13 08:22:27</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-05-13 09:14:30</t>
+          <t>2025-05-13 08:37:27</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-05-13 09:14:30</t>
+          <t>2025-05-13 08:37:27</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>2025-05-13 12:08:26</t>
+          <t>2025-05-13 11:44:59</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5397,7 +5397,7 @@
         </is>
       </c>
       <c r="R66" s="1" t="n">
-        <v>-4.505867552337963</v>
+        <v>0</v>
       </c>
       <c r="S66" t="n">
         <v>1</v>
@@ -5409,33 +5409,33 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>27</v>
+        <v>36.5</v>
       </c>
       <c r="D67" t="n">
-        <v>78.40845070422536</v>
+        <v>101.2181818181818</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-05-13 08:49:49</t>
+          <t>2025-05-13 08:26:00</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-05-13 09:16:49</t>
+          <t>2025-05-13 09:02:30</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-05-13 09:16:49</t>
+          <t>2025-05-13 09:02:30</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>2025-05-13 10:35:13</t>
+          <t>2025-05-13 10:43:43</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5469,7 +5469,7 @@
         </is>
       </c>
       <c r="R67" s="1" t="n">
-        <v>-4.441128716747685</v>
+        <v>0</v>
       </c>
       <c r="S67" t="n">
         <v>1</v>
@@ -5481,33 +5481,33 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D68" t="n">
-        <v>108.859375</v>
+        <v>114.2131147540984</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-05-13 08:50:26</t>
+          <t>2025-05-13 08:36:43</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-05-13 09:09:26</t>
+          <t>2025-05-13 09:05:43</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-05-13 09:09:26</t>
+          <t>2025-05-13 09:05:43</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>2025-05-13 10:58:17</t>
+          <t>2025-05-13 10:59:56</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5541,7 +5541,7 @@
         </is>
       </c>
       <c r="R68" s="1" t="n">
-        <v>-4.457150607638889</v>
+        <v>0</v>
       </c>
       <c r="S68" t="n">
         <v>1</v>
@@ -5553,33 +5553,33 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D69" t="n">
-        <v>117.2622950819672</v>
+        <v>145.9795918367347</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-05-13 08:54:35</t>
+          <t>2025-05-13 09:42:45</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-05-13 09:23:35</t>
+          <t>2025-05-13 10:42:45</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-05-13 09:23:35</t>
+          <t>2025-05-13 10:42:45</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2025-05-13 11:20:51</t>
+          <t>2025-05-13 13:08:44</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5613,7 +5613,7 @@
         </is>
       </c>
       <c r="R69" s="1" t="n">
-        <v>-4.472814207650463</v>
+        <v>0</v>
       </c>
       <c r="S69" t="n">
         <v>1</v>
@@ -5625,33 +5625,33 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="D70" t="n">
         <v>87.69014084507042</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-05-13 10:35:13</t>
+          <t>2025-05-13 09:58:10</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-05-13 10:52:13</t>
+          <t>2025-05-13 11:43:10</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-05-13 10:52:13</t>
+          <t>2025-05-13 11:43:10</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-05-13 12:19:54</t>
+          <t>2025-05-13 13:10:52</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5685,7 +5685,7 @@
         </is>
       </c>
       <c r="R70" s="1" t="n">
-        <v>-4.513830203437499</v>
+        <v>0</v>
       </c>
       <c r="S70" t="n">
         <v>1</v>
@@ -5697,33 +5697,33 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>19</v>
+        <v>32.5</v>
       </c>
       <c r="D71" t="n">
-        <v>97.28125</v>
+        <v>113.2</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-05-13 10:58:17</t>
+          <t>2025-05-13 10:43:43</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-05-13 11:17:17</t>
+          <t>2025-05-13 11:16:13</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-05-13 11:17:17</t>
+          <t>2025-05-13 11:16:13</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>2025-05-13 12:54:34</t>
+          <t>2025-05-13 13:09:25</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5757,7 +5757,7 @@
         </is>
       </c>
       <c r="R71" s="1" t="n">
-        <v>-4.537901475694444</v>
+        <v>0</v>
       </c>
       <c r="S71" t="n">
         <v>1</v>
@@ -5780,22 +5780,22 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-05-13 11:20:51</t>
+          <t>2025-05-13 10:59:56</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-05-13 11:49:51</t>
+          <t>2025-05-13 11:28:56</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-05-13 11:49:51</t>
+          <t>2025-05-13 11:28:56</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>2025-05-13 13:31:55</t>
+          <t>2025-05-13 13:11:00</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5829,7 +5829,7 @@
         </is>
       </c>
       <c r="R72" s="1" t="n">
-        <v>-4.563831967210648</v>
+        <v>0</v>
       </c>
       <c r="S72" t="n">
         <v>1</v>
@@ -5837,41 +5837,41 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>251520</v>
+        <v>251374</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="D73" t="n">
-        <v>230.1408450704225</v>
+        <v>448.2459016393443</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:38</t>
+          <t>2025-05-13 11:44:30</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-05-13 12:47:38</t>
+          <t>2025-05-13 12:19:30</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-05-13 12:47:38</t>
+          <t>2025-05-13 12:19:30</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>2025-05-14 08:37:47</t>
+          <t>2025-05-14 11:47:45</t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>16340</v>
+        <v>27343</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -5880,7 +5880,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L73" t="n">
@@ -5897,11 +5897,11 @@
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R73" s="1" t="n">
-        <v>-2.359575508611111</v>
+        <v>0</v>
       </c>
       <c r="S73" t="n">
         <v>1</v>
@@ -5909,41 +5909,41 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>251374</v>
+        <v>251580</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D74" t="n">
-        <v>448.2459016393443</v>
+        <v>111.765625</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-05-13 11:30:03</t>
+          <t>2025-05-13 11:44:59</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-05-13 12:05:03</t>
+          <t>2025-05-13 12:03:59</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-05-13 12:05:03</t>
+          <t>2025-05-13 12:03:59</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-05-14 11:33:18</t>
+          <t>2025-05-13 13:55:45</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>27343</v>
+        <v>7153</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -5952,11 +5952,11 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L74" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M74" t="n">
         <v>70</v>
@@ -5981,41 +5981,41 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>251580</v>
+        <v>251557</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D75" t="n">
-        <v>103.6666666666667</v>
+        <v>136.8367346938776</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-05-13 12:08:26</t>
+          <t>2025-05-13 13:08:44</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-05-13 12:43:26</t>
+          <t>2025-05-13 13:53:44</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-05-13 12:43:26</t>
+          <t>2025-05-13 13:53:44</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-05-13 14:27:06</t>
+          <t>2025-05-14 08:10:34</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>7153</v>
+        <v>6705</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
@@ -6028,7 +6028,7 @@
         </is>
       </c>
       <c r="L75" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M75" t="n">
         <v>70</v>
@@ -6053,41 +6053,41 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>251557</v>
+        <v>251520</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>15</v>
+        <v>40.5</v>
       </c>
       <c r="D76" t="n">
-        <v>94.43661971830986</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2025-05-13 12:19:54</t>
+          <t>2025-05-13 13:09:25</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-05-13 12:34:54</t>
+          <t>2025-05-13 13:49:55</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2025-05-13 12:34:54</t>
+          <t>2025-05-13 13:49:55</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>2025-05-13 14:09:21</t>
+          <t>2025-05-14 10:47:00</t>
         </is>
       </c>
       <c r="I76" t="n">
-        <v>6705</v>
+        <v>16340</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -6096,11 +6096,11 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L76" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M76" t="n">
         <v>70</v>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R76" s="1" t="n">
@@ -6129,33 +6129,33 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D77" t="n">
-        <v>127.21875</v>
+        <v>114.6760563380282</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2025-05-13 12:54:34</t>
+          <t>2025-05-13 13:10:52</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-05-13 13:09:34</t>
+          <t>2025-05-13 13:45:52</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>2025-05-13 13:09:34</t>
+          <t>2025-05-13 13:45:52</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>2025-05-14 07:16:47</t>
+          <t>2025-05-14 07:40:32</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6212,22 +6212,22 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-05-13 13:31:55</t>
+          <t>2025-05-13 13:11:00</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-05-13 14:04:55</t>
+          <t>2025-05-13 13:44:00</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>2025-05-13 14:04:55</t>
+          <t>2025-05-13 13:44:00</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>2025-05-14 08:38:30</t>
+          <t>2025-05-14 08:17:35</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6273,33 +6273,33 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D79" t="n">
-        <v>318.6478873239437</v>
+        <v>353.5</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2025-05-13 14:09:21</t>
+          <t>2025-05-13 13:55:45</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-05-13 14:32:21</t>
+          <t>2025-05-13 14:14:45</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>2025-05-13 14:32:21</t>
+          <t>2025-05-13 14:14:45</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>2025-05-14 11:51:00</t>
+          <t>2025-05-14 12:08:15</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6349,29 +6349,29 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D80" t="n">
         <v>218.5942028985507</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2025-05-13 14:27:06</t>
+          <t>2025-05-13 14:40:47</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-05-14 07:02:06</t>
+          <t>2025-05-14 07:05:47</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>2025-05-14 07:02:06</t>
+          <t>2025-05-14 07:05:47</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>2025-05-14 10:40:42</t>
+          <t>2025-05-14 10:44:23</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6417,33 +6417,33 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D81" t="n">
-        <v>247.8125</v>
+        <v>223.3802816901408</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2025-05-14 07:16:47</t>
+          <t>2025-05-13 14:50:36</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-05-14 07:39:47</t>
+          <t>2025-05-14 07:05:36</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2025-05-14 07:39:47</t>
+          <t>2025-05-14 07:05:36</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>2025-05-14 11:47:36</t>
+          <t>2025-05-14 10:48:59</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6557,41 +6557,41 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>251987</v>
+        <v>251249</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D83" t="n">
-        <v>2965.154929577465</v>
+        <v>97.10204081632654</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-05-14 08:33:23</t>
+          <t>2025-05-14 08:10:34</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-05-14 09:09:23</t>
+          <t>2025-05-14 09:05:34</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>2025-05-14 09:09:23</t>
+          <t>2025-05-14 09:05:34</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>2025-05-22 10:34:32</t>
+          <t>2025-05-14 10:42:40</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>210526</v>
+        <v>4758</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -6600,14 +6600,14 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L83" t="n">
         <v>6</v>
       </c>
       <c r="M83" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="O83" t="n">
         <v>0</v>
@@ -6617,7 +6617,7 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>2025-09-01 00:00:00</t>
+          <t>2025-06-06 00:00:00</t>
         </is>
       </c>
       <c r="R83" s="1" t="n">
@@ -6629,7 +6629,7 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>251249</v>
+        <v>251795</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -6640,30 +6640,30 @@
         <v>25</v>
       </c>
       <c r="D84" t="n">
-        <v>78</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-05-14 08:38:30</t>
+          <t>2025-05-14 08:17:35</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-05-14 09:03:30</t>
+          <t>2025-05-14 08:42:35</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2025-05-14 09:03:30</t>
+          <t>2025-05-14 08:42:35</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>2025-05-14 10:21:30</t>
+          <t>2025-05-14 13:49:47</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>4758</v>
+        <v>18739</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -6672,7 +6672,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L84" t="n">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>2025-06-06 00:00:00</t>
+          <t>2025-06-19 00:00:00</t>
         </is>
       </c>
       <c r="R84" s="1" t="n">
@@ -6701,41 +6701,41 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>251795</v>
+        <v>251987</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>30.5</v>
+        <v>36</v>
       </c>
       <c r="D85" t="n">
-        <v>340.7090909090909</v>
+        <v>2965.154929577465</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-05-14 09:25:12</t>
+          <t>2025-05-14 08:33:23</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-05-14 09:55:42</t>
+          <t>2025-05-14 09:09:23</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2025-05-14 09:55:42</t>
+          <t>2025-05-14 09:09:23</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>2025-05-15 07:36:24</t>
+          <t>2025-05-22 10:34:32</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>18739</v>
+        <v>210526</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -6744,14 +6744,14 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L85" t="n">
         <v>6</v>
       </c>
       <c r="M85" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="O85" t="n">
         <v>0</v>
@@ -6761,7 +6761,7 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>2025-06-19 00:00:00</t>
+          <t>2025-09-01 00:00:00</t>
         </is>
       </c>
       <c r="R85" s="1" t="n">
@@ -6777,33 +6777,33 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D86" t="n">
-        <v>8470.786885245901</v>
+        <v>7488.666666666667</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-05-14 10:21:30</t>
+          <t>2025-05-14 10:44:23</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-05-14 11:03:30</t>
+          <t>2025-05-14 11:19:23</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>2025-05-14 11:03:30</t>
+          <t>2025-05-14 11:19:23</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>2025-06-09 08:14:17</t>
+          <t>2025-06-05 08:08:03</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6849,33 +6849,33 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D87" t="n">
-        <v>1777.753623188406</v>
+        <v>1727.676056338028</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2025-05-14 10:40:42</t>
+          <t>2025-05-14 10:48:59</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-05-14 11:20:42</t>
+          <t>2025-05-14 11:22:59</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>2025-05-14 11:20:42</t>
+          <t>2025-05-14 11:22:59</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>2025-05-20 08:58:27</t>
+          <t>2025-05-20 08:10:39</t>
         </is>
       </c>
       <c r="I87" t="n">

</xml_diff>

<commit_message>
Non funzionano ancora in sequenza  LS2 e LS3
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -2671,14 +2671,14 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D30" t="n">
         <v>461.9718309859155</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-08 14:16:40</t>
+          <t>2025-05-08 14:14:40</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2955,33 +2955,33 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>34.5</v>
+        <v>200</v>
       </c>
       <c r="D34" t="n">
-        <v>259.1818181818182</v>
+        <v>200.7746478873239</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-09 12:29:25</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-05-09 13:12:05</t>
+          <t>2025-05-12 07:49:25</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-05-09 13:12:05</t>
+          <t>2025-05-12 07:49:25</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-05-12 09:31:16</t>
+          <t>2025-05-12 11:10:11</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3015,7 +3015,7 @@
         </is>
       </c>
       <c r="R34" s="1" t="n">
-        <v>-7.396717171712963</v>
+        <v>-7.465414710486112</v>
       </c>
       <c r="S34" t="n">
         <v>7</v>
@@ -3027,33 +3027,33 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>25</v>
+        <v>40.5</v>
       </c>
       <c r="D35" t="n">
-        <v>186.7540983606557</v>
+        <v>207.1272727272727</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-05-09 13:15:38</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-09 13:40:38</t>
+          <t>2025-05-09 13:18:05</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-05-09 13:40:38</t>
+          <t>2025-05-09 13:18:05</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-05-12 08:47:23</t>
+          <t>2025-05-12 08:45:13</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3110,22 +3110,22 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-05-09 13:19:51</t>
+          <t>2025-05-09 13:11:51</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-09 13:51:51</t>
+          <t>2025-05-09 13:43:51</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-05-09 13:51:51</t>
+          <t>2025-05-09 13:43:51</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-12 09:17:43</t>
+          <t>2025-05-12 09:09:43</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3171,33 +3171,33 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D37" t="n">
-        <v>348.8571428571428</v>
+        <v>280.2295081967213</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-05-09 13:37:56</t>
+          <t>2025-05-09 13:15:38</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-09 14:12:56</t>
+          <t>2025-05-09 13:45:38</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-05-09 14:12:56</t>
+          <t>2025-05-09 13:45:38</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-05-12 12:01:47</t>
+          <t>2025-05-12 10:25:52</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3231,7 +3231,7 @@
         </is>
       </c>
       <c r="R37" s="1" t="n">
-        <v>-14.50124716553241</v>
+        <v>-14.4346311475463</v>
       </c>
       <c r="S37" t="n">
         <v>4</v>
@@ -3239,41 +3239,41 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>245275</v>
+        <v>251424</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="D38" t="n">
-        <v>342.1690140845071</v>
+        <v>197.1836734693877</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-05-09 13:59:25</t>
+          <t>2025-05-09 13:37:56</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-05-12 07:04:25</t>
+          <t>2025-05-09 14:17:56</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-05-12 07:04:25</t>
+          <t>2025-05-09 14:17:56</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-05-12 12:46:35</t>
+          <t>2025-05-12 09:35:07</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>24294</v>
+        <v>9662</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3282,11 +3282,11 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L38" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="M38" t="n">
         <v>70</v>
@@ -3299,14 +3299,14 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>2025-12-31 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R38" s="1" t="n">
-        <v>0</v>
+        <v>-14.39939058957176</v>
       </c>
       <c r="S38" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -3527,41 +3527,41 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>251424</v>
+        <v>245275</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>30</v>
+        <v>54.5</v>
       </c>
       <c r="D42" t="n">
-        <v>158.3934426229508</v>
+        <v>441.7090909090909</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-05-12 08:47:23</t>
+          <t>2025-05-12 08:45:13</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-05-12 09:17:23</t>
+          <t>2025-05-12 09:39:43</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-05-12 09:17:23</t>
+          <t>2025-05-12 09:39:43</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-05-12 11:55:47</t>
+          <t>2025-05-13 09:01:25</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>9662</v>
+        <v>24294</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3570,11 +3570,11 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;CASON ;R6</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="M42" t="n">
         <v>70</v>
@@ -3587,14 +3587,14 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-12-31 00:00:00</t>
         </is>
       </c>
       <c r="R42" s="1" t="n">
-        <v>-14.49707422586805</v>
+        <v>0</v>
       </c>
       <c r="S42" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">
@@ -3614,22 +3614,22 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-05-12 09:17:43</t>
+          <t>2025-05-12 09:09:43</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-05-12 09:38:43</t>
+          <t>2025-05-12 09:30:43</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-05-12 09:38:43</t>
+          <t>2025-05-12 09:30:43</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-05-12 12:14:18</t>
+          <t>2025-05-12 12:06:18</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3663,7 +3663,7 @@
         </is>
       </c>
       <c r="R43" s="1" t="n">
-        <v>-553.5099392361111</v>
+        <v>-553.5043836805555</v>
       </c>
       <c r="S43" t="n">
         <v>4</v>
@@ -3675,33 +3675,33 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>34.5</v>
+        <v>40</v>
       </c>
       <c r="D44" t="n">
-        <v>98.81818181818181</v>
+        <v>110.9183673469388</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-05-12 09:31:16</t>
+          <t>2025-05-12 09:35:07</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-05-12 10:05:46</t>
+          <t>2025-05-12 10:15:07</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-05-12 10:05:46</t>
+          <t>2025-05-12 10:15:07</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-05-12 11:44:35</t>
+          <t>2025-05-12 12:06:02</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3735,7 +3735,7 @@
         </is>
       </c>
       <c r="R44" s="1" t="n">
-        <v>-14.48929924241898</v>
+        <v>-14.50419501134259</v>
       </c>
       <c r="S44" t="n">
         <v>4</v>
@@ -3747,33 +3747,33 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>32.5</v>
+        <v>25</v>
       </c>
       <c r="D45" t="n">
-        <v>157.8363636363636</v>
+        <v>142.3114754098361</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-05-12 11:44:35</t>
+          <t>2025-05-12 10:25:52</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-05-12 12:17:05</t>
+          <t>2025-05-12 10:50:52</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-05-12 12:17:05</t>
+          <t>2025-05-12 10:50:52</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-05-12 14:54:55</t>
+          <t>2025-05-12 13:13:10</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3807,7 +3807,7 @@
         </is>
       </c>
       <c r="R45" s="1" t="n">
-        <v>-12.62147727273148</v>
+        <v>-12.55081967212963</v>
       </c>
       <c r="S45" t="n">
         <v>4</v>
@@ -3819,33 +3819,33 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D46" t="n">
-        <v>106</v>
+        <v>91.07042253521126</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-05-12 11:55:47</t>
+          <t>2025-05-12 11:10:11</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-05-12 12:15:47</t>
+          <t>2025-05-12 11:50:11</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-05-12 12:15:47</t>
+          <t>2025-05-12 11:50:11</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-05-12 14:01:47</t>
+          <t>2025-05-12 13:21:16</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3879,7 +3879,7 @@
         </is>
       </c>
       <c r="R46" s="1" t="n">
-        <v>-5.584574225868056</v>
+        <v>-5.55643583724537</v>
       </c>
       <c r="S46" t="n">
         <v>4</v>
@@ -3974,22 +3974,22 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-05-12 12:01:47</t>
+          <t>2025-05-12 12:06:02</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-05-12 12:41:47</t>
+          <t>2025-05-12 12:46:02</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-05-12 12:41:47</t>
+          <t>2025-05-12 12:46:02</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-05-12 14:09:45</t>
+          <t>2025-05-12 14:14:00</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4023,7 +4023,7 @@
         </is>
       </c>
       <c r="R48" s="1" t="n">
-        <v>-4.59010770974537</v>
+        <v>-4.593055555555556</v>
       </c>
       <c r="S48" t="n">
         <v>4</v>
@@ -4046,22 +4046,22 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-05-12 12:14:18</t>
+          <t>2025-05-12 12:06:18</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-05-12 12:31:18</t>
+          <t>2025-05-12 12:23:18</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-05-12 12:31:18</t>
+          <t>2025-05-12 12:23:18</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-05-12 13:25:33</t>
+          <t>2025-05-12 13:17:33</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4095,7 +4095,7 @@
         </is>
       </c>
       <c r="R49" s="1" t="n">
-        <v>-4.559418402777778</v>
+        <v>-4.553862847222222</v>
       </c>
       <c r="S49" t="n">
         <v>4</v>
@@ -4179,33 +4179,33 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="D51" t="n">
-        <v>122.2676056338028</v>
+        <v>142.3114754098361</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-05-12 12:46:35</t>
+          <t>2025-05-12 13:13:10</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-05-12 14:11:35</t>
+          <t>2025-05-12 13:33:10</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-05-12 14:11:35</t>
+          <t>2025-05-12 13:33:10</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-05-13 08:13:51</t>
+          <t>2025-05-13 07:55:29</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4262,22 +4262,22 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-05-12 13:25:33</t>
+          <t>2025-05-12 13:17:33</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-05-12 13:44:33</t>
+          <t>2025-05-12 13:36:33</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-05-12 13:44:33</t>
+          <t>2025-05-12 13:36:33</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-05-13 07:57:47</t>
+          <t>2025-05-13 07:49:47</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4311,7 +4311,7 @@
         </is>
       </c>
       <c r="R52" s="1" t="n">
-        <v>-25.33180338541667</v>
+        <v>-25.32624782986111</v>
       </c>
       <c r="S52" t="n">
         <v>2</v>
@@ -4319,41 +4319,41 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>251485</v>
+        <v>251109</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="D53" t="n">
-        <v>67.71830985915493</v>
+        <v>266.5915492957747</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-05-12 13:30:39</t>
+          <t>2025-05-12 13:21:16</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-12 13:47:39</t>
+          <t>2025-05-12 14:56:16</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-12 13:47:39</t>
+          <t>2025-05-12 14:56:16</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-05-12 14:55:22</t>
+          <t>2025-05-13 11:22:51</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>4808</v>
+        <v>18928</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4362,11 +4362,11 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="L53" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="M53" t="n">
         <v>70</v>
@@ -4379,11 +4379,11 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-18 00:00:00</t>
         </is>
       </c>
       <c r="R53" s="1" t="n">
-        <v>-19.62179186228009</v>
+        <v>-25.47420774648148</v>
       </c>
       <c r="S53" t="n">
         <v>2</v>
@@ -4391,41 +4391,41 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>250670</v>
+        <v>251485</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D54" t="n">
-        <v>22.01408450704225</v>
+        <v>67.71830985915493</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-05-12 13:55:22</t>
+          <t>2025-05-12 13:30:39</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-12 14:29:22</t>
+          <t>2025-05-12 13:47:39</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-05-12 14:29:22</t>
+          <t>2025-05-12 13:47:39</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-05-12 14:51:23</t>
+          <t>2025-05-12 14:55:22</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>1563</v>
+        <v>4808</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -4434,14 +4434,14 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L54" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M54" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="O54" t="n">
         <v>0</v>
@@ -4451,11 +4451,11 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R54" s="1" t="n">
-        <v>-7.619023865416667</v>
+        <v>-19.62179186228009</v>
       </c>
       <c r="S54" t="n">
         <v>2</v>
@@ -4463,41 +4463,41 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>251346</v>
+        <v>250670</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D55" t="n">
-        <v>63.26229508196721</v>
+        <v>22.01408450704225</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-05-12 14:01:47</t>
+          <t>2025-05-12 13:55:22</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-12 14:41:47</t>
+          <t>2025-05-12 14:29:22</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-05-12 14:41:47</t>
+          <t>2025-05-12 14:29:22</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-05-13 07:45:02</t>
+          <t>2025-05-12 14:51:23</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>3859</v>
+        <v>1563</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -4506,14 +4506,14 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L55" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M55" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="O55" t="n">
         <v>0</v>
@@ -4523,11 +4523,11 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R55" s="1" t="n">
-        <v>-15.32295081967592</v>
+        <v>-7.619023865416667</v>
       </c>
       <c r="S55" t="n">
         <v>2</v>
@@ -4535,7 +4535,7 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>250641</v>
+        <v>251346</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -4543,33 +4543,33 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D56" t="n">
-        <v>104.4081632653061</v>
+        <v>78.75510204081633</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-05-12 14:09:45</t>
+          <t>2025-05-12 14:14:00</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-05-12 14:54:45</t>
+          <t>2025-05-13 07:09:00</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-05-12 14:54:45</t>
+          <t>2025-05-13 07:09:00</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-05-13 08:39:09</t>
+          <t>2025-05-13 08:27:45</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>5116</v>
+        <v>3859</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -4582,7 +4582,7 @@
         </is>
       </c>
       <c r="L56" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M56" t="n">
         <v>70</v>
@@ -4599,7 +4599,7 @@
         </is>
       </c>
       <c r="R56" s="1" t="n">
-        <v>-15.36053004534722</v>
+        <v>-15.35260770974537</v>
       </c>
       <c r="S56" t="n">
         <v>2</v>
@@ -4607,7 +4607,7 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>251259</v>
+        <v>250641</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -4615,10 +4615,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D57" t="n">
-        <v>72.46376811594203</v>
+        <v>74.14492753623189</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -4627,21 +4627,21 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-13 07:20:21</t>
+          <t>2025-05-13 07:35:21</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-05-13 07:20:21</t>
+          <t>2025-05-13 07:35:21</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-05-13 08:32:49</t>
+          <t>2025-05-13 08:49:30</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>5000</v>
+        <v>5116</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -4654,7 +4654,7 @@
         </is>
       </c>
       <c r="L57" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M57" t="n">
         <v>70</v>
@@ -4667,11 +4667,11 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R57" s="1" t="n">
-        <v>-7.356129227048611</v>
+        <v>-15.36771336554398</v>
       </c>
       <c r="S57" t="n">
         <v>2</v>
@@ -4751,41 +4751,41 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>251761</v>
+        <v>251259</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>30.5</v>
+        <v>23</v>
       </c>
       <c r="D59" t="n">
-        <v>241.4363636363636</v>
+        <v>70.4225352112676</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-05-12 14:54:55</t>
+          <t>2025-05-12 14:55:22</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-05-13 07:25:25</t>
+          <t>2025-05-13 07:18:22</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-05-13 07:25:25</t>
+          <t>2025-05-13 07:18:22</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2025-05-13 11:26:51</t>
+          <t>2025-05-13 08:28:48</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>13279</v>
+        <v>5000</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -4798,7 +4798,7 @@
         </is>
       </c>
       <c r="L59" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M59" t="n">
         <v>70</v>
@@ -4811,11 +4811,11 @@
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>2025-05-19 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R59" s="1" t="n">
-        <v>0</v>
+        <v>-7.353335289513889</v>
       </c>
       <c r="S59" t="n">
         <v>2</v>
@@ -4823,41 +4823,41 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>244023</v>
+        <v>251761</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D60" t="n">
-        <v>14.04225352112676</v>
+        <v>207.484375</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-05-12 14:55:22</t>
+          <t>2025-05-13 07:49:47</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-13 07:12:22</t>
+          <t>2025-05-13 08:08:47</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-05-13 07:12:22</t>
+          <t>2025-05-13 08:08:47</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-05-13 07:26:25</t>
+          <t>2025-05-13 11:36:16</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>997</v>
+        <v>13279</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4870,7 +4870,7 @@
         </is>
       </c>
       <c r="L60" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M60" t="n">
         <v>70</v>
@@ -4883,53 +4883,53 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>2024-09-30 00:00:00</t>
+          <t>2025-05-19 00:00:00</t>
         </is>
       </c>
       <c r="R60" s="1" t="n">
-        <v>-225.310015649456</v>
+        <v>0</v>
       </c>
       <c r="S60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>251283</v>
+        <v>244023</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D61" t="n">
-        <v>10.61971830985915</v>
+        <v>16.34426229508197</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-05-13 07:26:25</t>
+          <t>2025-05-13 07:55:21</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-13 07:41:25</t>
+          <t>2025-05-13 08:24:21</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-05-13 07:41:25</t>
+          <t>2025-05-13 08:24:21</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-05-13 07:52:02</t>
+          <t>2025-05-13 08:40:42</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>754</v>
+        <v>997</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -4938,7 +4938,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L61" t="n">
@@ -4955,11 +4955,11 @@
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>2025-03-18 00:00:00</t>
+          <t>2024-09-30 00:00:00</t>
         </is>
       </c>
       <c r="R61" s="1" t="n">
-        <v>-56.32780712049768</v>
+        <v>-225.3616006375231</v>
       </c>
       <c r="S61" t="n">
         <v>1</v>
@@ -4967,7 +4967,7 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>251245</v>
+        <v>251283</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -4982,22 +4982,22 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-05-13 07:45:02</t>
+          <t>2025-05-13 07:55:29</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:15:02</t>
+          <t>2025-05-13 08:25:29</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:15:02</t>
+          <t>2025-05-13 08:25:29</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-05-13 08:27:24</t>
+          <t>2025-05-13 08:37:51</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5027,11 +5027,11 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>2025-03-28 00:00:00</t>
+          <t>2025-03-18 00:00:00</t>
         </is>
       </c>
       <c r="R62" s="1" t="n">
-        <v>-46.35236794171296</v>
+        <v>-56.35961976320601</v>
       </c>
       <c r="S62" t="n">
         <v>1</v>
@@ -5039,41 +5039,41 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>251061</v>
+        <v>251245</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="D63" t="n">
-        <v>337.9859154929578</v>
+        <v>15.38775510204082</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-05-13 07:52:02</t>
+          <t>2025-05-13 08:27:45</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:02</t>
+          <t>2025-05-13 09:12:45</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-05-13 08:07:02</t>
+          <t>2025-05-13 09:12:45</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-05-13 13:45:01</t>
+          <t>2025-05-13 09:28:08</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>23997</v>
+        <v>754</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -5099,11 +5099,11 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-03-28 00:00:00</t>
         </is>
       </c>
       <c r="R63" s="1" t="n">
-        <v>-8.572936228483796</v>
+        <v>-46.39454365079861</v>
       </c>
       <c r="S63" t="n">
         <v>1</v>
@@ -5111,41 +5111,41 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>251247</v>
+        <v>251061</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D64" t="n">
-        <v>441.5409836065574</v>
+        <v>337.9859154929578</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-05-13 07:55:21</t>
+          <t>2025-05-13 08:28:48</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-05-13 08:24:21</t>
+          <t>2025-05-13 08:49:48</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-05-13 08:24:21</t>
+          <t>2025-05-13 08:49:48</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>2025-05-14 07:45:54</t>
+          <t>2025-05-13 14:27:47</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>26934</v>
+        <v>23997</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -5171,11 +5171,11 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R64" s="1" t="n">
-        <v>-5.323542805104167</v>
+        <v>-8.602631064166665</v>
       </c>
       <c r="S64" t="n">
         <v>1</v>
@@ -5183,41 +5183,41 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>251246</v>
+        <v>251247</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D65" t="n">
-        <v>187.53125</v>
+        <v>441.5409836065574</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-05-13 07:57:47</t>
+          <t>2025-05-13 08:37:51</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-05-13 08:12:47</t>
+          <t>2025-05-13 08:57:51</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-05-13 08:12:47</t>
+          <t>2025-05-13 08:57:51</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>2025-05-13 11:20:19</t>
+          <t>2025-05-14 08:19:23</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>12002</v>
+        <v>26934</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -5247,7 +5247,7 @@
         </is>
       </c>
       <c r="R65" s="1" t="n">
-        <v>-4.472450086805556</v>
+        <v>-5.34680100181713</v>
       </c>
       <c r="S65" t="n">
         <v>1</v>
@@ -5255,41 +5255,41 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>251109</v>
+        <v>251246</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="D66" t="n">
-        <v>266.5915492957747</v>
+        <v>196.7540983606557</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-05-13 08:13:51</t>
+          <t>2025-05-13 08:40:42</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-05-13 09:48:51</t>
+          <t>2025-05-13 09:05:42</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-05-13 09:48:51</t>
+          <t>2025-05-13 09:05:42</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>2025-05-13 14:15:27</t>
+          <t>2025-05-13 12:22:27</t>
         </is>
       </c>
       <c r="I66" t="n">
-        <v>18928</v>
+        <v>12002</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -5298,11 +5298,11 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L66" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="M66" t="n">
         <v>70</v>
@@ -5315,14 +5315,14 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>2025-04-18 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R66" s="1" t="n">
-        <v>-25.59406298905093</v>
+        <v>-4.515596539166667</v>
       </c>
       <c r="S66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -5331,33 +5331,33 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D67" t="n">
-        <v>91.26229508196721</v>
+        <v>80.68115942028986</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-05-13 08:27:24</t>
+          <t>2025-05-13 08:49:30</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-05-13 09:02:24</t>
+          <t>2025-05-13 09:29:30</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-05-13 09:02:24</t>
+          <t>2025-05-13 09:29:30</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>2025-05-13 10:33:40</t>
+          <t>2025-05-13 10:50:11</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5391,7 +5391,7 @@
         </is>
       </c>
       <c r="R67" s="1" t="n">
-        <v>-4.440050091076388</v>
+        <v>-4.45151972625</v>
       </c>
       <c r="S67" t="n">
         <v>1</v>
@@ -5403,33 +5403,33 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>50</v>
+        <v>50.5</v>
       </c>
       <c r="D68" t="n">
-        <v>100.9710144927536</v>
+        <v>126.6727272727273</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-05-13 08:32:49</t>
+          <t>2025-05-13 09:01:25</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-05-13 09:22:49</t>
+          <t>2025-05-13 09:51:55</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-05-13 09:22:49</t>
+          <t>2025-05-13 09:51:55</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>2025-05-13 11:03:47</t>
+          <t>2025-05-13 11:58:36</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5463,7 +5463,7 @@
         </is>
       </c>
       <c r="R68" s="1" t="n">
-        <v>-4.460970209340278</v>
+        <v>-4.499027777777778</v>
       </c>
       <c r="S68" t="n">
         <v>1</v>
@@ -5486,22 +5486,22 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-05-13 08:39:09</t>
+          <t>2025-05-13 09:28:08</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-05-13 09:24:09</t>
+          <t>2025-05-13 10:13:08</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-05-13 09:24:09</t>
+          <t>2025-05-13 10:13:08</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2025-05-13 11:50:08</t>
+          <t>2025-05-13 12:39:07</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5535,7 +5535,7 @@
         </is>
       </c>
       <c r="R69" s="1" t="n">
-        <v>-4.493154761909723</v>
+        <v>-4.527168367349537</v>
       </c>
       <c r="S69" t="n">
         <v>1</v>
@@ -5547,33 +5547,33 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D70" t="n">
-        <v>102.0655737704918</v>
+        <v>90.23188405797102</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-05-13 10:33:40</t>
+          <t>2025-05-13 10:50:11</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-05-13 10:58:40</t>
+          <t>2025-05-13 11:20:11</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-05-13 10:58:40</t>
+          <t>2025-05-13 11:20:11</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-05-13 12:40:44</t>
+          <t>2025-05-13 12:50:25</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5607,7 +5607,7 @@
         </is>
       </c>
       <c r="R70" s="1" t="n">
-        <v>-4.528290072858796</v>
+        <v>-4.535014090173611</v>
       </c>
       <c r="S70" t="n">
         <v>1</v>
@@ -5619,33 +5619,33 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="D71" t="n">
-        <v>90.23188405797102</v>
+        <v>87.69014084507042</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>2025-05-13 11:03:47</t>
+          <t>2025-05-13 11:22:51</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-05-13 11:38:47</t>
+          <t>2025-05-13 13:07:51</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025-05-13 11:38:47</t>
+          <t>2025-05-13 13:07:51</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>2025-05-13 13:09:01</t>
+          <t>2025-05-13 14:35:32</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5679,7 +5679,7 @@
         </is>
       </c>
       <c r="R71" s="1" t="n">
-        <v>-4.547936795486111</v>
+        <v>-4.608020344282407</v>
       </c>
       <c r="S71" t="n">
         <v>1</v>
@@ -5695,29 +5695,29 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D72" t="n">
         <v>97.28125</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-05-13 11:20:19</t>
+          <t>2025-05-13 11:36:16</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-05-13 11:43:19</t>
+          <t>2025-05-13 11:55:16</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-05-13 11:43:19</t>
+          <t>2025-05-13 11:55:16</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>2025-05-13 13:20:36</t>
+          <t>2025-05-13 13:32:33</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5751,7 +5751,7 @@
         </is>
       </c>
       <c r="R72" s="1" t="n">
-        <v>-4.555978732638889</v>
+        <v>-4.564279513888889</v>
       </c>
       <c r="S72" t="n">
         <v>1</v>
@@ -5774,22 +5774,22 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-05-13 11:26:51</t>
+          <t>2025-05-13 11:58:36</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-05-13 12:03:21</t>
+          <t>2025-05-13 12:35:06</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-05-13 12:03:21</t>
+          <t>2025-05-13 12:35:06</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>2025-05-14 09:00:27</t>
+          <t>2025-05-14 09:32:11</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5823,7 +5823,7 @@
         </is>
       </c>
       <c r="R73" s="1" t="n">
-        <v>-2.3753156565625</v>
+        <v>-2.397354797974537</v>
       </c>
       <c r="S73" t="n">
         <v>1</v>
@@ -5835,33 +5835,33 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D74" t="n">
-        <v>558.0204081632653</v>
+        <v>448.2459016393443</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-05-13 11:50:08</t>
+          <t>2025-05-13 12:22:27</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-05-13 12:40:08</t>
+          <t>2025-05-13 12:49:27</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-05-13 12:40:08</t>
+          <t>2025-05-13 12:49:27</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-05-14 13:58:09</t>
+          <t>2025-05-14 12:17:42</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -5907,33 +5907,33 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D75" t="n">
-        <v>117.2622950819672</v>
+        <v>145.9795918367347</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-05-13 12:40:44</t>
+          <t>2025-05-13 12:39:07</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-05-13 13:10:44</t>
+          <t>2025-05-13 13:14:07</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-05-13 13:10:44</t>
+          <t>2025-05-13 13:14:07</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-05-14 07:08:00</t>
+          <t>2025-05-14 07:40:06</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -5990,22 +5990,22 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2025-05-13 13:09:01</t>
+          <t>2025-05-13 12:50:25</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-05-13 13:34:01</t>
+          <t>2025-05-13 13:15:25</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>2025-05-13 13:34:01</t>
+          <t>2025-05-13 13:15:25</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>2025-05-14 07:11:12</t>
+          <t>2025-05-13 14:52:35</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6062,22 +6062,22 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2025-05-13 13:20:36</t>
+          <t>2025-05-13 13:32:33</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-05-13 13:35:36</t>
+          <t>2025-05-13 13:47:33</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>2025-05-13 13:35:36</t>
+          <t>2025-05-13 13:47:33</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>2025-05-14 07:42:49</t>
+          <t>2025-05-14 07:54:46</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6134,22 +6134,22 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2025-05-13 13:45:01</t>
+          <t>2025-05-13 14:27:47</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-05-13 14:00:01</t>
+          <t>2025-05-13 14:42:47</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>2025-05-13 14:00:01</t>
+          <t>2025-05-13 14:42:47</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>2025-05-14 08:11:59</t>
+          <t>2025-05-14 08:54:44</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6191,41 +6191,41 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>251750</v>
+        <v>251062</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D79" t="n">
-        <v>54.80281690140845</v>
+        <v>327.8840579710145</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2025-05-14 07:06:14</t>
+          <t>2025-05-13 14:52:35</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-05-14 07:23:14</t>
+          <t>2025-05-14 07:37:35</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>2025-05-14 07:23:14</t>
+          <t>2025-05-14 07:37:35</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>2025-05-14 08:18:02</t>
+          <t>2025-05-14 13:05:28</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>3891</v>
+        <v>22624</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -6234,14 +6234,14 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L79" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M79" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="O79" t="n">
         <v>0</v>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>2025-05-26 00:00:00</t>
+          <t>2025-05-23 00:00:00</t>
         </is>
       </c>
       <c r="R79" s="1" t="n">
@@ -6263,41 +6263,41 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>251062</v>
+        <v>251750</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D80" t="n">
-        <v>370.8852459016393</v>
+        <v>54.80281690140845</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2025-05-14 07:08:00</t>
+          <t>2025-05-14 07:06:14</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-05-14 07:38:00</t>
+          <t>2025-05-14 07:23:14</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>2025-05-14 07:38:00</t>
+          <t>2025-05-14 07:23:14</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>2025-05-14 13:48:53</t>
+          <t>2025-05-14 08:18:02</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>22624</v>
+        <v>3891</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -6306,14 +6306,14 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M80" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="O80" t="n">
         <v>0</v>
@@ -6323,7 +6323,7 @@
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>2025-05-23 00:00:00</t>
+          <t>2025-05-26 00:00:00</t>
         </is>
       </c>
       <c r="R80" s="1" t="n">
@@ -6339,33 +6339,33 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C81" t="n">
         <v>45</v>
       </c>
       <c r="D81" t="n">
-        <v>218.5942028985507</v>
+        <v>307.8163265306122</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2025-05-14 07:11:12</t>
+          <t>2025-05-14 07:40:06</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-05-14 07:56:12</t>
+          <t>2025-05-14 08:25:06</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>2025-05-14 07:56:12</t>
+          <t>2025-05-14 08:25:06</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>2025-05-14 11:34:47</t>
+          <t>2025-05-14 13:32:55</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6422,22 +6422,22 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2025-05-14 07:42:49</t>
+          <t>2025-05-14 07:54:46</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-05-14 08:05:49</t>
+          <t>2025-05-14 08:17:46</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>2025-05-14 08:05:49</t>
+          <t>2025-05-14 08:17:46</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>2025-05-14 12:13:38</t>
+          <t>2025-05-14 12:25:35</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6479,41 +6479,41 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>251249</v>
+        <v>251987</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D83" t="n">
-        <v>78</v>
+        <v>2965.154929577465</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2025-05-14 07:45:54</t>
+          <t>2025-05-14 08:18:02</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-05-14 08:10:54</t>
+          <t>2025-05-14 08:54:02</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>2025-05-14 08:10:54</t>
+          <t>2025-05-14 08:54:02</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>2025-05-14 09:28:54</t>
+          <t>2025-05-22 10:19:11</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>4758</v>
+        <v>210526</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -6522,14 +6522,14 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L83" t="n">
         <v>6</v>
       </c>
       <c r="M83" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="O83" t="n">
         <v>0</v>
@@ -6539,7 +6539,7 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>2025-06-06 00:00:00</t>
+          <t>2025-09-01 00:00:00</t>
         </is>
       </c>
       <c r="R83" s="1" t="n">
@@ -6551,41 +6551,41 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>251795</v>
+        <v>251249</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D84" t="n">
-        <v>263.9295774647887</v>
+        <v>78</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2025-05-14 08:11:59</t>
+          <t>2025-05-14 08:19:23</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-05-14 08:26:59</t>
+          <t>2025-05-14 08:39:23</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2025-05-14 08:26:59</t>
+          <t>2025-05-14 08:39:23</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>2025-05-14 12:50:54</t>
+          <t>2025-05-14 09:57:23</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>18739</v>
+        <v>4758</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
@@ -6594,7 +6594,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L84" t="n">
@@ -6611,7 +6611,7 @@
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>2025-06-19 00:00:00</t>
+          <t>2025-06-06 00:00:00</t>
         </is>
       </c>
       <c r="R84" s="1" t="n">
@@ -6623,41 +6623,41 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>251987</v>
+        <v>251795</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D85" t="n">
-        <v>2965.154929577465</v>
+        <v>263.9295774647887</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2025-05-14 08:18:02</t>
+          <t>2025-05-14 08:54:44</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-05-14 08:54:02</t>
+          <t>2025-05-14 09:09:44</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2025-05-14 08:54:02</t>
+          <t>2025-05-14 09:09:44</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>2025-05-22 10:19:11</t>
+          <t>2025-05-14 13:33:40</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>210526</v>
+        <v>18739</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -6666,14 +6666,14 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L85" t="n">
         <v>6</v>
       </c>
       <c r="M85" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="O85" t="n">
         <v>0</v>
@@ -6683,7 +6683,7 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>2025-09-01 00:00:00</t>
+          <t>2025-06-19 00:00:00</t>
         </is>
       </c>
       <c r="R85" s="1" t="n">
@@ -6703,29 +6703,29 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D86" t="n">
         <v>8470.786885245901</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2025-05-14 09:28:54</t>
+          <t>2025-05-14 12:17:42</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-05-14 10:10:54</t>
+          <t>2025-05-14 13:01:42</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>2025-05-14 10:10:54</t>
+          <t>2025-05-14 13:01:42</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>2025-06-09 07:21:41</t>
+          <t>2025-06-09 10:12:29</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6771,33 +6771,33 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D87" t="n">
-        <v>1777.753623188406</v>
+        <v>1916.640625</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2025-05-14 11:34:47</t>
+          <t>2025-05-14 12:25:35</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-05-14 12:14:47</t>
+          <t>2025-05-14 12:59:35</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>2025-05-14 12:14:47</t>
+          <t>2025-05-14 12:59:35</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>2025-05-20 09:52:33</t>
+          <t>2025-05-20 12:56:14</t>
         </is>
       </c>
       <c r="I87" t="n">

</xml_diff>

<commit_message>
Risoluzione di piccoli errori e debugging
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -671,7 +671,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251218</v>
+        <v>251752</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -679,10 +679,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>96.90140845070422</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -691,21 +691,21 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-06-04 12:23:00</t>
+          <t>2025-06-04 12:17:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-06-04 12:23:00</t>
+          <t>2025-06-04 12:17:00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-06-04 13:59:54</t>
+          <t>2025-06-04 12:17:00</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>6880</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -714,17 +714,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M4" t="n">
         <v>76</v>
       </c>
       <c r="N4" t="n">
-        <v>39885</v>
+        <v>39846</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -732,15 +732,15 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39885</v>
+        <v>39846</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-20 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0</v>
+        <v>-0.5118055555555555</v>
       </c>
       <c r="S4" t="n">
         <v>1</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251752</v>
+        <v>251218</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -759,30 +759,30 @@
         <v>21</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>96.90140845070422</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-06-04 13:59:54</t>
+          <t>2025-06-04 12:17:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-06-04 14:20:54</t>
+          <t>2025-06-04 12:38:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-06-04 14:20:54</t>
+          <t>2025-06-04 12:38:00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-06-04 14:20:54</t>
+          <t>2025-06-04 14:14:54</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>6880</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -791,17 +791,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M5" t="n">
         <v>76</v>
       </c>
       <c r="N5" t="n">
-        <v>39846</v>
+        <v>39885</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -809,15 +809,15 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>39846</v>
+        <v>39885</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-05-20 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-0.5978482003125</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
         <v>1</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251500</v>
+        <v>251565</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -833,14 +833,14 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D6" t="n">
-        <v>139.3802816901408</v>
+        <v>176.7464788732394</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-06-04 14:20:54</t>
+          <t>2025-06-04 14:14:54</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -855,11 +855,11 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-06-05 09:12:16</t>
+          <t>2025-06-05 09:49:38</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>9896</v>
+        <v>12549</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -868,11 +868,11 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M6" t="n">
         <v>70</v>
@@ -890,19 +890,19 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-26 00:00:00</t>
+          <t>2025-06-10 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-0.3835289514814815</v>
+        <v>-0.409477699525463</v>
       </c>
       <c r="S6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251565</v>
+        <v>251500</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -913,21 +913,21 @@
         <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>176.7464788732394</v>
+        <v>139.3802816901408</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-06-05 09:12:16</t>
+          <t>2025-06-05 09:49:38</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-06-05 09:31:16</t>
+          <t>2025-06-05 10:08:38</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-06-05 09:31:16</t>
+          <t>2025-06-05 10:08:38</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>12549</v>
+        <v>9896</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -945,11 +945,11 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
@@ -967,19 +967,19 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-06-10 00:00:00</t>
+          <t>2025-05-26 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
         <v>-0.5194640062615741</v>
       </c>
       <c r="S7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251180</v>
+        <v>251070</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>32.5</v>
+        <v>36.5</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -999,17 +999,17 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-06-05 07:32:30</t>
+          <t>2025-06-05 07:36:30</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-06-05 07:32:30</t>
+          <t>2025-06-05 07:36:30</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-06-05 07:32:30</t>
+          <t>2025-06-05 07:36:30</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1022,19 +1022,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>39887 (esterno)</t>
-        </is>
+      <c r="N8" t="n">
+        <v>39885</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,23 +1040,23 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39887</v>
+        <v>39885</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-05-20 00:00:00</t>
+          <t>2025-03-28 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-16.31423611111111</v>
+        <v>-0.3170138888888889</v>
       </c>
       <c r="S8" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251070</v>
+        <v>251773</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1066,29 +1064,29 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-06-05 07:32:30</t>
+          <t>2025-06-05 07:36:30</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-06-05 08:07:00</t>
+          <t>2025-06-05 08:09:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-06-05 08:07:00</t>
+          <t>2025-06-05 08:09:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-06-05 08:07:00</t>
+          <t>2025-06-05 08:09:00</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1101,17 +1099,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
       <c r="N9" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1119,23 +1117,23 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-03-28 00:00:00</t>
+          <t>2025-05-25 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-0.3381944444444445</v>
+        <v>-0.3395833333333333</v>
       </c>
       <c r="S9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251773</v>
+        <v>251180</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1143,29 +1141,29 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>32.5</v>
+        <v>36.5</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-06-05 08:07:00</t>
+          <t>2025-06-05 08:09:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-06-05 08:39:30</t>
+          <t>2025-06-05 08:45:30</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-06-05 08:39:30</t>
+          <t>2025-06-05 08:45:30</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-06-05 08:39:30</t>
+          <t>2025-06-05 08:45:30</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1178,17 +1176,19 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
       </c>
-      <c r="N10" t="n">
-        <v>39874</v>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>39887 (esterno)</t>
+        </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1196,18 +1196,18 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>39874</v>
+        <v>39887</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-05-25 00:00:00</t>
+          <t>2025-05-20 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-0.3607638888888889</v>
+        <v>-16.36493055555556</v>
       </c>
       <c r="S10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
@@ -1220,29 +1220,29 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>36.5</v>
+        <v>42.5</v>
       </c>
       <c r="D11" t="n">
         <v>321.7090909090909</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-06-05 08:39:30</t>
+          <t>2025-06-05 08:45:30</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-06-05 09:16:00</t>
+          <t>2025-06-05 09:28:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-06-05 09:16:00</t>
+          <t>2025-06-05 09:28:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-06-05 14:37:42</t>
+          <t>2025-06-05 14:49:42</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1283,7 +1283,7 @@
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-10.60952020202546</v>
+        <v>-10.6178535353588</v>
       </c>
       <c r="S11" t="n">
         <v>4</v>
@@ -1306,22 +1306,22 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-06-05 14:37:42</t>
+          <t>2025-06-05 14:49:42</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-06-06 07:22:12</t>
+          <t>2025-06-06 07:34:12</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-06-06 07:22:12</t>
+          <t>2025-06-06 07:34:12</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-06-06 14:44:00</t>
+          <t>2025-06-06 14:56:00</t>
         </is>
       </c>
       <c r="I12" t="n">

</xml_diff>

<commit_message>
Introdotto tracciamento ritardo pesato
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -748,7 +748,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251895</v>
+        <v>251218</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D5" t="n">
-        <v>249.2112676056338</v>
+        <v>96.90140845070422</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -768,21 +768,21 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-06-04 13:36:16</t>
+          <t>2025-06-04 13:13:16</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-06-04 13:36:16</t>
+          <t>2025-06-04 13:13:16</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-06-05 09:45:29</t>
+          <t>2025-06-04 14:50:10</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>17694</v>
+        <v>6880</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -791,19 +791,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M5" t="n">
-        <v>70</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>39891 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N5" t="n">
+        <v>39885</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -811,23 +809,23 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>39891</v>
+        <v>39885</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-05-26 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-10.40659233177083</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251218</v>
+        <v>251180</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -835,33 +833,33 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" t="n">
-        <v>96.90140845070422</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-06-05 09:45:29</t>
+          <t>2025-06-04 14:50:10</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-06-05 10:23:29</t>
+          <t>2025-06-05 07:24:10</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-06-05 10:23:29</t>
+          <t>2025-06-05 07:24:10</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-06-05 12:00:23</t>
+          <t>2025-06-05 07:24:10</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>6880</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -870,17 +868,19 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M6" t="n">
-        <v>76</v>
-      </c>
-      <c r="N6" t="n">
-        <v>39885</v>
+        <v>70</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>39887 (esterno)</t>
+        </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -888,23 +888,23 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39885</v>
+        <v>39887</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-20 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-0.5002738654166667</v>
+        <v>-16.30846048512732</v>
       </c>
       <c r="S6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251752</v>
+        <v>251780</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -912,33 +912,33 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>342.2394366197183</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-06-05 12:00:23</t>
+          <t>2025-06-05 07:24:10</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-06-05 12:21:23</t>
+          <t>2025-06-05 07:41:10</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-06-05 12:21:23</t>
+          <t>2025-06-05 07:41:10</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-06-05 12:21:23</t>
+          <t>2025-06-05 13:23:25</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>24299</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -947,17 +947,19 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
         <v>3</v>
       </c>
       <c r="M7" t="n">
-        <v>76</v>
-      </c>
-      <c r="N7" t="n">
-        <v>39846</v>
+        <v>70</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>39887 (esterno)</t>
+        </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -965,23 +967,23 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39846</v>
+        <v>39887</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-20 00:00:00</t>
+          <t>2025-06-18 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-1.51485719875</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251565</v>
+        <v>251895</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -989,33 +991,33 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" t="n">
-        <v>176.7464788732394</v>
+        <v>249.2112676056338</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-06-05 12:21:23</t>
+          <t>2025-06-05 13:23:25</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-06-05 12:53:23</t>
+          <t>2025-06-05 13:52:25</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-06-05 12:53:23</t>
+          <t>2025-06-05 13:52:25</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-06-06 07:50:08</t>
+          <t>2025-06-06 10:01:38</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>12549</v>
+        <v>17694</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1024,17 +1026,19 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M8" t="n">
         <v>70</v>
       </c>
-      <c r="N8" t="n">
-        <v>39885</v>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>39891 (esterno)</t>
+        </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,57 +1046,57 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39885</v>
+        <v>39891</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-06-10 00:00:00</t>
+          <t>2025-05-26 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.326486697962963</v>
+        <v>-11.41780125195602</v>
       </c>
       <c r="S8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251780</v>
+        <v>251500</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>32.5</v>
       </c>
       <c r="D9" t="n">
-        <v>342.2394366197183</v>
+        <v>179.9272727272727</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-06-06 07:50:08</t>
+          <t>2025-06-05 07:00:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-06-06 08:07:08</t>
+          <t>2025-06-05 07:32:30</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-06-06 08:07:08</t>
+          <t>2025-06-05 07:32:30</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-06-06 13:49:22</t>
+          <t>2025-06-05 10:32:25</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>24299</v>
+        <v>9896</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1101,19 +1105,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>39887 (esterno)</t>
-        </is>
+      <c r="N9" t="n">
+        <v>39885</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1121,23 +1123,23 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39887</v>
+        <v>39885</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-06-18 00:00:00</t>
+          <t>2025-05-26 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>0</v>
+        <v>-0.4391856060648148</v>
       </c>
       <c r="S9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251070</v>
+        <v>252282</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1145,33 +1147,33 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>36.5</v>
+        <v>32.5</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>49.78181818181818</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-06-05 07:00:00</t>
+          <t>2025-06-05 10:32:25</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-06-05 07:36:30</t>
+          <t>2025-06-05 11:04:55</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-06-05 07:36:30</t>
+          <t>2025-06-05 11:04:55</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-06-05 07:36:30</t>
+          <t>2025-06-05 11:54:42</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>2738</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1180,11 +1182,11 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
@@ -1202,19 +1204,19 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-03-28 00:00:00</t>
+          <t>2025-06-09 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-0.3170138888888889</v>
+        <v>-0.4963257575810185</v>
       </c>
       <c r="S10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251500</v>
+        <v>251070</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1222,33 +1224,33 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
       <c r="D11" t="n">
-        <v>179.9272727272727</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-06-05 07:36:30</t>
+          <t>2025-06-05 11:54:42</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-06-05 08:11:00</t>
+          <t>2025-06-05 12:27:12</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-06-05 08:11:00</t>
+          <t>2025-06-05 12:27:12</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-06-05 11:10:55</t>
+          <t>2025-06-05 12:27:12</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>9896</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1261,7 +1263,7 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M11" t="n">
         <v>70</v>
@@ -1279,11 +1281,11 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-05-26 00:00:00</t>
+          <t>2025-03-28 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-0.4659217171759259</v>
+        <v>-0.5188952020254629</v>
       </c>
       <c r="S11" t="n">
         <v>2</v>
@@ -1299,29 +1301,29 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>36.5</v>
+        <v>32.5</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-06-05 11:10:55</t>
+          <t>2025-06-05 12:27:12</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-06-05 11:47:25</t>
+          <t>2025-06-05 12:59:42</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-06-05 11:47:25</t>
+          <t>2025-06-05 12:59:42</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-06-05 11:47:25</t>
+          <t>2025-06-05 12:59:42</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1360,7 +1362,7 @@
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-0.4912689393981481</v>
+        <v>-0.5414646464699074</v>
       </c>
       <c r="S12" t="n">
         <v>1</v>
@@ -1368,7 +1370,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251180</v>
+        <v>251565</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1376,10 +1378,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>205.7213114754098</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1388,21 +1390,21 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-06-04 07:30:00</t>
+          <t>2025-06-04 07:20:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-06-04 07:30:00</t>
+          <t>2025-06-04 07:20:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-06-04 07:30:00</t>
+          <t>2025-06-04 10:45:43</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>12549</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1415,15 +1417,13 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>39887 (esterno)</t>
-        </is>
+      <c r="N13" t="n">
+        <v>39885</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1431,18 +1431,18 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39887</v>
+        <v>39885</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-20 00:00:00</t>
+          <t>2025-06-10 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-15.3125</v>
+        <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1455,29 +1455,29 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
         <v>641</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-06-04 07:30:00</t>
+          <t>2025-06-04 10:45:43</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-06-04 08:00:00</t>
+          <t>2025-06-04 11:05:43</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-06-04 08:00:00</t>
+          <t>2025-06-04 11:05:43</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-06-05 10:41:00</t>
+          <t>2025-06-05 13:46:43</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1516,7 +1516,7 @@
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-0.4451388888888889</v>
+        <v>-0.5741120218634259</v>
       </c>
       <c r="S14" t="n">
         <v>7</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>252282</v>
+        <v>251984</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1532,33 +1532,33 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D15" t="n">
-        <v>44.88524590163934</v>
+        <v>338.327868852459</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-06-05 10:41:00</t>
+          <t>2025-06-05 13:46:43</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-06-05 11:16:00</t>
+          <t>2025-06-05 14:11:43</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-06-05 11:16:00</t>
+          <t>2025-06-05 14:11:43</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-06-05 12:00:53</t>
+          <t>2025-06-06 11:50:02</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>2738</v>
+        <v>20638</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1571,13 +1571,13 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
       </c>
       <c r="N15" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1585,15 +1585,15 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-06-09 00:00:00</t>
+          <t>2025-06-10 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-0.5006147540972222</v>
+        <v>-1.493089708564815</v>
       </c>
       <c r="S15" t="n">
         <v>1</v>
@@ -1601,41 +1601,41 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251984</v>
+        <v>251752</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D16" t="n">
-        <v>338.327868852459</v>
+        <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-06-05 12:00:53</t>
+          <t>2025-06-05 07:00:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-06-05 12:30:53</t>
+          <t>2025-06-05 07:17:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-06-05 12:30:53</t>
+          <t>2025-06-05 07:17:00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-06-06 10:09:12</t>
+          <t>2025-06-05 07:17:00</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>20638</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1644,17 +1644,17 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L16" t="n">
         <v>3</v>
       </c>
       <c r="M16" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N16" t="n">
-        <v>39874</v>
+        <v>39846</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1662,15 +1662,15 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39874</v>
+        <v>39846</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-06-10 00:00:00</t>
+          <t>2025-05-20 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-1.423064663020833</v>
+        <v>-1.303472222222222</v>
       </c>
       <c r="S16" t="n">
         <v>1</v>
@@ -1686,29 +1686,29 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D17" t="n">
         <v>146.056338028169</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-06-05 07:00:00</t>
+          <t>2025-06-05 07:17:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-06-05 07:17:00</t>
+          <t>2025-06-05 07:32:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-06-05 07:17:00</t>
+          <t>2025-06-05 07:32:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-06-05 09:43:03</t>
+          <t>2025-06-05 09:58:03</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>-0.4049002347453703</v>
+        <v>-0.415316901412037</v>
       </c>
       <c r="S17" t="n">
         <v>2</v>
@@ -1770,22 +1770,22 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-06-05 09:43:03</t>
+          <t>2025-06-05 09:58:03</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-06-05 10:19:03</t>
+          <t>2025-06-05 10:34:03</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-06-05 10:19:03</t>
+          <t>2025-06-05 10:34:03</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-06-06 11:44:24</t>
+          <t>2025-06-06 11:59:24</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1824,7 +1824,7 @@
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>-1.489172535208333</v>
+        <v>-1.499589201875</v>
       </c>
       <c r="S18" t="n">
         <v>1</v>
@@ -2140,57 +2140,57 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>252375</v>
+        <v>251762</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D23" t="n">
-        <v>99.2063492063492</v>
+        <v>106.2857142857143</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-06-05 07:00:00</t>
+          <t>2025-06-04 11:54:08</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-06-05 07:00:00</t>
+          <t>2025-06-04 12:34:08</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-06-05 07:00:00</t>
+          <t>2025-06-04 12:34:08</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-06-05 08:39:12</t>
+          <t>2025-06-04 14:20:25</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>6250</v>
+        <v>5208</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>T1 ;T2 ;T8</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
@@ -2200,53 +2200,53 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-07-04 00:00:00</t>
+          <t>2025-05-21 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>0</v>
+        <v>-14.59751984127315</v>
       </c>
       <c r="S23" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251762</v>
+        <v>251911</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D24" t="n">
-        <v>73.35211267605634</v>
+        <v>191.3265306122449</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-06-05 12:15:23</t>
+          <t>2025-06-04 14:20:25</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-06-05 12:51:23</t>
+          <t>2025-06-05 07:00:25</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-06-05 12:51:23</t>
+          <t>2025-06-05 07:00:25</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-06-05 14:04:44</t>
+          <t>2025-06-05 10:11:45</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>5208</v>
+        <v>9375</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2259,7 +2259,7 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M24" t="n">
         <v>70</v>
@@ -2272,11 +2272,11 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-05-21 00:00:00</t>
+          <t>2025-05-28 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>-15.58662949921296</v>
+        <v>-8.424829931967592</v>
       </c>
       <c r="S24" t="n">
         <v>7</v>
@@ -2284,57 +2284,57 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251911</v>
+        <v>252375</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>191.3265306122449</v>
+        <v>99.2063492063492</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-06-05 12:45:02</t>
+          <t>2025-06-05 07:00:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-06-05 13:30:02</t>
+          <t>2025-06-05 07:00:00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-06-05 13:30:02</t>
+          <t>2025-06-05 07:00:00</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-06-06 08:41:22</t>
+          <t>2025-06-05 08:39:12</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>9375</v>
+        <v>6250</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>T1 ;T2 ;T8</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="O25" t="n">
         <v>0</v>
@@ -2344,14 +2344,14 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-05-28 00:00:00</t>
+          <t>2025-07-04 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>-9.362060657592592</v>
+        <v>0</v>
       </c>
       <c r="S25" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
@@ -2360,33 +2360,33 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D26" t="n">
-        <v>217.0819672131148</v>
+        <v>270.2448979591837</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-06-05 12:59:01</t>
+          <t>2025-06-05 10:11:45</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-06-05 13:36:01</t>
+          <t>2025-06-05 10:46:45</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-06-05 13:36:01</t>
+          <t>2025-06-05 10:46:45</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-06-06 09:13:06</t>
+          <t>2025-06-06 07:17:00</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2420,7 +2420,7 @@
         </is>
       </c>
       <c r="R26" s="1" t="n">
-        <v>-9.384107468125</v>
+        <v>-9.303472222222222</v>
       </c>
       <c r="S26" t="n">
         <v>7</v>
@@ -2432,33 +2432,33 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D27" t="n">
-        <v>76.54929577464789</v>
+        <v>89.09836065573771</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-06-05 14:04:44</t>
+          <t>2025-06-05 12:59:01</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-06-05 14:21:44</t>
+          <t>2025-06-05 13:36:01</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-06-05 14:21:44</t>
+          <t>2025-06-05 13:36:01</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-06-06 07:38:17</t>
+          <t>2025-06-06 07:05:07</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>-9.318260954618054</v>
+        <v>-9.295229963564815</v>
       </c>
       <c r="S27" t="n">
         <v>7</v>
@@ -2504,33 +2504,33 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>36</v>
+        <v>38.5</v>
       </c>
       <c r="D28" t="n">
-        <v>93.859375</v>
+        <v>109.2181818181818</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-06-05 14:23:30</t>
+          <t>2025-06-05 12:59:42</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-06-05 14:59:30</t>
+          <t>2025-06-05 13:38:12</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-06-05 14:59:30</t>
+          <t>2025-06-05 13:38:12</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-06-06 08:33:21</t>
+          <t>2025-06-06 07:27:25</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2564,7 +2564,7 @@
         </is>
       </c>
       <c r="R28" s="1" t="n">
-        <v>-7.356499565972222</v>
+        <v>-7.310713383842593</v>
       </c>
       <c r="S28" t="n">
         <v>7</v>
@@ -2576,33 +2576,33 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D29" t="n">
-        <v>83.14084507042253</v>
+        <v>92.234375</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-06-06 07:38:17</t>
+          <t>2025-06-05 14:23:30</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-06-06 07:53:17</t>
+          <t>2025-06-05 14:57:30</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-06-06 07:53:17</t>
+          <t>2025-06-05 14:57:30</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-06-06 09:16:26</t>
+          <t>2025-06-06 08:29:44</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2636,7 +2636,7 @@
         </is>
       </c>
       <c r="R29" s="1" t="n">
-        <v>-7.386414319247685</v>
+        <v>-7.353982204861111</v>
       </c>
       <c r="S29" t="n">
         <v>7</v>
@@ -2648,33 +2648,33 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>32.5</v>
+        <v>27</v>
       </c>
       <c r="D30" t="n">
-        <v>568.1818181818181</v>
+        <v>512.2950819672132</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-06-06 08:08:05</t>
+          <t>2025-06-06 07:05:07</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-06-06 08:40:35</t>
+          <t>2025-06-06 07:32:07</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-06-06 08:40:35</t>
+          <t>2025-06-06 07:32:07</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-06-09 10:08:46</t>
+          <t>2025-06-09 08:04:25</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2708,7 +2708,7 @@
         </is>
       </c>
       <c r="R30" s="1" t="n">
-        <v>-6.422758838379629</v>
+        <v>-6.336407103819445</v>
       </c>
       <c r="S30" t="n">
         <v>7</v>
@@ -2720,33 +2720,33 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D31" t="n">
-        <v>424.59375</v>
+        <v>554.5714285714286</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-06-06 08:33:21</t>
+          <t>2025-06-06 07:17:00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-06-06 08:48:21</t>
+          <t>2025-06-06 07:57:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-06-06 08:48:21</t>
+          <t>2025-06-06 07:57:00</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-06-09 07:52:57</t>
+          <t>2025-06-09 09:11:34</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2780,7 +2780,7 @@
         </is>
       </c>
       <c r="R31" s="1" t="n">
-        <v>-5.328439670138889</v>
+        <v>-5.383035714282407</v>
       </c>
       <c r="S31" t="n">
         <v>7</v>
@@ -2792,33 +2792,33 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>45</v>
+        <v>36.5</v>
       </c>
       <c r="D32" t="n">
-        <v>92.34693877551021</v>
+        <v>82.27272727272727</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-06-06 08:41:22</t>
+          <t>2025-06-06 07:27:25</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-06-06 09:26:22</t>
+          <t>2025-06-06 08:03:55</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-06-06 09:26:22</t>
+          <t>2025-06-06 08:03:55</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-06-06 10:58:42</t>
+          <t>2025-06-06 09:26:12</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2852,7 +2852,7 @@
         </is>
       </c>
       <c r="R32" s="1" t="n">
-        <v>-2.45744047619213</v>
+        <v>-2.393194444444445</v>
       </c>
       <c r="S32" t="n">
         <v>7</v>
@@ -2864,33 +2864,33 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D33" t="n">
-        <v>31.23188405797102</v>
+        <v>33.671875</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-06-06 09:04:53</t>
+          <t>2025-06-06 08:29:44</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-06-06 09:34:53</t>
+          <t>2025-06-06 08:44:44</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-06-06 09:34:53</t>
+          <t>2025-06-06 08:44:44</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-06-06 10:06:07</t>
+          <t>2025-06-06 09:18:24</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2936,33 +2936,33 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D34" t="n">
-        <v>215.983606557377</v>
+        <v>190.9420289855072</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-06-06 09:13:06</t>
+          <t>2025-06-06 09:04:53</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-06-06 09:42:06</t>
+          <t>2025-06-06 09:44:53</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-06-06 09:42:06</t>
+          <t>2025-06-06 09:44:53</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-06-06 13:18:05</t>
+          <t>2025-06-06 12:55:50</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3008,33 +3008,33 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C35" t="n">
         <v>17</v>
       </c>
       <c r="D35" t="n">
-        <v>723.5211267605633</v>
+        <v>802.65625</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-06-06 09:16:26</t>
+          <t>2025-06-06 09:18:24</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-06-06 09:33:26</t>
+          <t>2025-06-06 09:35:24</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-06-06 09:33:26</t>
+          <t>2025-06-06 09:35:24</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-06-09 13:36:57</t>
+          <t>2025-06-09 14:58:03</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3076,41 +3076,41 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>251935</v>
+        <v>251979</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>25</v>
+        <v>38.5</v>
       </c>
       <c r="D36" t="n">
-        <v>109.655737704918</v>
+        <v>374.1090909090909</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-06-06 09:49:12</t>
+          <t>2025-06-06 09:26:12</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-06-06 10:14:12</t>
+          <t>2025-06-06 10:04:42</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-06-06 10:14:12</t>
+          <t>2025-06-06 10:04:42</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-06-06 12:03:52</t>
+          <t>2025-06-09 08:18:48</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>6689</v>
+        <v>20576</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3119,11 +3119,11 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M36" t="n">
         <v>70</v>
@@ -3140,10 +3140,10 @@
         </is>
       </c>
       <c r="R36" s="1" t="n">
-        <v>-1.502686703101852</v>
+        <v>-4.346395202025463</v>
       </c>
       <c r="S36" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
@@ -3152,33 +3152,33 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D37" t="n">
-        <v>351.5652173913044</v>
+        <v>341.6619718309859</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-06-06 10:06:07</t>
+          <t>2025-06-06 10:01:38</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-06-06 10:56:07</t>
+          <t>2025-06-06 10:35:38</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-06-06 10:56:07</t>
+          <t>2025-06-06 10:35:38</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-06-09 08:47:41</t>
+          <t>2025-06-09 08:17:17</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3220,41 +3220,41 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>252395</v>
+        <v>251935</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="D38" t="n">
-        <v>1832.387755102041</v>
+        <v>109.655737704918</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-06-06 10:58:42</t>
+          <t>2025-06-06 11:50:02</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-06-06 11:55:42</t>
+          <t>2025-06-06 12:15:02</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-06-06 11:55:42</t>
+          <t>2025-06-06 12:15:02</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-06-12 10:28:06</t>
+          <t>2025-06-06 14:04:42</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>89787</v>
+        <v>6689</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3263,14 +3263,14 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M38" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="O38" t="n">
         <v>0</v>
@@ -3280,19 +3280,19 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>2025-08-04 00:00:00</t>
+          <t>2025-06-05 00:00:00</t>
         </is>
       </c>
       <c r="R38" s="1" t="n">
-        <v>0</v>
+        <v>-1.586600637523148</v>
       </c>
       <c r="S38" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>251958</v>
+        <v>252395</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -3300,33 +3300,33 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D39" t="n">
-        <v>122.2676056338028</v>
+        <v>1264.605633802817</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-06-06 11:44:24</t>
+          <t>2025-06-06 11:59:24</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-06-06 12:18:24</t>
+          <t>2025-06-06 12:37:24</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-06-06 12:18:24</t>
+          <t>2025-06-06 12:37:24</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-06-06 14:20:40</t>
+          <t>2025-06-11 09:42:00</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>8681</v>
+        <v>89787</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3339,7 +3339,7 @@
         </is>
       </c>
       <c r="L39" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M39" t="n">
         <v>76</v>
@@ -3352,14 +3352,14 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>2025-06-09 00:00:00</t>
+          <t>2025-08-04 00:00:00</t>
         </is>
       </c>
       <c r="R39" s="1" t="n">
         <v>0</v>
       </c>
       <c r="S39" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
@@ -3368,33 +3368,33 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D40" t="n">
-        <v>199.2295081967213</v>
+        <v>176.1304347826087</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-06-06 12:03:52</t>
+          <t>2025-06-06 12:55:50</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-06-06 12:23:52</t>
+          <t>2025-06-06 13:30:50</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-06-06 12:23:52</t>
+          <t>2025-06-06 13:30:50</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-06-09 07:43:05</t>
+          <t>2025-06-09 08:26:58</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3428,7 +3428,7 @@
         </is>
       </c>
       <c r="R40" s="1" t="n">
-        <v>-0.3215960837847222</v>
+        <v>-0.3520632045138889</v>
       </c>
       <c r="S40" t="n">
         <v>4</v>
@@ -3440,33 +3440,33 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D41" t="n">
         <v>255.016393442623</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-06-06 13:18:05</t>
+          <t>2025-06-06 14:04:42</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-06-06 13:45:05</t>
+          <t>2025-06-06 14:29:42</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-06-06 13:45:05</t>
+          <t>2025-06-06 14:29:42</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-06-09 10:00:06</t>
+          <t>2025-06-09 10:44:43</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3508,41 +3508,41 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>243569</v>
+        <v>251958</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D42" t="n">
-        <v>36.63380281690141</v>
+        <v>142.3114754098361</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-06-06 14:20:40</t>
+          <t>2025-06-09 08:04:25</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-06-06 14:37:40</t>
+          <t>2025-06-09 08:46:25</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-06-06 14:37:40</t>
+          <t>2025-06-09 08:46:25</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-06-09 07:14:18</t>
+          <t>2025-06-09 11:08:44</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>2601</v>
+        <v>8681</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3551,11 +3551,11 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M42" t="n">
         <v>76</v>
@@ -3568,53 +3568,53 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>2024-09-16 00:00:00</t>
+          <t>2025-06-09 00:00:00</t>
         </is>
       </c>
       <c r="R42" s="1" t="n">
-        <v>-266.3016040688542</v>
+        <v>-0.4644011839699074</v>
       </c>
       <c r="S42" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>245623</v>
+        <v>243569</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D43" t="n">
-        <v>372.0985915492957</v>
+        <v>36.63380281690141</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-06-09 07:14:18</t>
+          <t>2025-06-09 08:17:17</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-06-09 07:46:18</t>
+          <t>2025-06-09 08:42:17</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-06-09 07:46:18</t>
+          <t>2025-06-09 08:42:17</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-06-09 13:58:24</t>
+          <t>2025-06-09 09:18:55</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>26419</v>
+        <v>2601</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3627,10 +3627,10 @@
         </is>
       </c>
       <c r="L43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M43" t="n">
-        <v>152</v>
+        <v>76</v>
       </c>
       <c r="O43" t="n">
         <v>0</v>
@@ -3640,11 +3640,11 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>2025-01-25 00:00:00</t>
+          <t>2024-09-16 00:00:00</t>
         </is>
       </c>
       <c r="R43" s="1" t="n">
-        <v>-135.5822280907639</v>
+        <v>-266.3881455399074</v>
       </c>
       <c r="S43" t="n">
         <v>2</v>
@@ -3656,33 +3656,33 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>25</v>
+        <v>36.5</v>
       </c>
       <c r="D44" t="n">
-        <v>668.327868852459</v>
+        <v>741.2363636363636</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-06-09 07:43:05</t>
+          <t>2025-06-09 08:18:48</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-06-09 08:08:05</t>
+          <t>2025-06-09 08:55:18</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-06-09 08:08:05</t>
+          <t>2025-06-09 08:55:18</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-06-10 11:16:25</t>
+          <t>2025-06-10 13:16:32</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3716,7 +3716,7 @@
         </is>
       </c>
       <c r="R44" s="1" t="n">
-        <v>-15.46974043715278</v>
+        <v>-15.55315656565972</v>
       </c>
       <c r="S44" t="n">
         <v>2</v>
@@ -3724,41 +3724,41 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>251792</v>
+        <v>245623</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D45" t="n">
-        <v>143.8125</v>
+        <v>382.8840579710145</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-06-09 07:52:57</t>
+          <t>2025-06-09 08:26:58</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-06-09 08:22:57</t>
+          <t>2025-06-09 09:06:58</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-06-09 08:22:57</t>
+          <t>2025-06-09 09:06:58</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-06-09 10:46:45</t>
+          <t>2025-06-10 07:29:51</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>9204</v>
+        <v>26419</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3771,10 +3771,10 @@
         </is>
       </c>
       <c r="L45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M45" t="n">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="O45" t="n">
         <v>0</v>
@@ -3784,11 +3784,11 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>2025-05-26 00:00:00</t>
+          <t>2025-01-25 00:00:00</t>
         </is>
       </c>
       <c r="R45" s="1" t="n">
-        <v>-14.44914279513889</v>
+        <v>-136.3123993558796</v>
       </c>
       <c r="S45" t="n">
         <v>2</v>
@@ -3800,33 +3800,33 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D46" t="n">
-        <v>200.5942028985507</v>
+        <v>282.469387755102</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-06-09 08:47:41</t>
+          <t>2025-06-09 09:11:34</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-06-09 09:22:41</t>
+          <t>2025-06-09 10:03:34</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-06-09 09:22:41</t>
+          <t>2025-06-09 10:03:34</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-06-09 12:43:17</t>
+          <t>2025-06-09 14:46:02</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3860,7 +3860,7 @@
         </is>
       </c>
       <c r="R46" s="1" t="n">
-        <v>-12.53006239935185</v>
+        <v>-12.6153061224537</v>
       </c>
       <c r="S46" t="n">
         <v>2</v>
@@ -3868,41 +3868,41 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>252042</v>
+        <v>251792</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D47" t="n">
-        <v>125.9672131147541</v>
+        <v>129.6338028169014</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-06-09 10:00:06</t>
+          <t>2025-06-09 09:18:55</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-06-09 10:27:06</t>
+          <t>2025-06-09 09:33:55</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-06-09 10:27:06</t>
+          <t>2025-06-09 09:33:55</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-06-09 12:33:04</t>
+          <t>2025-06-09 11:43:33</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>7684</v>
+        <v>9204</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3911,14 +3911,14 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M47" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="O47" t="n">
         <v>0</v>
@@ -3928,11 +3928,11 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>2025-05-30 00:00:00</t>
+          <t>2025-05-26 00:00:00</t>
         </is>
       </c>
       <c r="R47" s="1" t="n">
-        <v>-10.52297358834491</v>
+        <v>-14.48858568075232</v>
       </c>
       <c r="S47" t="n">
         <v>2</v>
@@ -3940,41 +3940,41 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>251979</v>
+        <v>252042</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>32.5</v>
+        <v>25</v>
       </c>
       <c r="D48" t="n">
-        <v>374.1090909090909</v>
+        <v>125.9672131147541</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-06-09 10:08:46</t>
+          <t>2025-06-09 10:44:43</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-06-09 10:41:16</t>
+          <t>2025-06-09 11:09:43</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-06-09 10:41:16</t>
+          <t>2025-06-09 11:09:43</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-06-10 08:55:22</t>
+          <t>2025-06-09 13:15:41</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>20576</v>
+        <v>7684</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L48" t="n">
@@ -4000,14 +4000,14 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>2025-06-05 00:00:00</t>
+          <t>2025-05-30 00:00:00</t>
         </is>
       </c>
       <c r="R48" s="1" t="n">
-        <v>-5.371792929293981</v>
+        <v>-10.55256147540509</v>
       </c>
       <c r="S48" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -4016,33 +4016,33 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D49" t="n">
-        <v>103.203125</v>
+        <v>108.2786885245902</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-06-09 10:46:45</t>
+          <t>2025-06-09 11:08:44</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-06-09 11:03:45</t>
+          <t>2025-06-09 11:33:44</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-06-09 11:03:45</t>
+          <t>2025-06-09 11:33:44</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-06-09 12:46:58</t>
+          <t>2025-06-09 13:22:00</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4076,7 +4076,7 @@
         </is>
       </c>
       <c r="R49" s="1" t="n">
-        <v>-3.5326171875</v>
+        <v>-3.556955828784722</v>
       </c>
       <c r="S49" t="n">
         <v>2</v>
@@ -4088,33 +4088,33 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D50" t="n">
-        <v>86.88524590163935</v>
+        <v>74.64788732394366</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-06-09 12:33:04</t>
+          <t>2025-06-09 11:43:33</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-06-09 13:04:04</t>
+          <t>2025-06-09 12:17:33</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-06-09 13:04:04</t>
+          <t>2025-06-09 12:17:33</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-06-09 14:30:58</t>
+          <t>2025-06-09 13:32:12</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4148,7 +4148,7 @@
         </is>
       </c>
       <c r="R50" s="1" t="n">
-        <v>-0.6048383424421296</v>
+        <v>-0.5640356025</v>
       </c>
       <c r="S50" t="n">
         <v>2</v>
@@ -4160,33 +4160,33 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D51" t="n">
-        <v>650.5507246376811</v>
+        <v>735.8688524590164</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2025-06-09 12:43:17</t>
+          <t>2025-06-09 13:15:41</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-06-09 13:33:17</t>
+          <t>2025-06-09 13:35:41</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-06-09 13:33:17</t>
+          <t>2025-06-09 13:35:41</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-06-11 08:23:50</t>
+          <t>2025-06-11 09:51:33</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4220,7 +4220,7 @@
         </is>
       </c>
       <c r="R51" s="1" t="n">
-        <v>-1.349889291469907</v>
+        <v>-1.4108037340625</v>
       </c>
       <c r="S51" t="n">
         <v>2</v>
@@ -4232,33 +4232,33 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D52" t="n">
-        <v>353.828125</v>
+        <v>371.2295081967213</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-06-09 12:46:58</t>
+          <t>2025-06-09 13:22:00</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-06-09 13:01:58</t>
+          <t>2025-06-09 13:47:00</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-06-09 13:01:58</t>
+          <t>2025-06-09 13:47:00</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-06-10 10:55:47</t>
+          <t>2025-06-10 11:58:14</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4315,22 +4315,22 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-06-09 13:36:57</t>
+          <t>2025-06-09 13:32:12</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-06-09 13:53:57</t>
+          <t>2025-06-09 13:49:12</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-06-09 13:53:57</t>
+          <t>2025-06-09 13:49:12</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-06-12 12:15:20</t>
+          <t>2025-06-12 12:10:35</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4372,41 +4372,41 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>243335</v>
+        <v>244023</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D54" t="n">
-        <v>464.8450704225352</v>
+        <v>20.3469387755102</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-06-09 13:58:24</t>
+          <t>2025-06-09 14:46:02</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-06-09 14:17:24</t>
+          <t>2025-06-10 07:23:02</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-06-09 14:17:24</t>
+          <t>2025-06-10 07:23:02</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-06-10 14:02:15</t>
+          <t>2025-06-10 07:43:23</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>33004</v>
+        <v>997</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -4415,14 +4415,14 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L54" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M54" t="n">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="O54" t="n">
         <v>0</v>
@@ -4432,11 +4432,11 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>2024-08-02 00:00:00</t>
+          <t>2024-09-30 00:00:00</t>
         </is>
       </c>
       <c r="R54" s="1" t="n">
-        <v>-312.5848982785648</v>
+        <v>-253.3217970521528</v>
       </c>
       <c r="S54" t="n">
         <v>1</v>
@@ -4444,41 +4444,41 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>244023</v>
+        <v>243335</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D55" t="n">
-        <v>16.34426229508197</v>
+        <v>515.6875</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-06-09 14:30:58</t>
+          <t>2025-06-09 14:58:03</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-06-09 14:57:58</t>
+          <t>2025-06-10 07:30:03</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-06-09 14:57:58</t>
+          <t>2025-06-10 07:30:03</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-06-10 07:14:18</t>
+          <t>2025-06-11 08:05:45</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>997</v>
+        <v>33004</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -4487,14 +4487,14 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L55" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M55" t="n">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="O55" t="n">
         <v>0</v>
@@ -4504,11 +4504,11 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>2024-09-30 00:00:00</t>
+          <t>2024-08-02 00:00:00</t>
         </is>
       </c>
       <c r="R55" s="1" t="n">
-        <v>-253.3016051912616</v>
+        <v>-313.3373263888889</v>
       </c>
       <c r="S55" t="n">
         <v>1</v>
@@ -4520,33 +4520,33 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D56" t="n">
-        <v>418.2295081967213</v>
+        <v>369.7391304347826</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-06-10 07:14:18</t>
+          <t>2025-06-10 07:29:51</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-06-10 07:43:18</t>
+          <t>2025-06-10 08:09:51</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-06-10 07:43:18</t>
+          <t>2025-06-10 08:09:51</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-06-10 14:41:32</t>
+          <t>2025-06-10 14:19:35</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4580,7 +4580,7 @@
         </is>
       </c>
       <c r="R56" s="1" t="n">
-        <v>-11.61218123861111</v>
+        <v>-11.59694041868056</v>
       </c>
       <c r="S56" t="n">
         <v>1</v>
@@ -4592,33 +4592,33 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>32.5</v>
+        <v>50</v>
       </c>
       <c r="D57" t="n">
-        <v>330.6727272727273</v>
+        <v>371.1632653061225</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:55:22</t>
+          <t>2025-06-10 07:43:23</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-06-10 09:27:52</t>
+          <t>2025-06-10 08:33:23</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-06-10 09:27:52</t>
+          <t>2025-06-10 08:33:23</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-06-10 14:58:33</t>
+          <t>2025-06-10 14:44:33</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4652,7 +4652,7 @@
         </is>
       </c>
       <c r="R57" s="1" t="n">
-        <v>-5.623996212118056</v>
+        <v>-5.614271541944444</v>
       </c>
       <c r="S57" t="n">
         <v>1</v>
@@ -4736,33 +4736,33 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D59" t="n">
-        <v>75.75</v>
+        <v>79.47540983606558</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-06-10 10:55:47</t>
+          <t>2025-06-10 11:58:14</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-06-10 11:10:47</t>
+          <t>2025-06-10 12:23:14</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-06-10 11:10:47</t>
+          <t>2025-06-10 12:23:14</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2025-06-10 12:26:32</t>
+          <t>2025-06-10 13:42:43</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4796,7 +4796,7 @@
         </is>
       </c>
       <c r="R59" s="1" t="n">
-        <v>-11.51843532986111</v>
+        <v>-11.57133424408565</v>
       </c>
       <c r="S59" t="n">
         <v>1</v>
@@ -4808,33 +4808,33 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>30</v>
+        <v>34.5</v>
       </c>
       <c r="D60" t="n">
-        <v>234.4426229508197</v>
+        <v>260.0181818181818</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-06-10 11:16:25</t>
+          <t>2025-06-10 13:16:32</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-06-10 11:46:25</t>
+          <t>2025-06-10 13:51:02</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-06-10 11:46:25</t>
+          <t>2025-06-10 13:51:02</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-06-11 07:40:52</t>
+          <t>2025-06-11 10:11:03</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4868,7 +4868,7 @@
         </is>
       </c>
       <c r="R60" s="1" t="n">
-        <v>-5.320047814212963</v>
+        <v>-5.424349747476852</v>
       </c>
       <c r="S60" t="n">
         <v>1</v>
@@ -4880,33 +4880,33 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 4</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D61" t="n">
-        <v>732.421875</v>
+        <v>768.4426229508197</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-06-10 12:26:32</t>
+          <t>2025-06-10 13:42:43</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-06-10 12:56:32</t>
+          <t>2025-06-10 14:22:43</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-06-10 12:56:32</t>
+          <t>2025-06-10 14:22:43</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-06-12 09:08:58</t>
+          <t>2025-06-12 11:11:09</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -4948,41 +4948,41 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>245089</v>
+        <v>252196</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>R12</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C62" t="n">
         <v>30</v>
       </c>
       <c r="D62" t="n">
-        <v>1727.676056338028</v>
+        <v>682.4492753623189</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-06-10 14:02:15</t>
+          <t>2025-06-10 14:19:35</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-06-10 14:32:15</t>
+          <t>2025-06-10 14:49:35</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-06-10 14:32:15</t>
+          <t>2025-06-10 14:49:35</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-06-16 11:19:55</t>
+          <t>2025-06-12 10:12:02</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>122665</v>
+        <v>47089</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -4991,14 +4991,14 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M62" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="O62" t="n">
         <v>0</v>
@@ -5008,7 +5008,7 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>2025-12-31 00:00:00</t>
+          <t>2025-06-13 00:00:00</t>
         </is>
       </c>
       <c r="R62" s="1" t="n">
@@ -5020,41 +5020,41 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>252196</v>
+        <v>252195</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>BIMEC 4</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D63" t="n">
-        <v>771.9508196721312</v>
+        <v>729.6530612244898</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-06-10 14:41:32</t>
+          <t>2025-06-10 14:44:33</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-06-11 07:08:32</t>
+          <t>2025-06-11 07:19:33</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-06-11 07:08:32</t>
+          <t>2025-06-11 07:19:33</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-06-12 12:00:29</t>
+          <t>2025-06-12 11:29:12</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>47089</v>
+        <v>35753</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -5067,7 +5067,7 @@
         </is>
       </c>
       <c r="L63" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M63" t="n">
         <v>70</v>
@@ -5092,41 +5092,41 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>252195</v>
+        <v>252110</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>30.5</v>
+        <v>32</v>
       </c>
       <c r="D64" t="n">
-        <v>650.0545454545454</v>
+        <v>100.15625</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2025-06-10 14:58:33</t>
+          <t>2025-06-11 08:05:45</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-06-11 07:29:03</t>
+          <t>2025-06-11 08:37:45</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>2025-06-11 07:29:03</t>
+          <t>2025-06-11 08:37:45</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>2025-06-12 10:19:06</t>
+          <t>2025-06-11 10:17:54</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>35753</v>
+        <v>6410</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -5152,7 +5152,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>2025-06-13 00:00:00</t>
+          <t>2025-06-17 00:00:00</t>
         </is>
       </c>
       <c r="R64" s="1" t="n">
@@ -5164,41 +5164,41 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>252110</v>
+        <v>245089</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R12</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D65" t="n">
-        <v>105.0819672131148</v>
+        <v>1727.676056338028</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2025-06-11 07:40:52</t>
+          <t>2025-06-11 09:42:00</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-06-11 08:00:52</t>
+          <t>2025-06-11 10:01:00</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025-06-11 08:00:52</t>
+          <t>2025-06-11 10:01:00</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>2025-06-11 09:45:57</t>
+          <t>2025-06-16 14:48:41</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>6410</v>
+        <v>122665</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -5207,14 +5207,14 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L65" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M65" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="O65" t="n">
         <v>0</v>
@@ -5224,7 +5224,7 @@
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>2025-06-17 00:00:00</t>
+          <t>2025-12-31 00:00:00</t>
         </is>
       </c>
       <c r="R65" s="1" t="n">
@@ -5240,33 +5240,33 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D66" t="n">
-        <v>180.4782608695652</v>
+        <v>204.1475409836065</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>2025-06-11 08:23:50</t>
+          <t>2025-06-11 09:51:33</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-06-11 08:48:50</t>
+          <t>2025-06-11 10:11:33</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025-06-11 08:48:50</t>
+          <t>2025-06-11 10:11:33</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>2025-06-11 11:49:19</t>
+          <t>2025-06-11 13:35:42</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5312,33 +5312,33 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>35</v>
+        <v>36.5</v>
       </c>
       <c r="D67" t="n">
-        <v>123.6229508196721</v>
+        <v>137.1090909090909</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>2025-06-11 09:45:57</t>
+          <t>2025-06-11 10:11:03</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-06-11 10:20:57</t>
+          <t>2025-06-11 10:47:33</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>2025-06-11 10:20:57</t>
+          <t>2025-06-11 10:47:33</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>2025-06-11 12:24:34</t>
+          <t>2025-06-11 13:04:40</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5384,33 +5384,33 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D68" t="n">
-        <v>262.3188405797101</v>
+        <v>282.8125</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>2025-06-11 11:49:19</t>
+          <t>2025-06-11 10:17:54</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-06-11 12:34:19</t>
+          <t>2025-06-11 10:38:54</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>2025-06-11 12:34:19</t>
+          <t>2025-06-11 10:38:54</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>2025-06-12 08:56:38</t>
+          <t>2025-06-12 07:21:43</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5456,33 +5456,33 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>20</v>
+        <v>30.5</v>
       </c>
       <c r="D69" t="n">
-        <v>277.1475409836066</v>
+        <v>307.3818181818182</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>2025-06-11 12:24:34</t>
+          <t>2025-06-11 13:04:40</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-06-11 12:44:34</t>
+          <t>2025-06-11 13:35:10</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>2025-06-11 12:44:34</t>
+          <t>2025-06-11 13:35:10</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2025-06-12 09:21:43</t>
+          <t>2025-06-12 10:42:33</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5524,41 +5524,41 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>251681</v>
+        <v>251679</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C70" t="n">
         <v>40</v>
       </c>
       <c r="D70" t="n">
-        <v>56.12676056338028</v>
+        <v>260</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-06-11 13:54:25</t>
+          <t>2025-06-11 13:35:42</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-06-11 14:34:25</t>
+          <t>2025-06-11 14:15:42</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-06-11 14:34:25</t>
+          <t>2025-06-11 14:15:42</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-06-12 07:30:32</t>
+          <t>2025-06-12 10:35:42</t>
         </is>
       </c>
       <c r="I70" t="n">
-        <v>3985</v>
+        <v>15860</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -5567,11 +5567,11 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L70" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M70" t="n">
         <v>70</v>
@@ -5596,7 +5596,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>251917</v>
+        <v>251681</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -5604,33 +5604,33 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D71" t="n">
-        <v>32.26760563380282</v>
+        <v>56.12676056338028</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
+          <t>2025-06-11 13:54:25</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>2025-06-11 14:34:25</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2025-06-11 14:34:25</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
           <t>2025-06-12 07:30:32</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>2025-06-12 08:05:32</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>2025-06-12 08:05:32</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>2025-06-12 08:37:49</t>
-        </is>
-      </c>
       <c r="I71" t="n">
-        <v>2291</v>
+        <v>3985</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -5656,7 +5656,7 @@
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>2025-06-20 00:00:00</t>
+          <t>2025-06-18 00:00:00</t>
         </is>
       </c>
       <c r="R71" s="1" t="n">
@@ -5668,37 +5668,37 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>252293</v>
+        <v>251917</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>R6</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D72" t="n">
-        <v>32.26760563380282</v>
+        <v>35.796875</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2025-06-12 08:37:49</t>
+          <t>2025-06-12 07:21:43</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-06-12 09:12:49</t>
+          <t>2025-06-12 07:38:43</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025-06-12 09:12:49</t>
+          <t>2025-06-12 07:38:43</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>2025-06-12 09:45:05</t>
+          <t>2025-06-12 08:14:30</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5740,41 +5740,41 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>251679</v>
+        <v>252293</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>R6</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D73" t="n">
-        <v>229.8550724637681</v>
+        <v>32.26760563380282</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2025-06-12 08:56:38</t>
+          <t>2025-06-12 07:30:32</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-06-12 09:21:38</t>
+          <t>2025-06-12 08:05:32</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>2025-06-12 09:21:38</t>
+          <t>2025-06-12 08:05:32</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>2025-06-12 13:11:29</t>
+          <t>2025-06-12 08:37:49</t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>15860</v>
+        <v>2291</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -5783,11 +5783,11 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M73" t="n">
         <v>70</v>
@@ -5800,7 +5800,7 @@
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>2025-06-18 00:00:00</t>
+          <t>2025-06-20 00:00:00</t>
         </is>
       </c>
       <c r="R73" s="1" t="n">
@@ -5820,29 +5820,29 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D74" t="n">
         <v>400.640625</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-06-12 09:08:58</t>
+          <t>2025-06-12 08:14:30</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-06-12 09:27:58</t>
+          <t>2025-06-12 08:31:30</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-06-12 09:27:58</t>
+          <t>2025-06-12 08:31:30</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-06-13 08:08:36</t>
+          <t>2025-06-13 07:12:09</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -5888,33 +5888,33 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D75" t="n">
-        <v>247.2622950819672</v>
+        <v>218.5942028985507</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-06-12 09:21:43</t>
+          <t>2025-06-12 10:12:02</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-06-12 09:41:43</t>
+          <t>2025-06-12 10:42:02</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-06-12 09:41:43</t>
+          <t>2025-06-12 10:42:02</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-06-12 13:48:59</t>
+          <t>2025-06-12 14:20:38</t>
         </is>
       </c>
       <c r="I75" t="n">

</xml_diff>

<commit_message>
Tolto parametro "a" / beta dal main per testaggio
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -825,7 +825,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251895</v>
+        <v>251218</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -833,10 +833,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D6" t="n">
-        <v>249.2112676056338</v>
+        <v>96.90140845070422</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -845,21 +845,21 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-06-04 13:51:16</t>
+          <t>2025-06-04 13:28:16</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-06-04 13:51:16</t>
+          <t>2025-06-04 13:28:16</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-06-05 10:00:29</t>
+          <t>2025-06-05 07:05:10</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>17694</v>
+        <v>6880</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -868,19 +868,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M6" t="n">
-        <v>70</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>39891 (esterno)</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="N6" t="n">
+        <v>39885</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -888,23 +886,23 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39891</v>
+        <v>39885</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-26 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-10.4170089984375</v>
+        <v>-0.2952660406828704</v>
       </c>
       <c r="S6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251218</v>
+        <v>251895</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -915,30 +913,30 @@
         <v>38</v>
       </c>
       <c r="D7" t="n">
-        <v>96.90140845070422</v>
+        <v>249.2112676056338</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-06-05 10:00:29</t>
+          <t>2025-06-05 07:05:10</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-06-05 10:38:29</t>
+          <t>2025-06-05 07:43:10</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-06-05 10:38:29</t>
+          <t>2025-06-05 07:43:10</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-06-05 12:15:23</t>
+          <t>2025-06-05 11:52:23</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>6880</v>
+        <v>17694</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -947,17 +945,19 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M7" t="n">
-        <v>76</v>
-      </c>
-      <c r="N7" t="n">
-        <v>39885</v>
+        <v>70</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>39891 (esterno)</t>
+        </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -965,18 +965,18 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39885</v>
+        <v>39891</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-26 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-0.5106905320833334</v>
+        <v>-10.49471830986111</v>
       </c>
       <c r="S7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -989,29 +989,29 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D8" t="n">
         <v>176.7464788732394</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-06-05 12:15:23</t>
+          <t>2025-06-05 11:52:23</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-06-05 12:53:23</t>
+          <t>2025-06-05 12:23:23</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-06-05 12:53:23</t>
+          <t>2025-06-05 12:23:23</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-06-06 07:50:08</t>
+          <t>2025-06-06 07:20:08</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.326486697962963</v>
+        <v>-1.30565336462963</v>
       </c>
       <c r="S8" t="n">
         <v>1</v>
@@ -1073,22 +1073,22 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-06-06 07:50:08</t>
+          <t>2025-06-06 07:20:08</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-06-06 08:07:08</t>
+          <t>2025-06-06 07:37:08</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-06-06 08:07:08</t>
+          <t>2025-06-06 07:37:08</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-06-06 13:49:22</t>
+          <t>2025-06-06 13:19:22</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1368,7 +1368,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251984</v>
+        <v>252084</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1376,10 +1376,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D13" t="n">
-        <v>338.327868852459</v>
+        <v>641</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1388,21 +1388,21 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-06-04 07:25:00</t>
+          <t>2025-06-04 07:20:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-06-04 07:25:00</t>
+          <t>2025-06-04 07:20:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-06-04 13:03:19</t>
+          <t>2025-06-05 10:01:00</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>20638</v>
+        <v>39101</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1415,13 +1415,13 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
       <c r="N13" t="n">
-        <v>39874</v>
+        <v>39885</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1429,23 +1429,23 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39874</v>
+        <v>39885</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-06-10 00:00:00</t>
+          <t>2025-06-30 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>0</v>
+        <v>-0.4173611111111111</v>
       </c>
       <c r="S13" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251180</v>
+        <v>251984</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1456,30 +1456,30 @@
         <v>25</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>338.327868852459</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-06-04 13:03:19</t>
+          <t>2025-06-05 10:01:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-06-04 13:28:19</t>
+          <t>2025-06-05 10:26:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-06-04 13:28:19</t>
+          <t>2025-06-05 10:26:00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-06-04 13:28:19</t>
+          <t>2025-06-06 08:04:19</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>20638</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1492,15 +1492,13 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M14" t="n">
         <v>70</v>
       </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>39887 (esterno)</t>
-        </is>
+      <c r="N14" t="n">
+        <v>39874</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1508,18 +1506,18 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>39887</v>
+        <v>39874</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-05-20 00:00:00</t>
+          <t>2025-06-10 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-15.5613387978125</v>
+        <v>-1.3363387978125</v>
       </c>
       <c r="S14" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1532,29 +1530,29 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D15" t="n">
         <v>44.88524590163934</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-06-04 13:28:19</t>
+          <t>2025-06-06 08:04:19</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-06-04 13:53:19</t>
+          <t>2025-06-06 08:34:19</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-06-04 13:53:19</t>
+          <t>2025-06-06 08:34:19</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-06-04 14:38:12</t>
+          <t>2025-06-06 09:19:12</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1593,7 +1591,7 @@
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>0</v>
+        <v>-1.388342440798611</v>
       </c>
       <c r="S15" t="n">
         <v>1</v>
@@ -1601,7 +1599,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>252084</v>
+        <v>251180</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1609,33 +1607,33 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D16" t="n">
-        <v>641</v>
+        <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-06-04 14:38:12</t>
+          <t>2025-06-06 09:19:12</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-06-05 07:13:12</t>
+          <t>2025-06-06 09:44:12</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-06-05 07:13:12</t>
+          <t>2025-06-06 09:44:12</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-06-06 09:54:12</t>
+          <t>2025-06-06 09:44:12</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>39101</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1648,13 +1646,15 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
-      <c r="N16" t="n">
-        <v>39885</v>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>39887 (esterno)</t>
+        </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1662,15 +1662,15 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39885</v>
+        <v>39887</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-06-30 00:00:00</t>
+          <t>2025-05-20 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-1.412647996354166</v>
+        <v>-17.40570355190972</v>
       </c>
       <c r="S16" t="n">
         <v>7</v>
@@ -3084,29 +3084,29 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D36" t="n">
         <v>842.1311475409836</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-06-06 09:54:12</t>
+          <t>2025-06-06 09:44:12</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-06-06 10:29:12</t>
+          <t>2025-06-06 10:09:12</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-06-06 10:29:12</t>
+          <t>2025-06-06 10:09:12</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-06-10 08:31:20</t>
+          <t>2025-06-10 08:11:20</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3307,22 +3307,22 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-06-06 13:49:22</t>
+          <t>2025-06-06 13:19:22</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-06-06 14:06:22</t>
+          <t>2025-06-06 13:36:22</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-06-06 14:06:22</t>
+          <t>2025-06-06 13:36:22</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-06-09 07:40:35</t>
+          <t>2025-06-09 07:10:35</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3356,7 +3356,7 @@
         </is>
       </c>
       <c r="R39" s="1" t="n">
-        <v>-4.319855242569444</v>
+        <v>-4.299021909236111</v>
       </c>
       <c r="S39" t="n">
         <v>4</v>
@@ -3667,22 +3667,22 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-06-09 07:40:35</t>
+          <t>2025-06-09 07:10:35</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-06-09 08:14:35</t>
+          <t>2025-06-09 07:44:35</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-06-09 08:14:35</t>
+          <t>2025-06-09 07:44:35</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-06-09 14:26:41</t>
+          <t>2025-06-09 13:56:41</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3716,7 +3716,7 @@
         </is>
       </c>
       <c r="R44" s="1" t="n">
-        <v>-135.6018681533681</v>
+        <v>-135.5810348200347</v>
       </c>
       <c r="S44" t="n">
         <v>2</v>
@@ -4243,22 +4243,22 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-06-09 14:26:41</t>
+          <t>2025-06-09 13:56:41</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-06-10 07:00:41</t>
+          <t>2025-06-09 14:30:41</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-06-10 07:00:41</t>
+          <t>2025-06-09 14:30:41</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-06-10 12:19:38</t>
+          <t>2025-06-10 11:49:38</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4603,22 +4603,22 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:31:20</t>
+          <t>2025-06-10 08:11:20</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:56:20</t>
+          <t>2025-06-10 08:36:20</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:56:20</t>
+          <t>2025-06-10 08:36:20</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-06-11 13:18:00</t>
+          <t>2025-06-11 12:58:00</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4652,7 +4652,7 @@
         </is>
       </c>
       <c r="R57" s="1" t="n">
-        <v>-6.554178051006944</v>
+        <v>-6.540289162118055</v>
       </c>
       <c r="S57" t="n">
         <v>1</v>
@@ -4819,22 +4819,22 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-06-10 12:19:38</t>
+          <t>2025-06-10 11:49:38</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-06-10 12:34:38</t>
+          <t>2025-06-10 12:04:38</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-06-10 12:34:38</t>
+          <t>2025-06-10 12:04:38</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-06-10 13:42:54</t>
+          <t>2025-06-10 13:12:54</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4868,7 +4868,7 @@
         </is>
       </c>
       <c r="R60" s="1" t="n">
-        <v>-11.57146909232639</v>
+        <v>-11.55063575899305</v>
       </c>
       <c r="S60" t="n">
         <v>1</v>
@@ -4880,33 +4880,33 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>32.5</v>
+        <v>30</v>
       </c>
       <c r="D61" t="n">
-        <v>852.2727272727273</v>
+        <v>660.2112676056338</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-06-10 13:25:10</t>
+          <t>2025-06-10 13:12:54</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-06-10 13:57:40</t>
+          <t>2025-06-10 13:42:54</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-06-10 13:57:40</t>
+          <t>2025-06-10 13:42:54</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-06-12 12:09:57</t>
+          <t>2025-06-12 08:43:07</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -4952,33 +4952,33 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>32</v>
+        <v>34.5</v>
       </c>
       <c r="D62" t="n">
-        <v>663.2253521126761</v>
+        <v>856.1636363636363</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-06-10 13:42:54</t>
+          <t>2025-06-10 13:25:10</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-06-10 14:14:54</t>
+          <t>2025-06-10 13:59:40</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-06-10 14:14:54</t>
+          <t>2025-06-10 13:59:40</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-06-12 09:18:08</t>
+          <t>2025-06-12 12:15:50</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5539,22 +5539,22 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-06-11 13:18:00</t>
+          <t>2025-06-11 12:58:00</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-06-11 13:48:00</t>
+          <t>2025-06-11 13:28:00</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-06-11 13:48:00</t>
+          <t>2025-06-11 13:28:00</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-06-12 10:08:00</t>
+          <t>2025-06-12 09:48:00</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5816,33 +5816,33 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D74" t="n">
-        <v>371.6086956521739</v>
+        <v>361.1408450704225</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-06-12 08:59:10</t>
+          <t>2025-06-12 08:43:07</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-06-12 09:24:10</t>
+          <t>2025-06-12 09:02:07</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-06-12 09:24:10</t>
+          <t>2025-06-12 09:02:07</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-06-13 07:35:46</t>
+          <t>2025-06-13 07:03:16</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -5888,33 +5888,33 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D75" t="n">
-        <v>212.4366197183099</v>
+        <v>218.5942028985507</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-06-12 09:18:08</t>
+          <t>2025-06-12 08:59:10</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-06-12 09:35:08</t>
+          <t>2025-06-12 09:24:10</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-06-12 09:35:08</t>
+          <t>2025-06-12 09:24:10</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-06-12 13:07:34</t>
+          <t>2025-06-12 13:02:46</t>
         </is>
       </c>
       <c r="I75" t="n">

</xml_diff>

<commit_message>
Cambiato check_LS per funzionare correttamente
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -1368,7 +1368,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>252084</v>
+        <v>251984</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1376,10 +1376,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D13" t="n">
-        <v>641</v>
+        <v>338.327868852459</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1388,21 +1388,21 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-06-04 07:20:00</t>
+          <t>2025-06-04 07:25:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-06-04 07:20:00</t>
+          <t>2025-06-04 07:25:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-06-05 10:01:00</t>
+          <t>2025-06-04 13:03:19</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>39101</v>
+        <v>20638</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1415,13 +1415,13 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
       <c r="N13" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1429,23 +1429,23 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-06-30 00:00:00</t>
+          <t>2025-06-10 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-0.4173611111111111</v>
+        <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>252282</v>
+        <v>251180</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1453,33 +1453,33 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D14" t="n">
-        <v>44.88524590163934</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-06-05 10:01:00</t>
+          <t>2025-06-04 13:03:19</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-06-05 10:36:00</t>
+          <t>2025-06-04 13:28:19</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-06-05 10:36:00</t>
+          <t>2025-06-04 13:28:19</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-06-05 11:20:53</t>
+          <t>2025-06-04 13:28:19</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>2738</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1492,13 +1492,15 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M14" t="n">
         <v>70</v>
       </c>
-      <c r="N14" t="n">
-        <v>39885</v>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>39887 (esterno)</t>
+        </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1506,23 +1508,23 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>39885</v>
+        <v>39887</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-06-09 00:00:00</t>
+          <t>2025-05-20 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-0.4728369763194445</v>
+        <v>-15.5613387978125</v>
       </c>
       <c r="S14" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>251180</v>
+        <v>252282</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1533,30 +1535,30 @@
         <v>25</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>44.88524590163934</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-06-05 11:20:53</t>
+          <t>2025-06-04 13:28:19</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-06-05 11:45:53</t>
+          <t>2025-06-04 13:53:19</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-06-05 11:45:53</t>
+          <t>2025-06-04 13:53:19</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-06-05 11:45:53</t>
+          <t>2025-06-04 14:38:12</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>2738</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1569,15 +1571,13 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>39887 (esterno)</t>
-        </is>
+      <c r="N15" t="n">
+        <v>39885</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1585,23 +1585,23 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39887</v>
+        <v>39885</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-05-20 00:00:00</t>
+          <t>2025-06-09 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-16.49019808743056</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251984</v>
+        <v>252084</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1609,33 +1609,33 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D16" t="n">
-        <v>338.327868852459</v>
+        <v>641</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-06-05 11:45:53</t>
+          <t>2025-06-04 14:38:12</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-06-05 12:10:53</t>
+          <t>2025-06-05 07:13:12</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-06-05 12:10:53</t>
+          <t>2025-06-05 07:13:12</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-06-06 09:49:12</t>
+          <t>2025-06-06 09:54:12</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>20638</v>
+        <v>39101</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1648,13 +1648,13 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
       <c r="N16" t="n">
-        <v>39874</v>
+        <v>39885</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1662,18 +1662,18 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39874</v>
+        <v>39885</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-06-10 00:00:00</t>
+          <t>2025-06-30 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-1.409175774131944</v>
+        <v>-1.412647996354166</v>
       </c>
       <c r="S16" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -3084,29 +3084,29 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D36" t="n">
         <v>842.1311475409836</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-06-06 09:49:12</t>
+          <t>2025-06-06 09:54:12</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-06-06 10:19:12</t>
+          <t>2025-06-06 10:29:12</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-06-06 10:19:12</t>
+          <t>2025-06-06 10:29:12</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-06-10 08:21:20</t>
+          <t>2025-06-10 08:31:20</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -4603,22 +4603,22 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:21:20</t>
+          <t>2025-06-10 08:31:20</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:46:20</t>
+          <t>2025-06-10 08:56:20</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:46:20</t>
+          <t>2025-06-10 08:56:20</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-06-11 13:08:00</t>
+          <t>2025-06-11 13:18:00</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4652,7 +4652,7 @@
         </is>
       </c>
       <c r="R57" s="1" t="n">
-        <v>-6.5472336065625</v>
+        <v>-6.554178051006944</v>
       </c>
       <c r="S57" t="n">
         <v>1</v>
@@ -5539,22 +5539,22 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-06-11 13:08:00</t>
+          <t>2025-06-11 13:18:00</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-06-11 13:38:00</t>
+          <t>2025-06-11 13:48:00</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-06-11 13:38:00</t>
+          <t>2025-06-11 13:48:00</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-06-12 09:58:00</t>
+          <t>2025-06-12 10:08:00</t>
         </is>
       </c>
       <c r="I70" t="n">

</xml_diff>

<commit_message>
TEST TEST TEST TEST TEST
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/euristico_post.xlsx
+++ b/PS-VRP/Dati_output/euristico_post.xlsx
@@ -671,7 +671,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>251362</v>
+        <v>251752</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -682,7 +682,7 @@
         <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>35.28169014084507</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -701,11 +701,11 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-06-04 12:52:16</t>
+          <t>2025-06-04 12:17:00</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2505</v>
+        <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -714,7 +714,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L4" t="n">
@@ -724,7 +724,7 @@
         <v>76</v>
       </c>
       <c r="N4" t="n">
-        <v>39874</v>
+        <v>39846</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -732,23 +732,23 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>39874</v>
+        <v>39846</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-05-20 00:00:00</t>
         </is>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0</v>
+        <v>-0.5118055555555555</v>
       </c>
       <c r="S4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>251752</v>
+        <v>251218</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -756,33 +756,33 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>96.90140845070422</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-06-04 12:52:16</t>
+          <t>2025-06-04 12:17:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-06-04 13:07:16</t>
+          <t>2025-06-04 12:38:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-06-04 13:07:16</t>
+          <t>2025-06-04 12:38:00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-06-04 13:07:16</t>
+          <t>2025-06-04 14:14:54</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>6880</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -791,17 +791,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M5" t="n">
         <v>76</v>
       </c>
       <c r="N5" t="n">
-        <v>39846</v>
+        <v>39885</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -809,15 +809,15 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>39846</v>
+        <v>39885</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2025-05-20 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R5" s="1" t="n">
-        <v>-0.5467233959259259</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
         <v>1</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>251218</v>
+        <v>251895</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -833,33 +833,33 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D6" t="n">
-        <v>96.90140845070422</v>
+        <v>249.2112676056338</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-06-04 13:07:16</t>
+          <t>2025-06-04 14:14:54</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-06-04 13:28:16</t>
+          <t>2025-06-04 14:52:54</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-06-04 13:28:16</t>
+          <t>2025-06-04 14:52:54</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-06-05 07:05:10</t>
+          <t>2025-06-05 11:02:06</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>6880</v>
+        <v>17694</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -868,17 +868,19 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L6" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M6" t="n">
-        <v>76</v>
-      </c>
-      <c r="N6" t="n">
-        <v>39885</v>
+        <v>70</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>39891 (esterno)</t>
+        </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -886,23 +888,23 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>39885</v>
+        <v>39891</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-26 00:00:00</t>
         </is>
       </c>
       <c r="R6" s="1" t="n">
-        <v>-0.2952660406828704</v>
+        <v>-10.45980046947917</v>
       </c>
       <c r="S6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>251895</v>
+        <v>251565</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -910,33 +912,33 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D7" t="n">
-        <v>249.2112676056338</v>
+        <v>176.7464788732394</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-06-05 07:05:10</t>
+          <t>2025-06-05 11:02:06</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-06-05 07:43:10</t>
+          <t>2025-06-05 11:33:06</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-06-05 07:43:10</t>
+          <t>2025-06-05 11:33:06</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-06-05 11:52:23</t>
+          <t>2025-06-05 14:29:51</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>17694</v>
+        <v>12549</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -945,19 +947,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M7" t="n">
         <v>70</v>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>39891 (esterno)</t>
-        </is>
+      <c r="N7" t="n">
+        <v>39885</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -965,23 +965,23 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>39891</v>
+        <v>39885</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2025-05-26 00:00:00</t>
+          <t>2025-06-10 00:00:00</t>
         </is>
       </c>
       <c r="R7" s="1" t="n">
-        <v>-10.49471830986111</v>
+        <v>-0.6040688575925925</v>
       </c>
       <c r="S7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>251565</v>
+        <v>251362</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -989,33 +989,33 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="n">
-        <v>176.7464788732394</v>
+        <v>35.28169014084507</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2025-06-05 11:52:23</t>
+          <t>2025-06-05 14:29:51</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-06-05 12:23:23</t>
+          <t>2025-06-06 07:01:51</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-06-05 12:23:23</t>
+          <t>2025-06-06 07:01:51</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-06-06 07:20:08</t>
+          <t>2025-06-06 07:37:08</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>12549</v>
+        <v>2505</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1024,17 +1024,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N8" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,18 +1042,18 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2025-06-10 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R8" s="1" t="n">
-        <v>-1.30565336462963</v>
+        <v>-1.317458920185185</v>
       </c>
       <c r="S8" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -1066,29 +1066,29 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D9" t="n">
         <v>342.2394366197183</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-06-06 07:20:08</t>
+          <t>2025-06-06 07:37:08</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-06-06 07:37:08</t>
+          <t>2025-06-06 08:07:08</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-06-06 07:37:08</t>
+          <t>2025-06-06 08:07:08</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-06-06 13:19:22</t>
+          <t>2025-06-06 13:49:22</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1137,7 +1137,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251500</v>
+        <v>251070</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1145,10 +1145,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>32.5</v>
+        <v>36.5</v>
       </c>
       <c r="D10" t="n">
-        <v>179.9272727272727</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1157,21 +1157,21 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-06-05 07:32:30</t>
+          <t>2025-06-05 07:36:30</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-06-05 07:32:30</t>
+          <t>2025-06-05 07:36:30</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-06-05 10:32:25</t>
+          <t>2025-06-05 07:36:30</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>9896</v>
+        <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1184,7 +1184,7 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M10" t="n">
         <v>70</v>
@@ -1202,11 +1202,11 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-05-26 00:00:00</t>
+          <t>2025-03-28 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-0.4391856060648148</v>
+        <v>-0.3170138888888889</v>
       </c>
       <c r="S10" t="n">
         <v>2</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251070</v>
+        <v>251773</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1222,29 +1222,29 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-06-05 10:32:25</t>
+          <t>2025-06-05 07:36:30</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-06-05 11:06:55</t>
+          <t>2025-06-05 08:09:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-06-05 11:06:55</t>
+          <t>2025-06-05 08:09:00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-06-05 11:06:55</t>
+          <t>2025-06-05 08:09:00</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1257,17 +1257,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M11" t="n">
         <v>70</v>
       </c>
       <c r="N11" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1275,23 +1275,23 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2025-03-28 00:00:00</t>
+          <t>2025-05-25 00:00:00</t>
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-0.4631439393981481</v>
+        <v>-0.3395833333333333</v>
       </c>
       <c r="S11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251773</v>
+        <v>251500</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1299,33 +1299,33 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>32.5</v>
+        <v>36.5</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>179.9272727272727</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-06-05 11:06:55</t>
+          <t>2025-06-05 08:09:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-06-05 11:39:25</t>
+          <t>2025-06-05 08:45:30</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-06-05 11:39:25</t>
+          <t>2025-06-05 08:45:30</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-06-05 11:39:25</t>
+          <t>2025-06-05 11:45:25</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>9896</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1334,17 +1334,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M12" t="n">
         <v>70</v>
       </c>
       <c r="N12" t="n">
-        <v>39874</v>
+        <v>39885</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1352,23 +1352,23 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>39874</v>
+        <v>39885</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-05-25 00:00:00</t>
+          <t>2025-05-26 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
-        <v>-0.4857133838425925</v>
+        <v>-0.4898800505092593</v>
       </c>
       <c r="S12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>252084</v>
+        <v>251180</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1376,10 +1376,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>641</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1388,21 +1388,21 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-06-04 07:20:00</t>
+          <t>2025-06-04 07:30:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-06-04 07:20:00</t>
+          <t>2025-06-04 07:30:00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-06-05 10:01:00</t>
+          <t>2025-06-04 07:30:00</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>39101</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1415,13 +1415,15 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
       </c>
-      <c r="N13" t="n">
-        <v>39885</v>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>39887 (esterno)</t>
+        </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1429,15 +1431,15 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>39885</v>
+        <v>39887</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-06-30 00:00:00</t>
+          <t>2025-05-20 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
-        <v>-0.4173611111111111</v>
+        <v>-15.3125</v>
       </c>
       <c r="S13" t="n">
         <v>7</v>
@@ -1445,7 +1447,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251984</v>
+        <v>252282</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1456,30 +1458,30 @@
         <v>25</v>
       </c>
       <c r="D14" t="n">
-        <v>338.327868852459</v>
+        <v>44.88524590163934</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-06-05 10:01:00</t>
+          <t>2025-06-04 07:30:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-06-05 10:26:00</t>
+          <t>2025-06-04 07:55:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-06-05 10:26:00</t>
+          <t>2025-06-04 07:55:00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-06-06 08:04:19</t>
+          <t>2025-06-04 08:39:53</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>20638</v>
+        <v>2738</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1492,13 +1494,13 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M14" t="n">
         <v>70</v>
       </c>
       <c r="N14" t="n">
-        <v>39874</v>
+        <v>39885</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1506,15 +1508,15 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>39874</v>
+        <v>39885</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-06-10 00:00:00</t>
+          <t>2025-06-09 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
-        <v>-1.3363387978125</v>
+        <v>0</v>
       </c>
       <c r="S14" t="n">
         <v>1</v>
@@ -1522,7 +1524,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>252282</v>
+        <v>251984</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1533,30 +1535,30 @@
         <v>30</v>
       </c>
       <c r="D15" t="n">
-        <v>44.88524590163934</v>
+        <v>338.327868852459</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-06-06 08:04:19</t>
+          <t>2025-06-04 08:39:53</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-06-06 08:34:19</t>
+          <t>2025-06-04 09:09:53</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-06-06 08:34:19</t>
+          <t>2025-06-04 09:09:53</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-06-06 09:19:12</t>
+          <t>2025-06-04 14:48:12</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>2738</v>
+        <v>20638</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1569,13 +1571,13 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
       </c>
       <c r="N15" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1583,15 +1585,15 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>39885</v>
+        <v>39874</v>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-06-09 00:00:00</t>
+          <t>2025-06-10 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
-        <v>-1.388342440798611</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
         <v>1</v>
@@ -1599,7 +1601,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251180</v>
+        <v>252084</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1610,30 +1612,30 @@
         <v>25</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>641</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-06-06 09:19:12</t>
+          <t>2025-06-04 14:48:12</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-06-06 09:44:12</t>
+          <t>2025-06-05 07:13:12</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-06-06 09:44:12</t>
+          <t>2025-06-05 07:13:12</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-06-06 09:44:12</t>
+          <t>2025-06-06 09:54:12</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>39101</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1646,15 +1648,13 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M16" t="n">
         <v>70</v>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>39887 (esterno)</t>
-        </is>
+      <c r="N16" t="n">
+        <v>39885</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1662,15 +1662,15 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>39887</v>
+        <v>39885</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-20 00:00:00</t>
+          <t>2025-06-30 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>-17.40570355190972</v>
+        <v>-1.412647996354166</v>
       </c>
       <c r="S16" t="n">
         <v>7</v>
@@ -2436,14 +2436,14 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>36.5</v>
+        <v>30.5</v>
       </c>
       <c r="D27" t="n">
         <v>98.81818181818181</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-06-05 11:39:25</t>
+          <t>2025-06-05 11:45:25</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3084,29 +3084,29 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D36" t="n">
         <v>842.1311475409836</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-06-06 09:44:12</t>
+          <t>2025-06-06 09:54:12</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-06-06 10:09:12</t>
+          <t>2025-06-06 10:29:12</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-06-06 10:09:12</t>
+          <t>2025-06-06 10:29:12</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-06-10 08:11:20</t>
+          <t>2025-06-10 08:31:20</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3307,22 +3307,22 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-06-06 13:19:22</t>
+          <t>2025-06-06 13:49:22</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-06-06 13:36:22</t>
+          <t>2025-06-06 14:06:22</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-06-06 13:36:22</t>
+          <t>2025-06-06 14:06:22</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-06-09 07:10:35</t>
+          <t>2025-06-09 07:40:35</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3356,7 +3356,7 @@
         </is>
       </c>
       <c r="R39" s="1" t="n">
-        <v>-4.299021909236111</v>
+        <v>-4.319855242569444</v>
       </c>
       <c r="S39" t="n">
         <v>4</v>
@@ -3667,22 +3667,22 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-06-09 07:10:35</t>
+          <t>2025-06-09 07:40:35</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-06-09 07:44:35</t>
+          <t>2025-06-09 08:14:35</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-06-09 07:44:35</t>
+          <t>2025-06-09 08:14:35</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-06-09 13:56:41</t>
+          <t>2025-06-09 14:26:41</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3716,7 +3716,7 @@
         </is>
       </c>
       <c r="R44" s="1" t="n">
-        <v>-135.5810348200347</v>
+        <v>-135.6018681533681</v>
       </c>
       <c r="S44" t="n">
         <v>2</v>
@@ -4243,22 +4243,22 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-06-09 13:56:41</t>
+          <t>2025-06-09 14:26:41</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-06-09 14:30:41</t>
+          <t>2025-06-10 07:00:41</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-06-09 14:30:41</t>
+          <t>2025-06-10 07:00:41</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-06-10 11:49:38</t>
+          <t>2025-06-10 12:19:38</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4603,22 +4603,22 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:11:20</t>
+          <t>2025-06-10 08:31:20</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:36:20</t>
+          <t>2025-06-10 08:56:20</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-06-10 08:36:20</t>
+          <t>2025-06-10 08:56:20</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-06-11 12:58:00</t>
+          <t>2025-06-11 13:18:00</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4652,7 +4652,7 @@
         </is>
       </c>
       <c r="R57" s="1" t="n">
-        <v>-6.540289162118055</v>
+        <v>-6.554178051006944</v>
       </c>
       <c r="S57" t="n">
         <v>1</v>
@@ -4819,22 +4819,22 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-06-10 11:49:38</t>
+          <t>2025-06-10 12:19:38</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-06-10 12:04:38</t>
+          <t>2025-06-10 12:34:38</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-06-10 12:04:38</t>
+          <t>2025-06-10 12:34:38</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-06-10 13:12:54</t>
+          <t>2025-06-10 13:42:54</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4868,7 +4868,7 @@
         </is>
       </c>
       <c r="R60" s="1" t="n">
-        <v>-11.55063575899305</v>
+        <v>-11.57146909232639</v>
       </c>
       <c r="S60" t="n">
         <v>1</v>
@@ -4880,33 +4880,33 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>30</v>
+        <v>32.5</v>
       </c>
       <c r="D61" t="n">
-        <v>660.2112676056338</v>
+        <v>852.2727272727273</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-06-10 13:12:54</t>
+          <t>2025-06-10 13:25:10</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-06-10 13:42:54</t>
+          <t>2025-06-10 13:57:40</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-06-10 13:42:54</t>
+          <t>2025-06-10 13:57:40</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-06-12 08:43:07</t>
+          <t>2025-06-12 12:09:57</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -4952,33 +4952,33 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>34.5</v>
+        <v>32</v>
       </c>
       <c r="D62" t="n">
-        <v>856.1636363636363</v>
+        <v>663.2253521126761</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-06-10 13:25:10</t>
+          <t>2025-06-10 13:42:54</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-06-10 13:59:40</t>
+          <t>2025-06-10 14:14:54</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-06-10 13:59:40</t>
+          <t>2025-06-10 14:14:54</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-06-12 12:15:50</t>
+          <t>2025-06-12 09:18:08</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5539,22 +5539,22 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2025-06-11 12:58:00</t>
+          <t>2025-06-11 13:18:00</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-06-11 13:28:00</t>
+          <t>2025-06-11 13:48:00</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025-06-11 13:28:00</t>
+          <t>2025-06-11 13:48:00</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2025-06-12 09:48:00</t>
+          <t>2025-06-12 10:08:00</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5816,33 +5816,33 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R9</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D74" t="n">
-        <v>361.1408450704225</v>
+        <v>371.6086956521739</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>2025-06-12 08:43:07</t>
+          <t>2025-06-12 08:59:10</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-06-12 09:02:07</t>
+          <t>2025-06-12 09:24:10</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>2025-06-12 09:02:07</t>
+          <t>2025-06-12 09:24:10</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>2025-06-13 07:03:16</t>
+          <t>2025-06-13 07:35:46</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -5888,33 +5888,33 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>R9</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D75" t="n">
-        <v>218.5942028985507</v>
+        <v>212.4366197183099</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2025-06-12 08:59:10</t>
+          <t>2025-06-12 09:18:08</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-06-12 09:24:10</t>
+          <t>2025-06-12 09:35:08</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>2025-06-12 09:24:10</t>
+          <t>2025-06-12 09:35:08</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>2025-06-12 13:02:46</t>
+          <t>2025-06-12 13:07:34</t>
         </is>
       </c>
       <c r="I75" t="n">

</xml_diff>